<commit_message>
update with electron desktop
</commit_message>
<xml_diff>
--- a/+dataLH/test_files/readTest.xlsx
+++ b/+dataLH/test_files/readTest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11045" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11570" uniqueCount="525">
   <si>
     <t>Code</t>
   </si>
@@ -1610,7 +1610,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1660,11 +1660,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1708,6 +1710,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1726,13 +1730,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="43" t="s">
         <v>524</v>
       </c>
     </row>
@@ -1740,7 +1744,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -1751,7 +1755,7 @@
       <c r="A3">
         <v>-1</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="43" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -1762,7 +1766,7 @@
       <c r="A4">
         <v>100</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -1773,7 +1777,7 @@
       <c r="A5">
         <v>200</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="43" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -1784,7 +1788,7 @@
       <c r="A6">
         <v>300</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -1795,7 +1799,7 @@
       <c r="A7">
         <v>401</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -1806,7 +1810,7 @@
       <c r="A8">
         <v>402</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="43" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -1817,7 +1821,7 @@
       <c r="A9">
         <v>403</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -1828,7 +1832,7 @@
       <c r="A10">
         <v>411</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="43" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -1839,7 +1843,7 @@
       <c r="A11">
         <v>412</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -1850,7 +1854,7 @@
       <c r="A12">
         <v>413</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="43" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -1861,7 +1865,7 @@
       <c r="A13">
         <v>501</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -1872,7 +1876,7 @@
       <c r="A14">
         <v>502</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="43" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -1883,7 +1887,7 @@
       <c r="A15">
         <v>503</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="43" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -1894,7 +1898,7 @@
       <c r="A16">
         <v>511</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1905,7 +1909,7 @@
       <c r="A17">
         <v>512</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -1916,7 +1920,7 @@
       <c r="A18">
         <v>513</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="43" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -1927,7 +1931,7 @@
       <c r="A19">
         <v>-1</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="43" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -1938,7 +1942,7 @@
       <c r="A20">
         <v>1111</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1949,7 +1953,7 @@
       <c r="A21">
         <v>1112</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="43" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -1960,7 +1964,7 @@
       <c r="A22">
         <v>1113</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="43" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1971,7 +1975,7 @@
       <c r="A23">
         <v>1122</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="43" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -1982,7 +1986,7 @@
       <c r="A24">
         <v>1123</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="43" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -1993,7 +1997,7 @@
       <c r="A25">
         <v>1130</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="43" t="s">
         <v>25</v>
       </c>
       <c r="C25">
@@ -2004,7 +2008,7 @@
       <c r="A26">
         <v>1140</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="43" t="s">
         <v>27</v>
       </c>
       <c r="C26">
@@ -2015,7 +2019,7 @@
       <c r="A27">
         <v>1210</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="43" t="s">
         <v>28</v>
       </c>
       <c r="C27">
@@ -2026,7 +2030,7 @@
       <c r="A28">
         <v>1219</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="43" t="s">
         <v>29</v>
       </c>
       <c r="C28">
@@ -2037,7 +2041,7 @@
       <c r="A29">
         <v>1220</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C29">
@@ -2048,7 +2052,7 @@
       <c r="A30">
         <v>1230</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="43" t="s">
         <v>31</v>
       </c>
       <c r="C30">
@@ -2059,7 +2063,7 @@
       <c r="A31">
         <v>1310</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="43" t="s">
         <v>32</v>
       </c>
       <c r="C31">
@@ -2070,7 +2074,7 @@
       <c r="A32">
         <v>1320</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="43" t="s">
         <v>33</v>
       </c>
       <c r="C32">
@@ -2081,7 +2085,7 @@
       <c r="A33">
         <v>-1</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="43" t="s">
         <v>34</v>
       </c>
       <c r="C33">
@@ -2092,7 +2096,7 @@
       <c r="A34">
         <v>2011</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="43" t="s">
         <v>35</v>
       </c>
       <c r="C34">
@@ -2103,7 +2107,7 @@
       <c r="A35">
         <v>2012</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="43" t="s">
         <v>36</v>
       </c>
       <c r="C35">
@@ -2114,7 +2118,7 @@
       <c r="A36">
         <v>2021</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="43" t="s">
         <v>37</v>
       </c>
       <c r="C36">
@@ -2125,7 +2129,7 @@
       <c r="A37">
         <v>2111</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="43" t="s">
         <v>38</v>
       </c>
       <c r="C37">
@@ -2136,7 +2140,7 @@
       <c r="A38">
         <v>2112</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="43" t="s">
         <v>39</v>
       </c>
       <c r="C38">
@@ -2147,7 +2151,7 @@
       <c r="A39">
         <v>2121</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="43" t="s">
         <v>40</v>
       </c>
       <c r="C39">
@@ -2158,7 +2162,7 @@
       <c r="A40">
         <v>2122</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="43" t="s">
         <v>41</v>
       </c>
       <c r="C40">
@@ -2169,7 +2173,7 @@
       <c r="A41">
         <v>2123</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="43" t="s">
         <v>42</v>
       </c>
       <c r="C41">
@@ -2180,7 +2184,7 @@
       <c r="A42">
         <v>2124</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C42">
@@ -2191,7 +2195,7 @@
       <c r="A43">
         <v>2125</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="43" t="s">
         <v>44</v>
       </c>
       <c r="C43">
@@ -2202,7 +2206,7 @@
       <c r="A44">
         <v>2131</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="43" t="s">
         <v>45</v>
       </c>
       <c r="C44">
@@ -2213,7 +2217,7 @@
       <c r="A45">
         <v>2132</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="43" t="s">
         <v>46</v>
       </c>
       <c r="C45">
@@ -2224,7 +2228,7 @@
       <c r="A46">
         <v>2133</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="43" t="s">
         <v>47</v>
       </c>
       <c r="C46">
@@ -2235,7 +2239,7 @@
       <c r="A47">
         <v>2134</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="43" t="s">
         <v>48</v>
       </c>
       <c r="C47">
@@ -2246,7 +2250,7 @@
       <c r="A48">
         <v>2140</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="43" t="s">
         <v>49</v>
       </c>
       <c r="C48">
@@ -2257,7 +2261,7 @@
       <c r="A49">
         <v>2141</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="43" t="s">
         <v>50</v>
       </c>
       <c r="C49">
@@ -2268,7 +2272,7 @@
       <c r="A50">
         <v>2142</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="43" t="s">
         <v>51</v>
       </c>
       <c r="C50">
@@ -2279,7 +2283,7 @@
       <c r="A51">
         <v>2143</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C51">
@@ -2290,7 +2294,7 @@
       <c r="A52">
         <v>2144</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="43" t="s">
         <v>53</v>
       </c>
       <c r="C52">
@@ -2301,7 +2305,7 @@
       <c r="A53">
         <v>2145</v>
       </c>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="43" t="s">
         <v>54</v>
       </c>
       <c r="C53">
@@ -2312,7 +2316,7 @@
       <c r="A54">
         <v>2146</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C54">
@@ -2323,7 +2327,7 @@
       <c r="A55">
         <v>2147</v>
       </c>
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="43" t="s">
         <v>56</v>
       </c>
       <c r="C55">
@@ -2334,7 +2338,7 @@
       <c r="A56">
         <v>2148</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="43" t="s">
         <v>57</v>
       </c>
       <c r="C56">
@@ -2345,7 +2349,7 @@
       <c r="A57">
         <v>2149</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="43" t="s">
         <v>58</v>
       </c>
       <c r="C57">
@@ -2356,7 +2360,7 @@
       <c r="A58">
         <v>2151</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="43" t="s">
         <v>59</v>
       </c>
       <c r="C58">
@@ -2367,7 +2371,7 @@
       <c r="A59">
         <v>2152</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C59">
@@ -2378,7 +2382,7 @@
       <c r="A60">
         <v>2153</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="43" t="s">
         <v>61</v>
       </c>
       <c r="C60">
@@ -2389,7 +2393,7 @@
       <c r="A61">
         <v>2211</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="43" t="s">
         <v>62</v>
       </c>
       <c r="C61">
@@ -2400,7 +2404,7 @@
       <c r="A62">
         <v>2221</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C62">
@@ -2411,7 +2415,7 @@
       <c r="A63">
         <v>2231</v>
       </c>
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="43" t="s">
         <v>64</v>
       </c>
       <c r="C63">
@@ -2422,7 +2426,7 @@
       <c r="A64">
         <v>2232</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C64">
@@ -2433,7 +2437,7 @@
       <c r="A65">
         <v>2233</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C65">
@@ -2444,7 +2448,7 @@
       <c r="A66">
         <v>2234</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="43" t="s">
         <v>67</v>
       </c>
       <c r="C66">
@@ -2455,7 +2459,7 @@
       <c r="A67">
         <v>2235</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C67">
@@ -2466,7 +2470,7 @@
       <c r="A68">
         <v>2236</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="43" t="s">
         <v>69</v>
       </c>
       <c r="C68">
@@ -2477,7 +2481,7 @@
       <c r="A69">
         <v>2237</v>
       </c>
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="43" t="s">
         <v>70</v>
       </c>
       <c r="C69">
@@ -2488,7 +2492,7 @@
       <c r="A70">
         <v>2311</v>
       </c>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="43" t="s">
         <v>71</v>
       </c>
       <c r="C70">
@@ -2499,7 +2503,7 @@
       <c r="A71">
         <v>2312</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="43" t="s">
         <v>72</v>
       </c>
       <c r="C71">
@@ -2510,7 +2514,7 @@
       <c r="A72">
         <v>2313</v>
       </c>
-      <c r="B72" s="41" t="s">
+      <c r="B72" s="43" t="s">
         <v>73</v>
       </c>
       <c r="C72">
@@ -2521,7 +2525,7 @@
       <c r="A73">
         <v>2321</v>
       </c>
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="43" t="s">
         <v>74</v>
       </c>
       <c r="C73">
@@ -2532,7 +2536,7 @@
       <c r="A74">
         <v>2330</v>
       </c>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="43" t="s">
         <v>75</v>
       </c>
       <c r="C74">
@@ -2543,7 +2547,7 @@
       <c r="A75">
         <v>2340</v>
       </c>
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="43" t="s">
         <v>76</v>
       </c>
       <c r="C75">
@@ -2554,7 +2558,7 @@
       <c r="A76">
         <v>2391</v>
       </c>
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="43" t="s">
         <v>77</v>
       </c>
       <c r="C76">
@@ -2565,7 +2569,7 @@
       <c r="A77">
         <v>2392</v>
       </c>
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="43" t="s">
         <v>78</v>
       </c>
       <c r="C77">
@@ -2576,7 +2580,7 @@
       <c r="A78">
         <v>2394</v>
       </c>
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="43" t="s">
         <v>79</v>
       </c>
       <c r="C78">
@@ -2587,7 +2591,7 @@
       <c r="A79">
         <v>2410</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="43" t="s">
         <v>80</v>
       </c>
       <c r="C79">
@@ -2598,7 +2602,7 @@
       <c r="A80">
         <v>2412</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="43" t="s">
         <v>81</v>
       </c>
       <c r="C80">
@@ -2609,7 +2613,7 @@
       <c r="A81">
         <v>2419</v>
       </c>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="43" t="s">
         <v>82</v>
       </c>
       <c r="C81">
@@ -2620,7 +2624,7 @@
       <c r="A82">
         <v>2421</v>
       </c>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="43" t="s">
         <v>83</v>
       </c>
       <c r="C82">
@@ -2631,7 +2635,7 @@
       <c r="A83">
         <v>2422</v>
       </c>
-      <c r="B83" s="41" t="s">
+      <c r="B83" s="43" t="s">
         <v>84</v>
       </c>
       <c r="C83">
@@ -2642,7 +2646,7 @@
       <c r="A84">
         <v>2423</v>
       </c>
-      <c r="B84" s="41" t="s">
+      <c r="B84" s="43" t="s">
         <v>85</v>
       </c>
       <c r="C84">
@@ -2653,7 +2657,7 @@
       <c r="A85">
         <v>2511</v>
       </c>
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="43" t="s">
         <v>86</v>
       </c>
       <c r="C85">
@@ -2664,7 +2668,7 @@
       <c r="A86">
         <v>2512</v>
       </c>
-      <c r="B86" s="41" t="s">
+      <c r="B86" s="43" t="s">
         <v>87</v>
       </c>
       <c r="C86">
@@ -2675,7 +2679,7 @@
       <c r="A87">
         <v>2513</v>
       </c>
-      <c r="B87" s="41" t="s">
+      <c r="B87" s="43" t="s">
         <v>88</v>
       </c>
       <c r="C87">
@@ -2686,7 +2690,7 @@
       <c r="A88">
         <v>2514</v>
       </c>
-      <c r="B88" s="41" t="s">
+      <c r="B88" s="43" t="s">
         <v>89</v>
       </c>
       <c r="C88">
@@ -2697,7 +2701,7 @@
       <c r="A89">
         <v>2515</v>
       </c>
-      <c r="B89" s="41" t="s">
+      <c r="B89" s="43" t="s">
         <v>90</v>
       </c>
       <c r="C89">
@@ -2708,7 +2712,7 @@
       <c r="A90">
         <v>2516</v>
       </c>
-      <c r="B90" s="41" t="s">
+      <c r="B90" s="43" t="s">
         <v>91</v>
       </c>
       <c r="C90">
@@ -2719,7 +2723,7 @@
       <c r="A91">
         <v>2521</v>
       </c>
-      <c r="B91" s="41" t="s">
+      <c r="B91" s="43" t="s">
         <v>92</v>
       </c>
       <c r="C91">
@@ -2730,7 +2734,7 @@
       <c r="A92">
         <v>2522</v>
       </c>
-      <c r="B92" s="41" t="s">
+      <c r="B92" s="43" t="s">
         <v>93</v>
       </c>
       <c r="C92">
@@ -2741,7 +2745,7 @@
       <c r="A93">
         <v>2523</v>
       </c>
-      <c r="B93" s="41" t="s">
+      <c r="B93" s="43" t="s">
         <v>94</v>
       </c>
       <c r="C93">
@@ -2752,7 +2756,7 @@
       <c r="A94">
         <v>2524</v>
       </c>
-      <c r="B94" s="41" t="s">
+      <c r="B94" s="43" t="s">
         <v>95</v>
       </c>
       <c r="C94">
@@ -2763,7 +2767,7 @@
       <c r="A95">
         <v>2525</v>
       </c>
-      <c r="B95" s="41" t="s">
+      <c r="B95" s="43" t="s">
         <v>96</v>
       </c>
       <c r="C95">
@@ -2774,7 +2778,7 @@
       <c r="A96">
         <v>2531</v>
       </c>
-      <c r="B96" s="41" t="s">
+      <c r="B96" s="43" t="s">
         <v>97</v>
       </c>
       <c r="C96">
@@ -2785,7 +2789,7 @@
       <c r="A97">
         <v>2611</v>
       </c>
-      <c r="B97" s="41" t="s">
+      <c r="B97" s="43" t="s">
         <v>98</v>
       </c>
       <c r="C97">
@@ -2796,7 +2800,7 @@
       <c r="A98">
         <v>2612</v>
       </c>
-      <c r="B98" s="41" t="s">
+      <c r="B98" s="43" t="s">
         <v>99</v>
       </c>
       <c r="C98">
@@ -2807,7 +2811,7 @@
       <c r="A99">
         <v>2613</v>
       </c>
-      <c r="B99" s="41" t="s">
+      <c r="B99" s="43" t="s">
         <v>100</v>
       </c>
       <c r="C99">
@@ -2818,7 +2822,7 @@
       <c r="A100">
         <v>2614</v>
       </c>
-      <c r="B100" s="41" t="s">
+      <c r="B100" s="43" t="s">
         <v>101</v>
       </c>
       <c r="C100">
@@ -2829,7 +2833,7 @@
       <c r="A101">
         <v>2615</v>
       </c>
-      <c r="B101" s="41" t="s">
+      <c r="B101" s="43" t="s">
         <v>102</v>
       </c>
       <c r="C101">
@@ -2840,7 +2844,7 @@
       <c r="A102">
         <v>2616</v>
       </c>
-      <c r="B102" s="41" t="s">
+      <c r="B102" s="43" t="s">
         <v>103</v>
       </c>
       <c r="C102">
@@ -2851,7 +2855,7 @@
       <c r="A103">
         <v>2617</v>
       </c>
-      <c r="B103" s="41" t="s">
+      <c r="B103" s="43" t="s">
         <v>104</v>
       </c>
       <c r="C103">
@@ -2862,7 +2866,7 @@
       <c r="A104">
         <v>2621</v>
       </c>
-      <c r="B104" s="41" t="s">
+      <c r="B104" s="43" t="s">
         <v>105</v>
       </c>
       <c r="C104">
@@ -2873,7 +2877,7 @@
       <c r="A105">
         <v>2622</v>
       </c>
-      <c r="B105" s="41" t="s">
+      <c r="B105" s="43" t="s">
         <v>106</v>
       </c>
       <c r="C105">
@@ -2884,7 +2888,7 @@
       <c r="A106">
         <v>2623</v>
       </c>
-      <c r="B106" s="41" t="s">
+      <c r="B106" s="43" t="s">
         <v>107</v>
       </c>
       <c r="C106">
@@ -2895,7 +2899,7 @@
       <c r="A107">
         <v>2624</v>
       </c>
-      <c r="B107" s="41" t="s">
+      <c r="B107" s="43" t="s">
         <v>108</v>
       </c>
       <c r="C107">
@@ -2906,7 +2910,7 @@
       <c r="A108">
         <v>2625</v>
       </c>
-      <c r="B108" s="41" t="s">
+      <c r="B108" s="43" t="s">
         <v>109</v>
       </c>
       <c r="C108">
@@ -2917,7 +2921,7 @@
       <c r="A109">
         <v>2627</v>
       </c>
-      <c r="B109" s="41" t="s">
+      <c r="B109" s="43" t="s">
         <v>110</v>
       </c>
       <c r="C109">
@@ -2928,7 +2932,7 @@
       <c r="A110">
         <v>2631</v>
       </c>
-      <c r="B110" s="41" t="s">
+      <c r="B110" s="43" t="s">
         <v>111</v>
       </c>
       <c r="C110">
@@ -2939,7 +2943,7 @@
       <c r="A111">
         <v>-1</v>
       </c>
-      <c r="B111" s="41" t="s">
+      <c r="B111" s="43" t="s">
         <v>112</v>
       </c>
       <c r="C111">
@@ -2950,7 +2954,7 @@
       <c r="A112">
         <v>3001</v>
       </c>
-      <c r="B112" s="41" t="s">
+      <c r="B112" s="43" t="s">
         <v>113</v>
       </c>
       <c r="C112">
@@ -2961,7 +2965,7 @@
       <c r="A113">
         <v>3003</v>
       </c>
-      <c r="B113" s="41" t="s">
+      <c r="B113" s="43" t="s">
         <v>114</v>
       </c>
       <c r="C113">
@@ -2972,7 +2976,7 @@
       <c r="A114">
         <v>3011</v>
       </c>
-      <c r="B114" s="41" t="s">
+      <c r="B114" s="43" t="s">
         <v>115</v>
       </c>
       <c r="C114">
@@ -2983,7 +2987,7 @@
       <c r="A115">
         <v>3012</v>
       </c>
-      <c r="B115" s="41" t="s">
+      <c r="B115" s="43" t="s">
         <v>116</v>
       </c>
       <c r="C115">
@@ -2994,7 +2998,7 @@
       <c r="A116">
         <v>3111</v>
       </c>
-      <c r="B116" s="41" t="s">
+      <c r="B116" s="43" t="s">
         <v>117</v>
       </c>
       <c r="C116">
@@ -3005,7 +3009,7 @@
       <c r="A117">
         <v>3112</v>
       </c>
-      <c r="B117" s="41" t="s">
+      <c r="B117" s="43" t="s">
         <v>118</v>
       </c>
       <c r="C117">
@@ -3016,7 +3020,7 @@
       <c r="A118">
         <v>3113</v>
       </c>
-      <c r="B118" s="41" t="s">
+      <c r="B118" s="43" t="s">
         <v>119</v>
       </c>
       <c r="C118">
@@ -3027,7 +3031,7 @@
       <c r="A119">
         <v>3114</v>
       </c>
-      <c r="B119" s="41" t="s">
+      <c r="B119" s="43" t="s">
         <v>120</v>
       </c>
       <c r="C119">
@@ -3038,7 +3042,7 @@
       <c r="A120">
         <v>3115</v>
       </c>
-      <c r="B120" s="41" t="s">
+      <c r="B120" s="43" t="s">
         <v>121</v>
       </c>
       <c r="C120">
@@ -3049,7 +3053,7 @@
       <c r="A121">
         <v>3116</v>
       </c>
-      <c r="B121" s="41" t="s">
+      <c r="B121" s="43" t="s">
         <v>122</v>
       </c>
       <c r="C121">
@@ -3060,7 +3064,7 @@
       <c r="A122">
         <v>3117</v>
       </c>
-      <c r="B122" s="41" t="s">
+      <c r="B122" s="43" t="s">
         <v>123</v>
       </c>
       <c r="C122">
@@ -3071,7 +3075,7 @@
       <c r="A123">
         <v>3121</v>
       </c>
-      <c r="B123" s="41" t="s">
+      <c r="B123" s="43" t="s">
         <v>124</v>
       </c>
       <c r="C123">
@@ -3082,7 +3086,7 @@
       <c r="A124">
         <v>3122</v>
       </c>
-      <c r="B124" s="41" t="s">
+      <c r="B124" s="43" t="s">
         <v>125</v>
       </c>
       <c r="C124">
@@ -3093,7 +3097,7 @@
       <c r="A125">
         <v>3123</v>
       </c>
-      <c r="B125" s="41" t="s">
+      <c r="B125" s="43" t="s">
         <v>126</v>
       </c>
       <c r="C125">
@@ -3104,7 +3108,7 @@
       <c r="A126">
         <v>3131</v>
       </c>
-      <c r="B126" s="41" t="s">
+      <c r="B126" s="43" t="s">
         <v>127</v>
       </c>
       <c r="C126">
@@ -3115,7 +3119,7 @@
       <c r="A127">
         <v>3132</v>
       </c>
-      <c r="B127" s="41" t="s">
+      <c r="B127" s="43" t="s">
         <v>128</v>
       </c>
       <c r="C127">
@@ -3126,7 +3130,7 @@
       <c r="A128">
         <v>3134</v>
       </c>
-      <c r="B128" s="41" t="s">
+      <c r="B128" s="43" t="s">
         <v>129</v>
       </c>
       <c r="C128">
@@ -3137,7 +3141,7 @@
       <c r="A129">
         <v>3135</v>
       </c>
-      <c r="B129" s="41" t="s">
+      <c r="B129" s="43" t="s">
         <v>130</v>
       </c>
       <c r="C129">
@@ -3148,7 +3152,7 @@
       <c r="A130">
         <v>3136</v>
       </c>
-      <c r="B130" s="41" t="s">
+      <c r="B130" s="43" t="s">
         <v>131</v>
       </c>
       <c r="C130">
@@ -3159,7 +3163,7 @@
       <c r="A131">
         <v>3141</v>
       </c>
-      <c r="B131" s="41" t="s">
+      <c r="B131" s="43" t="s">
         <v>132</v>
       </c>
       <c r="C131">
@@ -3170,7 +3174,7 @@
       <c r="A132">
         <v>3142</v>
       </c>
-      <c r="B132" s="41" t="s">
+      <c r="B132" s="43" t="s">
         <v>133</v>
       </c>
       <c r="C132">
@@ -3181,7 +3185,7 @@
       <c r="A133">
         <v>3143</v>
       </c>
-      <c r="B133" s="41" t="s">
+      <c r="B133" s="43" t="s">
         <v>134</v>
       </c>
       <c r="C133">
@@ -3192,7 +3196,7 @@
       <c r="A134">
         <v>3144</v>
       </c>
-      <c r="B134" s="41" t="s">
+      <c r="B134" s="43" t="s">
         <v>135</v>
       </c>
       <c r="C134">
@@ -3203,7 +3207,7 @@
       <c r="A135">
         <v>3146</v>
       </c>
-      <c r="B135" s="41" t="s">
+      <c r="B135" s="43" t="s">
         <v>136</v>
       </c>
       <c r="C135">
@@ -3214,7 +3218,7 @@
       <c r="A136">
         <v>3147</v>
       </c>
-      <c r="B136" s="41" t="s">
+      <c r="B136" s="43" t="s">
         <v>137</v>
       </c>
       <c r="C136">
@@ -3225,7 +3229,7 @@
       <c r="A137">
         <v>3161</v>
       </c>
-      <c r="B137" s="41" t="s">
+      <c r="B137" s="43" t="s">
         <v>138</v>
       </c>
       <c r="C137">
@@ -3236,7 +3240,7 @@
       <c r="A138">
         <v>3162</v>
       </c>
-      <c r="B138" s="41" t="s">
+      <c r="B138" s="43" t="s">
         <v>139</v>
       </c>
       <c r="C138">
@@ -3247,7 +3251,7 @@
       <c r="A139">
         <v>3163</v>
       </c>
-      <c r="B139" s="41" t="s">
+      <c r="B139" s="43" t="s">
         <v>140</v>
       </c>
       <c r="C139">
@@ -3258,7 +3262,7 @@
       <c r="A140">
         <v>3171</v>
       </c>
-      <c r="B140" s="41" t="s">
+      <c r="B140" s="43" t="s">
         <v>141</v>
       </c>
       <c r="C140">
@@ -3269,7 +3273,7 @@
       <c r="A141">
         <v>3172</v>
       </c>
-      <c r="B141" s="41" t="s">
+      <c r="B141" s="43" t="s">
         <v>142</v>
       </c>
       <c r="C141">
@@ -3280,7 +3284,7 @@
       <c r="A142">
         <v>3189</v>
       </c>
-      <c r="B142" s="41" t="s">
+      <c r="B142" s="43" t="s">
         <v>143</v>
       </c>
       <c r="C142">
@@ -3291,7 +3295,7 @@
       <c r="A143">
         <v>3191</v>
       </c>
-      <c r="B143" s="41" t="s">
+      <c r="B143" s="43" t="s">
         <v>144</v>
       </c>
       <c r="C143">
@@ -3302,7 +3306,7 @@
       <c r="A144">
         <v>3192</v>
       </c>
-      <c r="B144" s="41" t="s">
+      <c r="B144" s="43" t="s">
         <v>145</v>
       </c>
       <c r="C144">
@@ -3313,7 +3317,7 @@
       <c r="A145">
         <v>3201</v>
       </c>
-      <c r="B145" s="41" t="s">
+      <c r="B145" s="43" t="s">
         <v>146</v>
       </c>
       <c r="C145">
@@ -3324,7 +3328,7 @@
       <c r="A146">
         <v>3210</v>
       </c>
-      <c r="B146" s="41" t="s">
+      <c r="B146" s="43" t="s">
         <v>147</v>
       </c>
       <c r="C146">
@@ -3335,7 +3339,7 @@
       <c r="A147">
         <v>3211</v>
       </c>
-      <c r="B147" s="41" t="s">
+      <c r="B147" s="43" t="s">
         <v>148</v>
       </c>
       <c r="C147">
@@ -3346,7 +3350,7 @@
       <c r="A148">
         <v>3212</v>
       </c>
-      <c r="B148" s="41" t="s">
+      <c r="B148" s="43" t="s">
         <v>149</v>
       </c>
       <c r="C148">
@@ -3357,7 +3361,7 @@
       <c r="A149">
         <v>3213</v>
       </c>
-      <c r="B149" s="41" t="s">
+      <c r="B149" s="43" t="s">
         <v>150</v>
       </c>
       <c r="C149">
@@ -3368,7 +3372,7 @@
       <c r="A150">
         <v>3214</v>
       </c>
-      <c r="B150" s="41" t="s">
+      <c r="B150" s="43" t="s">
         <v>151</v>
       </c>
       <c r="C150">
@@ -3379,7 +3383,7 @@
       <c r="A151">
         <v>3221</v>
       </c>
-      <c r="B151" s="41" t="s">
+      <c r="B151" s="43" t="s">
         <v>152</v>
       </c>
       <c r="C151">
@@ -3390,7 +3394,7 @@
       <c r="A152">
         <v>3222</v>
       </c>
-      <c r="B152" s="41" t="s">
+      <c r="B152" s="43" t="s">
         <v>153</v>
       </c>
       <c r="C152">
@@ -3401,7 +3405,7 @@
       <c r="A153">
         <v>3223</v>
       </c>
-      <c r="B153" s="41" t="s">
+      <c r="B153" s="43" t="s">
         <v>154</v>
       </c>
       <c r="C153">
@@ -3412,7 +3416,7 @@
       <c r="A154">
         <v>3224</v>
       </c>
-      <c r="B154" s="41" t="s">
+      <c r="B154" s="43" t="s">
         <v>155</v>
       </c>
       <c r="C154">
@@ -3423,7 +3427,7 @@
       <c r="A155">
         <v>3225</v>
       </c>
-      <c r="B155" s="41" t="s">
+      <c r="B155" s="43" t="s">
         <v>156</v>
       </c>
       <c r="C155">
@@ -3434,7 +3438,7 @@
       <c r="A156">
         <v>3231</v>
       </c>
-      <c r="B156" s="41" t="s">
+      <c r="B156" s="43" t="s">
         <v>157</v>
       </c>
       <c r="C156">
@@ -3445,7 +3449,7 @@
       <c r="A157">
         <v>3232</v>
       </c>
-      <c r="B157" s="41" t="s">
+      <c r="B157" s="43" t="s">
         <v>158</v>
       </c>
       <c r="C157">
@@ -3456,7 +3460,7 @@
       <c r="A158">
         <v>3241</v>
       </c>
-      <c r="B158" s="41" t="s">
+      <c r="B158" s="43" t="s">
         <v>159</v>
       </c>
       <c r="C158">
@@ -3467,7 +3471,7 @@
       <c r="A159">
         <v>3242</v>
       </c>
-      <c r="B159" s="41" t="s">
+      <c r="B159" s="43" t="s">
         <v>160</v>
       </c>
       <c r="C159">
@@ -3478,7 +3482,7 @@
       <c r="A160">
         <v>3250</v>
       </c>
-      <c r="B160" s="41" t="s">
+      <c r="B160" s="43" t="s">
         <v>161</v>
       </c>
       <c r="C160">
@@ -3489,7 +3493,7 @@
       <c r="A161">
         <v>3251</v>
       </c>
-      <c r="B161" s="41" t="s">
+      <c r="B161" s="43" t="s">
         <v>162</v>
       </c>
       <c r="C161">
@@ -3500,7 +3504,7 @@
       <c r="A162">
         <v>3252</v>
       </c>
-      <c r="B162" s="41" t="s">
+      <c r="B162" s="43" t="s">
         <v>163</v>
       </c>
       <c r="C162">
@@ -3511,7 +3515,7 @@
       <c r="A163">
         <v>3253</v>
       </c>
-      <c r="B163" s="41" t="s">
+      <c r="B163" s="43" t="s">
         <v>164</v>
       </c>
       <c r="C163">
@@ -3522,7 +3526,7 @@
       <c r="A164">
         <v>3281</v>
       </c>
-      <c r="B164" s="41" t="s">
+      <c r="B164" s="43" t="s">
         <v>165</v>
       </c>
       <c r="C164">
@@ -3533,7 +3537,7 @@
       <c r="A165">
         <v>3311</v>
       </c>
-      <c r="B165" s="41" t="s">
+      <c r="B165" s="43" t="s">
         <v>166</v>
       </c>
       <c r="C165">
@@ -3544,7 +3548,7 @@
       <c r="A166">
         <v>3312</v>
       </c>
-      <c r="B166" s="41" t="s">
+      <c r="B166" s="43" t="s">
         <v>167</v>
       </c>
       <c r="C166">
@@ -3555,7 +3559,7 @@
       <c r="A167">
         <v>3313</v>
       </c>
-      <c r="B167" s="41" t="s">
+      <c r="B167" s="43" t="s">
         <v>168</v>
       </c>
       <c r="C167">
@@ -3566,7 +3570,7 @@
       <c r="A168">
         <v>3321</v>
       </c>
-      <c r="B168" s="41" t="s">
+      <c r="B168" s="43" t="s">
         <v>169</v>
       </c>
       <c r="C168">
@@ -3577,7 +3581,7 @@
       <c r="A169">
         <v>3322</v>
       </c>
-      <c r="B169" s="41" t="s">
+      <c r="B169" s="43" t="s">
         <v>170</v>
       </c>
       <c r="C169">
@@ -3588,7 +3592,7 @@
       <c r="A170">
         <v>3331</v>
       </c>
-      <c r="B170" s="41" t="s">
+      <c r="B170" s="43" t="s">
         <v>171</v>
       </c>
       <c r="C170">
@@ -3599,7 +3603,7 @@
       <c r="A171">
         <v>3341</v>
       </c>
-      <c r="B171" s="41" t="s">
+      <c r="B171" s="43" t="s">
         <v>172</v>
       </c>
       <c r="C171">
@@ -3610,7 +3614,7 @@
       <c r="A172">
         <v>3411</v>
       </c>
-      <c r="B172" s="41" t="s">
+      <c r="B172" s="43" t="s">
         <v>173</v>
       </c>
       <c r="C172">
@@ -3621,7 +3625,7 @@
       <c r="A173">
         <v>3412</v>
       </c>
-      <c r="B173" s="41" t="s">
+      <c r="B173" s="43" t="s">
         <v>174</v>
       </c>
       <c r="C173">
@@ -3632,7 +3636,7 @@
       <c r="A174">
         <v>3413</v>
       </c>
-      <c r="B174" s="41" t="s">
+      <c r="B174" s="43" t="s">
         <v>175</v>
       </c>
       <c r="C174">
@@ -3643,7 +3647,7 @@
       <c r="A175">
         <v>3421</v>
       </c>
-      <c r="B175" s="41" t="s">
+      <c r="B175" s="43" t="s">
         <v>176</v>
       </c>
       <c r="C175">
@@ -3654,7 +3658,7 @@
       <c r="A176">
         <v>3422</v>
       </c>
-      <c r="B176" s="41" t="s">
+      <c r="B176" s="43" t="s">
         <v>177</v>
       </c>
       <c r="C176">
@@ -3665,7 +3669,7 @@
       <c r="A177">
         <v>3423</v>
       </c>
-      <c r="B177" s="41" t="s">
+      <c r="B177" s="43" t="s">
         <v>178</v>
       </c>
       <c r="C177">
@@ -3676,7 +3680,7 @@
       <c r="A178">
         <v>3424</v>
       </c>
-      <c r="B178" s="41" t="s">
+      <c r="B178" s="43" t="s">
         <v>179</v>
       </c>
       <c r="C178">
@@ -3687,7 +3691,7 @@
       <c r="A179">
         <v>3425</v>
       </c>
-      <c r="B179" s="41" t="s">
+      <c r="B179" s="43" t="s">
         <v>180</v>
       </c>
       <c r="C179">
@@ -3698,7 +3702,7 @@
       <c r="A180">
         <v>3426</v>
       </c>
-      <c r="B180" s="41" t="s">
+      <c r="B180" s="43" t="s">
         <v>181</v>
       </c>
       <c r="C180">
@@ -3709,7 +3713,7 @@
       <c r="A181">
         <v>3511</v>
       </c>
-      <c r="B181" s="41" t="s">
+      <c r="B181" s="43" t="s">
         <v>182</v>
       </c>
       <c r="C181">
@@ -3720,7 +3724,7 @@
       <c r="A182">
         <v>3512</v>
       </c>
-      <c r="B182" s="41" t="s">
+      <c r="B182" s="43" t="s">
         <v>183</v>
       </c>
       <c r="C182">
@@ -3731,7 +3735,7 @@
       <c r="A183">
         <v>3513</v>
       </c>
-      <c r="B183" s="41" t="s">
+      <c r="B183" s="43" t="s">
         <v>184</v>
       </c>
       <c r="C183">
@@ -3742,7 +3746,7 @@
       <c r="A184">
         <v>3514</v>
       </c>
-      <c r="B184" s="41" t="s">
+      <c r="B184" s="43" t="s">
         <v>185</v>
       </c>
       <c r="C184">
@@ -3753,7 +3757,7 @@
       <c r="A185">
         <v>3515</v>
       </c>
-      <c r="B185" s="41" t="s">
+      <c r="B185" s="43" t="s">
         <v>186</v>
       </c>
       <c r="C185">
@@ -3764,7 +3768,7 @@
       <c r="A186">
         <v>3516</v>
       </c>
-      <c r="B186" s="41" t="s">
+      <c r="B186" s="43" t="s">
         <v>187</v>
       </c>
       <c r="C186">
@@ -3775,7 +3779,7 @@
       <c r="A187">
         <v>3517</v>
       </c>
-      <c r="B187" s="41" t="s">
+      <c r="B187" s="43" t="s">
         <v>188</v>
       </c>
       <c r="C187">
@@ -3786,7 +3790,7 @@
       <c r="A188">
         <v>3518</v>
       </c>
-      <c r="B188" s="41" t="s">
+      <c r="B188" s="43" t="s">
         <v>189</v>
       </c>
       <c r="C188">
@@ -3797,7 +3801,7 @@
       <c r="A189">
         <v>3522</v>
       </c>
-      <c r="B189" s="41" t="s">
+      <c r="B189" s="43" t="s">
         <v>190</v>
       </c>
       <c r="C189">
@@ -3808,7 +3812,7 @@
       <c r="A190">
         <v>3523</v>
       </c>
-      <c r="B190" s="41" t="s">
+      <c r="B190" s="43" t="s">
         <v>191</v>
       </c>
       <c r="C190">
@@ -3819,7 +3823,7 @@
       <c r="A191">
         <v>3524</v>
       </c>
-      <c r="B191" s="41" t="s">
+      <c r="B191" s="43" t="s">
         <v>192</v>
       </c>
       <c r="C191">
@@ -3830,7 +3834,7 @@
       <c r="A192">
         <v>3525</v>
       </c>
-      <c r="B192" s="41" t="s">
+      <c r="B192" s="43" t="s">
         <v>193</v>
       </c>
       <c r="C192">
@@ -3841,7 +3845,7 @@
       <c r="A193">
         <v>3531</v>
       </c>
-      <c r="B193" s="41" t="s">
+      <c r="B193" s="43" t="s">
         <v>194</v>
       </c>
       <c r="C193">
@@ -3852,7 +3856,7 @@
       <c r="A194">
         <v>3532</v>
       </c>
-      <c r="B194" s="41" t="s">
+      <c r="B194" s="43" t="s">
         <v>195</v>
       </c>
       <c r="C194">
@@ -3863,7 +3867,7 @@
       <c r="A195">
         <v>3541</v>
       </c>
-      <c r="B195" s="41" t="s">
+      <c r="B195" s="43" t="s">
         <v>196</v>
       </c>
       <c r="C195">
@@ -3874,7 +3878,7 @@
       <c r="A196">
         <v>3542</v>
       </c>
-      <c r="B196" s="41" t="s">
+      <c r="B196" s="43" t="s">
         <v>197</v>
       </c>
       <c r="C196">
@@ -3885,7 +3889,7 @@
       <c r="A197">
         <v>3543</v>
       </c>
-      <c r="B197" s="41" t="s">
+      <c r="B197" s="43" t="s">
         <v>198</v>
       </c>
       <c r="C197">
@@ -3896,7 +3900,7 @@
       <c r="A198">
         <v>3544</v>
       </c>
-      <c r="B198" s="41" t="s">
+      <c r="B198" s="43" t="s">
         <v>199</v>
       </c>
       <c r="C198">
@@ -3907,7 +3911,7 @@
       <c r="A199">
         <v>3545</v>
       </c>
-      <c r="B199" s="41" t="s">
+      <c r="B199" s="43" t="s">
         <v>200</v>
       </c>
       <c r="C199">
@@ -3918,7 +3922,7 @@
       <c r="A200">
         <v>3546</v>
       </c>
-      <c r="B200" s="41" t="s">
+      <c r="B200" s="43" t="s">
         <v>201</v>
       </c>
       <c r="C200">
@@ -3929,7 +3933,7 @@
       <c r="A201">
         <v>3547</v>
       </c>
-      <c r="B201" s="41" t="s">
+      <c r="B201" s="43" t="s">
         <v>202</v>
       </c>
       <c r="C201">
@@ -3940,7 +3944,7 @@
       <c r="A202">
         <v>3548</v>
       </c>
-      <c r="B202" s="41" t="s">
+      <c r="B202" s="43" t="s">
         <v>203</v>
       </c>
       <c r="C202">
@@ -3951,7 +3955,7 @@
       <c r="A203">
         <v>3711</v>
       </c>
-      <c r="B203" s="41" t="s">
+      <c r="B203" s="43" t="s">
         <v>204</v>
       </c>
       <c r="C203">
@@ -3962,7 +3966,7 @@
       <c r="A204">
         <v>3712</v>
       </c>
-      <c r="B204" s="41" t="s">
+      <c r="B204" s="43" t="s">
         <v>205</v>
       </c>
       <c r="C204">
@@ -3973,7 +3977,7 @@
       <c r="A205">
         <v>3713</v>
       </c>
-      <c r="B205" s="41" t="s">
+      <c r="B205" s="43" t="s">
         <v>206</v>
       </c>
       <c r="C205">
@@ -3984,7 +3988,7 @@
       <c r="A206">
         <v>3721</v>
       </c>
-      <c r="B206" s="41" t="s">
+      <c r="B206" s="43" t="s">
         <v>207</v>
       </c>
       <c r="C206">
@@ -3995,7 +3999,7 @@
       <c r="A207">
         <v>3722</v>
       </c>
-      <c r="B207" s="41" t="s">
+      <c r="B207" s="43" t="s">
         <v>208</v>
       </c>
       <c r="C207">
@@ -4006,7 +4010,7 @@
       <c r="A208">
         <v>3723</v>
       </c>
-      <c r="B208" s="41" t="s">
+      <c r="B208" s="43" t="s">
         <v>209</v>
       </c>
       <c r="C208">
@@ -4017,7 +4021,7 @@
       <c r="A209">
         <v>3731</v>
       </c>
-      <c r="B209" s="41" t="s">
+      <c r="B209" s="43" t="s">
         <v>210</v>
       </c>
       <c r="C209">
@@ -4028,7 +4032,7 @@
       <c r="A210">
         <v>3732</v>
       </c>
-      <c r="B210" s="41" t="s">
+      <c r="B210" s="43" t="s">
         <v>211</v>
       </c>
       <c r="C210">
@@ -4039,7 +4043,7 @@
       <c r="A211">
         <v>3741</v>
       </c>
-      <c r="B211" s="41" t="s">
+      <c r="B211" s="43" t="s">
         <v>212</v>
       </c>
       <c r="C211">
@@ -4050,7 +4054,7 @@
       <c r="A212">
         <v>3742</v>
       </c>
-      <c r="B212" s="41" t="s">
+      <c r="B212" s="43" t="s">
         <v>213</v>
       </c>
       <c r="C212">
@@ -4061,7 +4065,7 @@
       <c r="A213">
         <v>3743</v>
       </c>
-      <c r="B213" s="41" t="s">
+      <c r="B213" s="43" t="s">
         <v>214</v>
       </c>
       <c r="C213">
@@ -4072,7 +4076,7 @@
       <c r="A214">
         <v>3751</v>
       </c>
-      <c r="B214" s="41" t="s">
+      <c r="B214" s="43" t="s">
         <v>215</v>
       </c>
       <c r="C214">
@@ -4083,7 +4087,7 @@
       <c r="A215">
         <v>3761</v>
       </c>
-      <c r="B215" s="41" t="s">
+      <c r="B215" s="43" t="s">
         <v>216</v>
       </c>
       <c r="C215">
@@ -4094,7 +4098,7 @@
       <c r="A216">
         <v>3762</v>
       </c>
-      <c r="B216" s="41" t="s">
+      <c r="B216" s="43" t="s">
         <v>217</v>
       </c>
       <c r="C216">
@@ -4105,7 +4109,7 @@
       <c r="A217">
         <v>3763</v>
       </c>
-      <c r="B217" s="41" t="s">
+      <c r="B217" s="43" t="s">
         <v>218</v>
       </c>
       <c r="C217">
@@ -4116,7 +4120,7 @@
       <c r="A218">
         <v>3764</v>
       </c>
-      <c r="B218" s="41" t="s">
+      <c r="B218" s="43" t="s">
         <v>219</v>
       </c>
       <c r="C218">
@@ -4127,7 +4131,7 @@
       <c r="A219">
         <v>3765</v>
       </c>
-      <c r="B219" s="41" t="s">
+      <c r="B219" s="43" t="s">
         <v>220</v>
       </c>
       <c r="C219">
@@ -4138,7 +4142,7 @@
       <c r="A220">
         <v>3771</v>
       </c>
-      <c r="B220" s="41" t="s">
+      <c r="B220" s="43" t="s">
         <v>221</v>
       </c>
       <c r="C220">
@@ -4149,7 +4153,7 @@
       <c r="A221">
         <v>3772</v>
       </c>
-      <c r="B221" s="41" t="s">
+      <c r="B221" s="43" t="s">
         <v>222</v>
       </c>
       <c r="C221">
@@ -4160,7 +4164,7 @@
       <c r="A222">
         <v>3773</v>
       </c>
-      <c r="B222" s="41" t="s">
+      <c r="B222" s="43" t="s">
         <v>223</v>
       </c>
       <c r="C222">
@@ -4171,7 +4175,7 @@
       <c r="A223">
         <v>3911</v>
       </c>
-      <c r="B223" s="41" t="s">
+      <c r="B223" s="43" t="s">
         <v>224</v>
       </c>
       <c r="C223">
@@ -4182,7 +4186,7 @@
       <c r="A224">
         <v>3912</v>
       </c>
-      <c r="B224" s="41" t="s">
+      <c r="B224" s="43" t="s">
         <v>225</v>
       </c>
       <c r="C224">
@@ -4193,7 +4197,7 @@
       <c r="A225">
         <v>-1</v>
       </c>
-      <c r="B225" s="41" t="s">
+      <c r="B225" s="43" t="s">
         <v>226</v>
       </c>
       <c r="C225">
@@ -4204,7 +4208,7 @@
       <c r="A226">
         <v>4101</v>
       </c>
-      <c r="B226" s="41" t="s">
+      <c r="B226" s="43" t="s">
         <v>227</v>
       </c>
       <c r="C226">
@@ -4215,7 +4219,7 @@
       <c r="A227">
         <v>4102</v>
       </c>
-      <c r="B227" s="41" t="s">
+      <c r="B227" s="43" t="s">
         <v>228</v>
       </c>
       <c r="C227">
@@ -4226,7 +4230,7 @@
       <c r="A228">
         <v>4110</v>
       </c>
-      <c r="B228" s="41" t="s">
+      <c r="B228" s="43" t="s">
         <v>229</v>
       </c>
       <c r="C228">
@@ -4237,7 +4241,7 @@
       <c r="A229">
         <v>4121</v>
       </c>
-      <c r="B229" s="41" t="s">
+      <c r="B229" s="43" t="s">
         <v>230</v>
       </c>
       <c r="C229">
@@ -4248,7 +4252,7 @@
       <c r="A230">
         <v>4122</v>
       </c>
-      <c r="B230" s="41" t="s">
+      <c r="B230" s="43" t="s">
         <v>231</v>
       </c>
       <c r="C230">
@@ -4259,7 +4263,7 @@
       <c r="A231">
         <v>4123</v>
       </c>
-      <c r="B231" s="41" t="s">
+      <c r="B231" s="43" t="s">
         <v>232</v>
       </c>
       <c r="C231">
@@ -4270,7 +4274,7 @@
       <c r="A232">
         <v>4131</v>
       </c>
-      <c r="B232" s="41" t="s">
+      <c r="B232" s="43" t="s">
         <v>233</v>
       </c>
       <c r="C232">
@@ -4281,7 +4285,7 @@
       <c r="A233">
         <v>4132</v>
       </c>
-      <c r="B233" s="41" t="s">
+      <c r="B233" s="43" t="s">
         <v>234</v>
       </c>
       <c r="C233">
@@ -4292,7 +4296,7 @@
       <c r="A234">
         <v>4141</v>
       </c>
-      <c r="B234" s="41" t="s">
+      <c r="B234" s="43" t="s">
         <v>235</v>
       </c>
       <c r="C234">
@@ -4303,7 +4307,7 @@
       <c r="A235">
         <v>4142</v>
       </c>
-      <c r="B235" s="41" t="s">
+      <c r="B235" s="43" t="s">
         <v>236</v>
       </c>
       <c r="C235">
@@ -4314,7 +4318,7 @@
       <c r="A236">
         <v>4151</v>
       </c>
-      <c r="B236" s="41" t="s">
+      <c r="B236" s="43" t="s">
         <v>237</v>
       </c>
       <c r="C236">
@@ -4325,7 +4329,7 @@
       <c r="A237">
         <v>4152</v>
       </c>
-      <c r="B237" s="41" t="s">
+      <c r="B237" s="43" t="s">
         <v>238</v>
       </c>
       <c r="C237">
@@ -4336,7 +4340,7 @@
       <c r="A238">
         <v>4201</v>
       </c>
-      <c r="B238" s="41" t="s">
+      <c r="B238" s="43" t="s">
         <v>239</v>
       </c>
       <c r="C238">
@@ -4347,7 +4351,7 @@
       <c r="A239">
         <v>4211</v>
       </c>
-      <c r="B239" s="41" t="s">
+      <c r="B239" s="43" t="s">
         <v>240</v>
       </c>
       <c r="C239">
@@ -4358,7 +4362,7 @@
       <c r="A240">
         <v>4212</v>
       </c>
-      <c r="B240" s="41" t="s">
+      <c r="B240" s="43" t="s">
         <v>241</v>
       </c>
       <c r="C240">
@@ -4369,7 +4373,7 @@
       <c r="A241">
         <v>4213</v>
       </c>
-      <c r="B241" s="41" t="s">
+      <c r="B241" s="43" t="s">
         <v>242</v>
       </c>
       <c r="C241">
@@ -4380,7 +4384,7 @@
       <c r="A242">
         <v>4214</v>
       </c>
-      <c r="B242" s="41" t="s">
+      <c r="B242" s="43" t="s">
         <v>243</v>
       </c>
       <c r="C242">
@@ -4391,7 +4395,7 @@
       <c r="A243">
         <v>4221</v>
       </c>
-      <c r="B243" s="41" t="s">
+      <c r="B243" s="43" t="s">
         <v>244</v>
       </c>
       <c r="C243">
@@ -4402,7 +4406,7 @@
       <c r="A244">
         <v>4222</v>
       </c>
-      <c r="B244" s="41" t="s">
+      <c r="B244" s="43" t="s">
         <v>245</v>
       </c>
       <c r="C244">
@@ -4413,7 +4417,7 @@
       <c r="A245">
         <v>4223</v>
       </c>
-      <c r="B245" s="41" t="s">
+      <c r="B245" s="43" t="s">
         <v>246</v>
       </c>
       <c r="C245">
@@ -4424,7 +4428,7 @@
       <c r="A246">
         <v>4231</v>
       </c>
-      <c r="B246" s="41" t="s">
+      <c r="B246" s="43" t="s">
         <v>247</v>
       </c>
       <c r="C246">
@@ -4435,7 +4439,7 @@
       <c r="A247">
         <v>4241</v>
       </c>
-      <c r="B247" s="41" t="s">
+      <c r="B247" s="43" t="s">
         <v>248</v>
       </c>
       <c r="C247">
@@ -4446,7 +4450,7 @@
       <c r="A248">
         <v>-1</v>
       </c>
-      <c r="B248" s="41" t="s">
+      <c r="B248" s="43" t="s">
         <v>249</v>
       </c>
       <c r="C248">
@@ -4457,7 +4461,7 @@
       <c r="A249">
         <v>5101</v>
       </c>
-      <c r="B249" s="41" t="s">
+      <c r="B249" s="43" t="s">
         <v>250</v>
       </c>
       <c r="C249">
@@ -4468,7 +4472,7 @@
       <c r="A250">
         <v>5102</v>
       </c>
-      <c r="B250" s="41" t="s">
+      <c r="B250" s="43" t="s">
         <v>251</v>
       </c>
       <c r="C250">
@@ -4479,7 +4483,7 @@
       <c r="A251">
         <v>5103</v>
       </c>
-      <c r="B251" s="41" t="s">
+      <c r="B251" s="43" t="s">
         <v>252</v>
       </c>
       <c r="C251">
@@ -4490,7 +4494,7 @@
       <c r="A252">
         <v>5111</v>
       </c>
-      <c r="B252" s="41" t="s">
+      <c r="B252" s="43" t="s">
         <v>253</v>
       </c>
       <c r="C252">
@@ -4501,7 +4505,7 @@
       <c r="A253">
         <v>5112</v>
       </c>
-      <c r="B253" s="41" t="s">
+      <c r="B253" s="43" t="s">
         <v>254</v>
       </c>
       <c r="C253">
@@ -4512,7 +4516,7 @@
       <c r="A254">
         <v>5114</v>
       </c>
-      <c r="B254" s="41" t="s">
+      <c r="B254" s="43" t="s">
         <v>255</v>
       </c>
       <c r="C254">
@@ -4523,7 +4527,7 @@
       <c r="A255">
         <v>5121</v>
       </c>
-      <c r="B255" s="41" t="s">
+      <c r="B255" s="43" t="s">
         <v>256</v>
       </c>
       <c r="C255">
@@ -4534,7 +4538,7 @@
       <c r="A256">
         <v>5131</v>
       </c>
-      <c r="B256" s="41" t="s">
+      <c r="B256" s="43" t="s">
         <v>257</v>
       </c>
       <c r="C256">
@@ -4545,7 +4549,7 @@
       <c r="A257">
         <v>5132</v>
       </c>
-      <c r="B257" s="41" t="s">
+      <c r="B257" s="43" t="s">
         <v>258</v>
       </c>
       <c r="C257">
@@ -4556,7 +4560,7 @@
       <c r="A258">
         <v>5133</v>
       </c>
-      <c r="B258" s="41" t="s">
+      <c r="B258" s="43" t="s">
         <v>259</v>
       </c>
       <c r="C258">
@@ -4567,7 +4571,7 @@
       <c r="A259">
         <v>5134</v>
       </c>
-      <c r="B259" s="41" t="s">
+      <c r="B259" s="43" t="s">
         <v>260</v>
       </c>
       <c r="C259">
@@ -4578,7 +4582,7 @@
       <c r="A260">
         <v>5141</v>
       </c>
-      <c r="B260" s="41" t="s">
+      <c r="B260" s="43" t="s">
         <v>261</v>
       </c>
       <c r="C260">
@@ -4589,7 +4593,7 @@
       <c r="A261">
         <v>5142</v>
       </c>
-      <c r="B261" s="41" t="s">
+      <c r="B261" s="43" t="s">
         <v>262</v>
       </c>
       <c r="C261">
@@ -4600,7 +4604,7 @@
       <c r="A262">
         <v>5151</v>
       </c>
-      <c r="B262" s="41" t="s">
+      <c r="B262" s="43" t="s">
         <v>263</v>
       </c>
       <c r="C262">
@@ -4611,7 +4615,7 @@
       <c r="A263">
         <v>5152</v>
       </c>
-      <c r="B263" s="41" t="s">
+      <c r="B263" s="43" t="s">
         <v>264</v>
       </c>
       <c r="C263">
@@ -4622,7 +4626,7 @@
       <c r="A264">
         <v>5161</v>
       </c>
-      <c r="B264" s="41" t="s">
+      <c r="B264" s="43" t="s">
         <v>265</v>
       </c>
       <c r="C264">
@@ -4633,7 +4637,7 @@
       <c r="A265">
         <v>5162</v>
       </c>
-      <c r="B265" s="41" t="s">
+      <c r="B265" s="43" t="s">
         <v>266</v>
       </c>
       <c r="C265">
@@ -4644,7 +4648,7 @@
       <c r="A266">
         <v>5165</v>
       </c>
-      <c r="B266" s="41" t="s">
+      <c r="B266" s="43" t="s">
         <v>267</v>
       </c>
       <c r="C266">
@@ -4655,7 +4659,7 @@
       <c r="A267">
         <v>5166</v>
       </c>
-      <c r="B267" s="41" t="s">
+      <c r="B267" s="43" t="s">
         <v>268</v>
       </c>
       <c r="C267">
@@ -4666,7 +4670,7 @@
       <c r="A268">
         <v>5167</v>
       </c>
-      <c r="B268" s="41" t="s">
+      <c r="B268" s="43" t="s">
         <v>269</v>
       </c>
       <c r="C268">
@@ -4677,7 +4681,7 @@
       <c r="A269">
         <v>5169</v>
       </c>
-      <c r="B269" s="41" t="s">
+      <c r="B269" s="43" t="s">
         <v>270</v>
       </c>
       <c r="C269">
@@ -4688,7 +4692,7 @@
       <c r="A270">
         <v>5171</v>
       </c>
-      <c r="B270" s="41" t="s">
+      <c r="B270" s="43" t="s">
         <v>271</v>
       </c>
       <c r="C270">
@@ -4699,7 +4703,7 @@
       <c r="A271">
         <v>5172</v>
       </c>
-      <c r="B271" s="41" t="s">
+      <c r="B271" s="43" t="s">
         <v>272</v>
       </c>
       <c r="C271">
@@ -4710,7 +4714,7 @@
       <c r="A272">
         <v>5173</v>
       </c>
-      <c r="B272" s="41" t="s">
+      <c r="B272" s="43" t="s">
         <v>273</v>
       </c>
       <c r="C272">
@@ -4721,7 +4725,7 @@
       <c r="A273">
         <v>5174</v>
       </c>
-      <c r="B273" s="41" t="s">
+      <c r="B273" s="43" t="s">
         <v>274</v>
       </c>
       <c r="C273">
@@ -4732,7 +4736,7 @@
       <c r="A274">
         <v>5191</v>
       </c>
-      <c r="B274" s="41" t="s">
+      <c r="B274" s="43" t="s">
         <v>275</v>
       </c>
       <c r="C274">
@@ -4743,7 +4747,7 @@
       <c r="A275">
         <v>5192</v>
       </c>
-      <c r="B275" s="41" t="s">
+      <c r="B275" s="43" t="s">
         <v>276</v>
       </c>
       <c r="C275">
@@ -4754,7 +4758,7 @@
       <c r="A276">
         <v>5198</v>
       </c>
-      <c r="B276" s="41" t="s">
+      <c r="B276" s="43" t="s">
         <v>277</v>
       </c>
       <c r="C276">
@@ -4765,7 +4769,7 @@
       <c r="A277">
         <v>5199</v>
       </c>
-      <c r="B277" s="41" t="s">
+      <c r="B277" s="43" t="s">
         <v>278</v>
       </c>
       <c r="C277">
@@ -4776,7 +4780,7 @@
       <c r="A278">
         <v>5201</v>
       </c>
-      <c r="B278" s="41" t="s">
+      <c r="B278" s="43" t="s">
         <v>279</v>
       </c>
       <c r="C278">
@@ -4787,7 +4791,7 @@
       <c r="A279">
         <v>5211</v>
       </c>
-      <c r="B279" s="41" t="s">
+      <c r="B279" s="43" t="s">
         <v>280</v>
       </c>
       <c r="C279">
@@ -4798,7 +4802,7 @@
       <c r="A280">
         <v>5221</v>
       </c>
-      <c r="B280" s="41" t="s">
+      <c r="B280" s="43" t="s">
         <v>281</v>
       </c>
       <c r="C280">
@@ -4809,7 +4813,7 @@
       <c r="A281">
         <v>5231</v>
       </c>
-      <c r="B281" s="41" t="s">
+      <c r="B281" s="43" t="s">
         <v>282</v>
       </c>
       <c r="C281">
@@ -4820,7 +4824,7 @@
       <c r="A282">
         <v>5241</v>
       </c>
-      <c r="B282" s="41" t="s">
+      <c r="B282" s="43" t="s">
         <v>283</v>
       </c>
       <c r="C282">
@@ -4831,7 +4835,7 @@
       <c r="A283">
         <v>5242</v>
       </c>
-      <c r="B283" s="41" t="s">
+      <c r="B283" s="43" t="s">
         <v>284</v>
       </c>
       <c r="C283">
@@ -4842,7 +4846,7 @@
       <c r="A284">
         <v>5243</v>
       </c>
-      <c r="B284" s="41" t="s">
+      <c r="B284" s="43" t="s">
         <v>285</v>
       </c>
       <c r="C284">
@@ -4853,7 +4857,7 @@
       <c r="A285">
         <v>-1</v>
       </c>
-      <c r="B285" s="41" t="s">
+      <c r="B285" s="43" t="s">
         <v>286</v>
       </c>
       <c r="C285">
@@ -4864,7 +4868,7 @@
       <c r="A286">
         <v>6110</v>
       </c>
-      <c r="B286" s="41" t="s">
+      <c r="B286" s="43" t="s">
         <v>287</v>
       </c>
       <c r="C286">
@@ -4875,7 +4879,7 @@
       <c r="A287">
         <v>6129</v>
       </c>
-      <c r="B287" s="41" t="s">
+      <c r="B287" s="43" t="s">
         <v>288</v>
       </c>
       <c r="C287">
@@ -4886,7 +4890,7 @@
       <c r="A288">
         <v>6139</v>
       </c>
-      <c r="B288" s="41" t="s">
+      <c r="B288" s="43" t="s">
         <v>289</v>
       </c>
       <c r="C288">
@@ -4897,7 +4901,7 @@
       <c r="A289">
         <v>6201</v>
       </c>
-      <c r="B289" s="41" t="s">
+      <c r="B289" s="43" t="s">
         <v>290</v>
       </c>
       <c r="C289">
@@ -4908,7 +4912,7 @@
       <c r="A290">
         <v>6210</v>
       </c>
-      <c r="B290" s="41" t="s">
+      <c r="B290" s="43" t="s">
         <v>291</v>
       </c>
       <c r="C290">
@@ -4919,7 +4923,7 @@
       <c r="A291">
         <v>6229</v>
       </c>
-      <c r="B291" s="41" t="s">
+      <c r="B291" s="43" t="s">
         <v>292</v>
       </c>
       <c r="C291">
@@ -4930,7 +4934,7 @@
       <c r="A292">
         <v>6239</v>
       </c>
-      <c r="B292" s="41" t="s">
+      <c r="B292" s="43" t="s">
         <v>293</v>
       </c>
       <c r="C292">
@@ -4941,7 +4945,7 @@
       <c r="A293">
         <v>6301</v>
       </c>
-      <c r="B293" s="41" t="s">
+      <c r="B293" s="43" t="s">
         <v>294</v>
       </c>
       <c r="C293">
@@ -4952,7 +4956,7 @@
       <c r="A294">
         <v>6319</v>
       </c>
-      <c r="B294" s="41" t="s">
+      <c r="B294" s="43" t="s">
         <v>295</v>
       </c>
       <c r="C294">
@@ -4963,7 +4967,7 @@
       <c r="A295">
         <v>6329</v>
       </c>
-      <c r="B295" s="41" t="s">
+      <c r="B295" s="43" t="s">
         <v>296</v>
       </c>
       <c r="C295">
@@ -4974,7 +4978,7 @@
       <c r="A296">
         <v>6410</v>
       </c>
-      <c r="B296" s="41" t="s">
+      <c r="B296" s="43" t="s">
         <v>297</v>
       </c>
       <c r="C296">
@@ -4985,7 +4989,7 @@
       <c r="A297">
         <v>6420</v>
       </c>
-      <c r="B297" s="41" t="s">
+      <c r="B297" s="43" t="s">
         <v>298</v>
       </c>
       <c r="C297">
@@ -4996,7 +5000,7 @@
       <c r="A298">
         <v>6430</v>
       </c>
-      <c r="B298" s="41" t="s">
+      <c r="B298" s="43" t="s">
         <v>299</v>
       </c>
       <c r="C298">
@@ -5007,7 +5011,7 @@
       <c r="A299">
         <v>-1</v>
       </c>
-      <c r="B299" s="41" t="s">
+      <c r="B299" s="43" t="s">
         <v>300</v>
       </c>
       <c r="C299">
@@ -5018,7 +5022,7 @@
       <c r="A300">
         <v>7101</v>
       </c>
-      <c r="B300" s="41" t="s">
+      <c r="B300" s="43" t="s">
         <v>301</v>
       </c>
       <c r="C300">
@@ -5029,7 +5033,7 @@
       <c r="A301">
         <v>7102</v>
       </c>
-      <c r="B301" s="41" t="s">
+      <c r="B301" s="43" t="s">
         <v>302</v>
       </c>
       <c r="C301">
@@ -5040,7 +5044,7 @@
       <c r="A302">
         <v>7111</v>
       </c>
-      <c r="B302" s="41" t="s">
+      <c r="B302" s="43" t="s">
         <v>303</v>
       </c>
       <c r="C302">
@@ -5051,7 +5055,7 @@
       <c r="A303">
         <v>7112</v>
       </c>
-      <c r="B303" s="41" t="s">
+      <c r="B303" s="43" t="s">
         <v>304</v>
       </c>
       <c r="C303">
@@ -5062,7 +5066,7 @@
       <c r="A304">
         <v>7113</v>
       </c>
-      <c r="B304" s="41" t="s">
+      <c r="B304" s="43" t="s">
         <v>305</v>
       </c>
       <c r="C304">
@@ -5073,7 +5077,7 @@
       <c r="A305">
         <v>7114</v>
       </c>
-      <c r="B305" s="41" t="s">
+      <c r="B305" s="43" t="s">
         <v>306</v>
       </c>
       <c r="C305">
@@ -5084,7 +5088,7 @@
       <c r="A306">
         <v>7121</v>
       </c>
-      <c r="B306" s="41" t="s">
+      <c r="B306" s="43" t="s">
         <v>307</v>
       </c>
       <c r="C306">
@@ -5095,7 +5099,7 @@
       <c r="A307">
         <v>7122</v>
       </c>
-      <c r="B307" s="41" t="s">
+      <c r="B307" s="43" t="s">
         <v>308</v>
       </c>
       <c r="C307">
@@ -5106,7 +5110,7 @@
       <c r="A308">
         <v>7151</v>
       </c>
-      <c r="B308" s="41" t="s">
+      <c r="B308" s="43" t="s">
         <v>309</v>
       </c>
       <c r="C308">
@@ -5117,7 +5121,7 @@
       <c r="A309">
         <v>7152</v>
       </c>
-      <c r="B309" s="41" t="s">
+      <c r="B309" s="43" t="s">
         <v>310</v>
       </c>
       <c r="C309">
@@ -5128,7 +5132,7 @@
       <c r="A310">
         <v>7153</v>
       </c>
-      <c r="B310" s="41" t="s">
+      <c r="B310" s="43" t="s">
         <v>311</v>
       </c>
       <c r="C310">
@@ -5139,7 +5143,7 @@
       <c r="A311">
         <v>7154</v>
       </c>
-      <c r="B311" s="41" t="s">
+      <c r="B311" s="43" t="s">
         <v>312</v>
       </c>
       <c r="C311">
@@ -5150,7 +5154,7 @@
       <c r="A312">
         <v>7155</v>
       </c>
-      <c r="B312" s="41" t="s">
+      <c r="B312" s="43" t="s">
         <v>313</v>
       </c>
       <c r="C312">
@@ -5161,7 +5165,7 @@
       <c r="A313">
         <v>7156</v>
       </c>
-      <c r="B313" s="41" t="s">
+      <c r="B313" s="43" t="s">
         <v>314</v>
       </c>
       <c r="C313">
@@ -5172,7 +5176,7 @@
       <c r="A314">
         <v>7157</v>
       </c>
-      <c r="B314" s="41" t="s">
+      <c r="B314" s="43" t="s">
         <v>315</v>
       </c>
       <c r="C314">
@@ -5183,7 +5187,7 @@
       <c r="A315">
         <v>7161</v>
       </c>
-      <c r="B315" s="41" t="s">
+      <c r="B315" s="43" t="s">
         <v>316</v>
       </c>
       <c r="C315">
@@ -5194,7 +5198,7 @@
       <c r="A316">
         <v>7162</v>
       </c>
-      <c r="B316" s="41" t="s">
+      <c r="B316" s="43" t="s">
         <v>317</v>
       </c>
       <c r="C316">
@@ -5205,7 +5209,7 @@
       <c r="A317">
         <v>7163</v>
       </c>
-      <c r="B317" s="41" t="s">
+      <c r="B317" s="43" t="s">
         <v>318</v>
       </c>
       <c r="C317">
@@ -5216,7 +5220,7 @@
       <c r="A318">
         <v>7164</v>
       </c>
-      <c r="B318" s="41" t="s">
+      <c r="B318" s="43" t="s">
         <v>319</v>
       </c>
       <c r="C318">
@@ -5227,7 +5231,7 @@
       <c r="A319">
         <v>7165</v>
       </c>
-      <c r="B319" s="41" t="s">
+      <c r="B319" s="43" t="s">
         <v>320</v>
       </c>
       <c r="C319">
@@ -5238,7 +5242,7 @@
       <c r="A320">
         <v>7166</v>
       </c>
-      <c r="B320" s="41" t="s">
+      <c r="B320" s="43" t="s">
         <v>321</v>
       </c>
       <c r="C320">
@@ -5249,7 +5253,7 @@
       <c r="A321">
         <v>7170</v>
       </c>
-      <c r="B321" s="41" t="s">
+      <c r="B321" s="43" t="s">
         <v>322</v>
       </c>
       <c r="C321">
@@ -5260,7 +5264,7 @@
       <c r="A322">
         <v>7201</v>
       </c>
-      <c r="B322" s="41" t="s">
+      <c r="B322" s="43" t="s">
         <v>323</v>
       </c>
       <c r="C322">
@@ -5271,7 +5275,7 @@
       <c r="A323">
         <v>7202</v>
       </c>
-      <c r="B323" s="41" t="s">
+      <c r="B323" s="43" t="s">
         <v>324</v>
       </c>
       <c r="C323">
@@ -5282,7 +5286,7 @@
       <c r="A324">
         <v>7211</v>
       </c>
-      <c r="B324" s="41" t="s">
+      <c r="B324" s="43" t="s">
         <v>325</v>
       </c>
       <c r="C324">
@@ -5293,7 +5297,7 @@
       <c r="A325">
         <v>7212</v>
       </c>
-      <c r="B325" s="41" t="s">
+      <c r="B325" s="43" t="s">
         <v>326</v>
       </c>
       <c r="C325">
@@ -5304,7 +5308,7 @@
       <c r="A326">
         <v>7213</v>
       </c>
-      <c r="B326" s="41" t="s">
+      <c r="B326" s="43" t="s">
         <v>327</v>
       </c>
       <c r="C326">
@@ -5315,7 +5319,7 @@
       <c r="A327">
         <v>7214</v>
       </c>
-      <c r="B327" s="41" t="s">
+      <c r="B327" s="43" t="s">
         <v>328</v>
       </c>
       <c r="C327">
@@ -5326,7 +5330,7 @@
       <c r="A328">
         <v>7215</v>
       </c>
-      <c r="B328" s="41" t="s">
+      <c r="B328" s="43" t="s">
         <v>329</v>
       </c>
       <c r="C328">
@@ -5337,7 +5341,7 @@
       <c r="A329">
         <v>7221</v>
       </c>
-      <c r="B329" s="41" t="s">
+      <c r="B329" s="43" t="s">
         <v>330</v>
       </c>
       <c r="C329">
@@ -5348,7 +5352,7 @@
       <c r="A330">
         <v>7222</v>
       </c>
-      <c r="B330" s="41" t="s">
+      <c r="B330" s="43" t="s">
         <v>331</v>
       </c>
       <c r="C330">
@@ -5359,7 +5363,7 @@
       <c r="A331">
         <v>7223</v>
       </c>
-      <c r="B331" s="41" t="s">
+      <c r="B331" s="43" t="s">
         <v>332</v>
       </c>
       <c r="C331">
@@ -5370,7 +5374,7 @@
       <c r="A332">
         <v>7224</v>
       </c>
-      <c r="B332" s="41" t="s">
+      <c r="B332" s="43" t="s">
         <v>333</v>
       </c>
       <c r="C332">
@@ -5381,7 +5385,7 @@
       <c r="A333">
         <v>7231</v>
       </c>
-      <c r="B333" s="41" t="s">
+      <c r="B333" s="43" t="s">
         <v>334</v>
       </c>
       <c r="C333">
@@ -5392,7 +5396,7 @@
       <c r="A334">
         <v>7232</v>
       </c>
-      <c r="B334" s="41" t="s">
+      <c r="B334" s="43" t="s">
         <v>335</v>
       </c>
       <c r="C334">
@@ -5403,7 +5407,7 @@
       <c r="A335">
         <v>7233</v>
       </c>
-      <c r="B335" s="41" t="s">
+      <c r="B335" s="43" t="s">
         <v>336</v>
       </c>
       <c r="C335">
@@ -5414,7 +5418,7 @@
       <c r="A336">
         <v>7241</v>
       </c>
-      <c r="B336" s="41" t="s">
+      <c r="B336" s="43" t="s">
         <v>337</v>
       </c>
       <c r="C336">
@@ -5425,7 +5429,7 @@
       <c r="A337">
         <v>7242</v>
       </c>
-      <c r="B337" s="41" t="s">
+      <c r="B337" s="43" t="s">
         <v>338</v>
       </c>
       <c r="C337">
@@ -5436,7 +5440,7 @@
       <c r="A338">
         <v>7243</v>
       </c>
-      <c r="B338" s="41" t="s">
+      <c r="B338" s="43" t="s">
         <v>339</v>
       </c>
       <c r="C338">
@@ -5447,7 +5451,7 @@
       <c r="A339">
         <v>7244</v>
       </c>
-      <c r="B339" s="41" t="s">
+      <c r="B339" s="43" t="s">
         <v>340</v>
       </c>
       <c r="C339">
@@ -5458,7 +5462,7 @@
       <c r="A340">
         <v>7245</v>
       </c>
-      <c r="B340" s="41" t="s">
+      <c r="B340" s="43" t="s">
         <v>341</v>
       </c>
       <c r="C340">
@@ -5469,7 +5473,7 @@
       <c r="A341">
         <v>7246</v>
       </c>
-      <c r="B341" s="41" t="s">
+      <c r="B341" s="43" t="s">
         <v>342</v>
       </c>
       <c r="C341">
@@ -5480,7 +5484,7 @@
       <c r="A342">
         <v>7250</v>
       </c>
-      <c r="B342" s="41" t="s">
+      <c r="B342" s="43" t="s">
         <v>343</v>
       </c>
       <c r="C342">
@@ -5491,7 +5495,7 @@
       <c r="A343">
         <v>7251</v>
       </c>
-      <c r="B343" s="41" t="s">
+      <c r="B343" s="43" t="s">
         <v>344</v>
       </c>
       <c r="C343">
@@ -5502,7 +5506,7 @@
       <c r="A344">
         <v>7252</v>
       </c>
-      <c r="B344" s="41" t="s">
+      <c r="B344" s="43" t="s">
         <v>345</v>
       </c>
       <c r="C344">
@@ -5513,7 +5517,7 @@
       <c r="A345">
         <v>7253</v>
       </c>
-      <c r="B345" s="41" t="s">
+      <c r="B345" s="43" t="s">
         <v>346</v>
       </c>
       <c r="C345">
@@ -5524,7 +5528,7 @@
       <c r="A346">
         <v>7254</v>
       </c>
-      <c r="B346" s="41" t="s">
+      <c r="B346" s="43" t="s">
         <v>347</v>
       </c>
       <c r="C346">
@@ -5535,7 +5539,7 @@
       <c r="A347">
         <v>7255</v>
       </c>
-      <c r="B347" s="41" t="s">
+      <c r="B347" s="43" t="s">
         <v>348</v>
       </c>
       <c r="C347">
@@ -5546,7 +5550,7 @@
       <c r="A348">
         <v>7256</v>
       </c>
-      <c r="B348" s="41" t="s">
+      <c r="B348" s="43" t="s">
         <v>349</v>
       </c>
       <c r="C348">
@@ -5557,7 +5561,7 @@
       <c r="A349">
         <v>7257</v>
       </c>
-      <c r="B349" s="41" t="s">
+      <c r="B349" s="43" t="s">
         <v>350</v>
       </c>
       <c r="C349">
@@ -5568,7 +5572,7 @@
       <c r="A350">
         <v>7301</v>
       </c>
-      <c r="B350" s="41" t="s">
+      <c r="B350" s="43" t="s">
         <v>351</v>
       </c>
       <c r="C350">
@@ -5579,7 +5583,7 @@
       <c r="A351">
         <v>7311</v>
       </c>
-      <c r="B351" s="41" t="s">
+      <c r="B351" s="43" t="s">
         <v>352</v>
       </c>
       <c r="C351">
@@ -5590,7 +5594,7 @@
       <c r="A352">
         <v>7312</v>
       </c>
-      <c r="B352" s="41" t="s">
+      <c r="B352" s="43" t="s">
         <v>353</v>
       </c>
       <c r="C352">
@@ -5601,7 +5605,7 @@
       <c r="A353">
         <v>7313</v>
       </c>
-      <c r="B353" s="41" t="s">
+      <c r="B353" s="43" t="s">
         <v>354</v>
       </c>
       <c r="C353">
@@ -5612,7 +5616,7 @@
       <c r="A354">
         <v>7321</v>
       </c>
-      <c r="B354" s="41" t="s">
+      <c r="B354" s="43" t="s">
         <v>355</v>
       </c>
       <c r="C354">
@@ -5623,7 +5627,7 @@
       <c r="A355">
         <v>7401</v>
       </c>
-      <c r="B355" s="41" t="s">
+      <c r="B355" s="43" t="s">
         <v>356</v>
       </c>
       <c r="C355">
@@ -5634,7 +5638,7 @@
       <c r="A356">
         <v>7411</v>
       </c>
-      <c r="B356" s="41" t="s">
+      <c r="B356" s="43" t="s">
         <v>357</v>
       </c>
       <c r="C356">
@@ -5645,7 +5649,7 @@
       <c r="A357">
         <v>7421</v>
       </c>
-      <c r="B357" s="41" t="s">
+      <c r="B357" s="43" t="s">
         <v>358</v>
       </c>
       <c r="C357">
@@ -5656,7 +5660,7 @@
       <c r="A358">
         <v>7501</v>
       </c>
-      <c r="B358" s="41" t="s">
+      <c r="B358" s="43" t="s">
         <v>359</v>
       </c>
       <c r="C358">
@@ -5667,7 +5671,7 @@
       <c r="A359">
         <v>7502</v>
       </c>
-      <c r="B359" s="41" t="s">
+      <c r="B359" s="43" t="s">
         <v>360</v>
       </c>
       <c r="C359">
@@ -5678,7 +5682,7 @@
       <c r="A360">
         <v>7519</v>
       </c>
-      <c r="B360" s="41" t="s">
+      <c r="B360" s="43" t="s">
         <v>361</v>
       </c>
       <c r="C360">
@@ -5689,7 +5693,7 @@
       <c r="A361">
         <v>7521</v>
       </c>
-      <c r="B361" s="41" t="s">
+      <c r="B361" s="43" t="s">
         <v>362</v>
       </c>
       <c r="C361">
@@ -5700,7 +5704,7 @@
       <c r="A362">
         <v>7522</v>
       </c>
-      <c r="B362" s="41" t="s">
+      <c r="B362" s="43" t="s">
         <v>363</v>
       </c>
       <c r="C362">
@@ -5711,7 +5715,7 @@
       <c r="A363">
         <v>7523</v>
       </c>
-      <c r="B363" s="41" t="s">
+      <c r="B363" s="43" t="s">
         <v>364</v>
       </c>
       <c r="C363">
@@ -5722,7 +5726,7 @@
       <c r="A364">
         <v>7524</v>
       </c>
-      <c r="B364" s="41" t="s">
+      <c r="B364" s="43" t="s">
         <v>365</v>
       </c>
       <c r="C364">
@@ -5733,7 +5737,7 @@
       <c r="A365">
         <v>7601</v>
       </c>
-      <c r="B365" s="41" t="s">
+      <c r="B365" s="43" t="s">
         <v>366</v>
       </c>
       <c r="C365">
@@ -5744,7 +5748,7 @@
       <c r="A366">
         <v>7602</v>
       </c>
-      <c r="B366" s="41" t="s">
+      <c r="B366" s="43" t="s">
         <v>367</v>
       </c>
       <c r="C366">
@@ -5755,7 +5759,7 @@
       <c r="A367">
         <v>7603</v>
       </c>
-      <c r="B367" s="41" t="s">
+      <c r="B367" s="43" t="s">
         <v>368</v>
       </c>
       <c r="C367">
@@ -5766,7 +5770,7 @@
       <c r="A368">
         <v>7604</v>
       </c>
-      <c r="B368" s="41" t="s">
+      <c r="B368" s="43" t="s">
         <v>369</v>
       </c>
       <c r="C368">
@@ -5777,7 +5781,7 @@
       <c r="A369">
         <v>7605</v>
       </c>
-      <c r="B369" s="41" t="s">
+      <c r="B369" s="43" t="s">
         <v>370</v>
       </c>
       <c r="C369">
@@ -5788,7 +5792,7 @@
       <c r="A370">
         <v>7606</v>
       </c>
-      <c r="B370" s="41" t="s">
+      <c r="B370" s="43" t="s">
         <v>371</v>
       </c>
       <c r="C370">
@@ -5799,7 +5803,7 @@
       <c r="A371">
         <v>7610</v>
       </c>
-      <c r="B371" s="41" t="s">
+      <c r="B371" s="43" t="s">
         <v>372</v>
       </c>
       <c r="C371">
@@ -5810,7 +5814,7 @@
       <c r="A372">
         <v>7611</v>
       </c>
-      <c r="B372" s="41" t="s">
+      <c r="B372" s="43" t="s">
         <v>373</v>
       </c>
       <c r="C372">
@@ -5821,7 +5825,7 @@
       <c r="A373">
         <v>7612</v>
       </c>
-      <c r="B373" s="41" t="s">
+      <c r="B373" s="43" t="s">
         <v>374</v>
       </c>
       <c r="C373">
@@ -5832,7 +5836,7 @@
       <c r="A374">
         <v>7613</v>
       </c>
-      <c r="B374" s="41" t="s">
+      <c r="B374" s="43" t="s">
         <v>375</v>
       </c>
       <c r="C374">
@@ -5843,7 +5847,7 @@
       <c r="A375">
         <v>7614</v>
       </c>
-      <c r="B375" s="41" t="s">
+      <c r="B375" s="43" t="s">
         <v>376</v>
       </c>
       <c r="C375">
@@ -5854,7 +5858,7 @@
       <c r="A376">
         <v>7618</v>
       </c>
-      <c r="B376" s="41" t="s">
+      <c r="B376" s="43" t="s">
         <v>377</v>
       </c>
       <c r="C376">
@@ -5865,7 +5869,7 @@
       <c r="A377">
         <v>7620</v>
       </c>
-      <c r="B377" s="41" t="s">
+      <c r="B377" s="43" t="s">
         <v>378</v>
       </c>
       <c r="C377">
@@ -5876,7 +5880,7 @@
       <c r="A378">
         <v>7621</v>
       </c>
-      <c r="B378" s="41" t="s">
+      <c r="B378" s="43" t="s">
         <v>379</v>
       </c>
       <c r="C378">
@@ -5887,7 +5891,7 @@
       <c r="A379">
         <v>7622</v>
       </c>
-      <c r="B379" s="41" t="s">
+      <c r="B379" s="43" t="s">
         <v>380</v>
       </c>
       <c r="C379">
@@ -5898,7 +5902,7 @@
       <c r="A380">
         <v>7623</v>
       </c>
-      <c r="B380" s="41" t="s">
+      <c r="B380" s="43" t="s">
         <v>381</v>
       </c>
       <c r="C380">
@@ -5909,7 +5913,7 @@
       <c r="A381">
         <v>7630</v>
       </c>
-      <c r="B381" s="41" t="s">
+      <c r="B381" s="43" t="s">
         <v>382</v>
       </c>
       <c r="C381">
@@ -5920,7 +5924,7 @@
       <c r="A382">
         <v>7631</v>
       </c>
-      <c r="B382" s="41" t="s">
+      <c r="B382" s="43" t="s">
         <v>383</v>
       </c>
       <c r="C382">
@@ -5931,7 +5935,7 @@
       <c r="A383">
         <v>7632</v>
       </c>
-      <c r="B383" s="41" t="s">
+      <c r="B383" s="43" t="s">
         <v>384</v>
       </c>
       <c r="C383">
@@ -5942,7 +5946,7 @@
       <c r="A384">
         <v>7633</v>
       </c>
-      <c r="B384" s="41" t="s">
+      <c r="B384" s="43" t="s">
         <v>385</v>
       </c>
       <c r="C384">
@@ -5953,7 +5957,7 @@
       <c r="A385">
         <v>7640</v>
       </c>
-      <c r="B385" s="41" t="s">
+      <c r="B385" s="43" t="s">
         <v>386</v>
       </c>
       <c r="C385">
@@ -5964,7 +5968,7 @@
       <c r="A386">
         <v>7641</v>
       </c>
-      <c r="B386" s="41" t="s">
+      <c r="B386" s="43" t="s">
         <v>387</v>
       </c>
       <c r="C386">
@@ -5975,7 +5979,7 @@
       <c r="A387">
         <v>7642</v>
       </c>
-      <c r="B387" s="41" t="s">
+      <c r="B387" s="43" t="s">
         <v>388</v>
       </c>
       <c r="C387">
@@ -5986,7 +5990,7 @@
       <c r="A388">
         <v>7643</v>
       </c>
-      <c r="B388" s="41" t="s">
+      <c r="B388" s="43" t="s">
         <v>389</v>
       </c>
       <c r="C388">
@@ -5997,7 +6001,7 @@
       <c r="A389">
         <v>7650</v>
       </c>
-      <c r="B389" s="41" t="s">
+      <c r="B389" s="43" t="s">
         <v>390</v>
       </c>
       <c r="C389">
@@ -6008,7 +6012,7 @@
       <c r="A390">
         <v>7651</v>
       </c>
-      <c r="B390" s="41" t="s">
+      <c r="B390" s="43" t="s">
         <v>391</v>
       </c>
       <c r="C390">
@@ -6019,7 +6023,7 @@
       <c r="A391">
         <v>7652</v>
       </c>
-      <c r="B391" s="41" t="s">
+      <c r="B391" s="43" t="s">
         <v>392</v>
       </c>
       <c r="C391">
@@ -6030,7 +6034,7 @@
       <c r="A392">
         <v>7653</v>
       </c>
-      <c r="B392" s="41" t="s">
+      <c r="B392" s="43" t="s">
         <v>393</v>
       </c>
       <c r="C392">
@@ -6041,7 +6045,7 @@
       <c r="A393">
         <v>7654</v>
       </c>
-      <c r="B393" s="41" t="s">
+      <c r="B393" s="43" t="s">
         <v>394</v>
       </c>
       <c r="C393">
@@ -6052,7 +6056,7 @@
       <c r="A394">
         <v>7660</v>
       </c>
-      <c r="B394" s="41" t="s">
+      <c r="B394" s="43" t="s">
         <v>395</v>
       </c>
       <c r="C394">
@@ -6063,7 +6067,7 @@
       <c r="A395">
         <v>7661</v>
       </c>
-      <c r="B395" s="41" t="s">
+      <c r="B395" s="43" t="s">
         <v>396</v>
       </c>
       <c r="C395">
@@ -6074,7 +6078,7 @@
       <c r="A396">
         <v>7662</v>
       </c>
-      <c r="B396" s="41" t="s">
+      <c r="B396" s="43" t="s">
         <v>397</v>
       </c>
       <c r="C396">
@@ -6085,7 +6089,7 @@
       <c r="A397">
         <v>7663</v>
       </c>
-      <c r="B397" s="41" t="s">
+      <c r="B397" s="43" t="s">
         <v>398</v>
       </c>
       <c r="C397">
@@ -6096,7 +6100,7 @@
       <c r="A398">
         <v>7664</v>
       </c>
-      <c r="B398" s="41" t="s">
+      <c r="B398" s="43" t="s">
         <v>399</v>
       </c>
       <c r="C398">
@@ -6107,7 +6111,7 @@
       <c r="A399">
         <v>7681</v>
       </c>
-      <c r="B399" s="41" t="s">
+      <c r="B399" s="43" t="s">
         <v>400</v>
       </c>
       <c r="C399">
@@ -6118,7 +6122,7 @@
       <c r="A400">
         <v>7682</v>
       </c>
-      <c r="B400" s="41" t="s">
+      <c r="B400" s="43" t="s">
         <v>401</v>
       </c>
       <c r="C400">
@@ -6129,7 +6133,7 @@
       <c r="A401">
         <v>7683</v>
       </c>
-      <c r="B401" s="41" t="s">
+      <c r="B401" s="43" t="s">
         <v>402</v>
       </c>
       <c r="C401">
@@ -6140,7 +6144,7 @@
       <c r="A402">
         <v>7686</v>
       </c>
-      <c r="B402" s="41" t="s">
+      <c r="B402" s="43" t="s">
         <v>403</v>
       </c>
       <c r="C402">
@@ -6151,7 +6155,7 @@
       <c r="A403">
         <v>7687</v>
       </c>
-      <c r="B403" s="41" t="s">
+      <c r="B403" s="43" t="s">
         <v>404</v>
       </c>
       <c r="C403">
@@ -6162,7 +6166,7 @@
       <c r="A404">
         <v>7701</v>
       </c>
-      <c r="B404" s="41" t="s">
+      <c r="B404" s="43" t="s">
         <v>405</v>
       </c>
       <c r="C404">
@@ -6173,7 +6177,7 @@
       <c r="A405">
         <v>7711</v>
       </c>
-      <c r="B405" s="41" t="s">
+      <c r="B405" s="43" t="s">
         <v>406</v>
       </c>
       <c r="C405">
@@ -6184,7 +6188,7 @@
       <c r="A406">
         <v>7721</v>
       </c>
-      <c r="B406" s="41" t="s">
+      <c r="B406" s="43" t="s">
         <v>407</v>
       </c>
       <c r="C406">
@@ -6195,7 +6199,7 @@
       <c r="A407">
         <v>7731</v>
       </c>
-      <c r="B407" s="41" t="s">
+      <c r="B407" s="43" t="s">
         <v>408</v>
       </c>
       <c r="C407">
@@ -6206,7 +6210,7 @@
       <c r="A408">
         <v>7732</v>
       </c>
-      <c r="B408" s="41" t="s">
+      <c r="B408" s="43" t="s">
         <v>409</v>
       </c>
       <c r="C408">
@@ -6217,7 +6221,7 @@
       <c r="A409">
         <v>7733</v>
       </c>
-      <c r="B409" s="41" t="s">
+      <c r="B409" s="43" t="s">
         <v>410</v>
       </c>
       <c r="C409">
@@ -6228,7 +6232,7 @@
       <c r="A410">
         <v>7734</v>
       </c>
-      <c r="B410" s="41" t="s">
+      <c r="B410" s="43" t="s">
         <v>411</v>
       </c>
       <c r="C410">
@@ -6239,7 +6243,7 @@
       <c r="A411">
         <v>7735</v>
       </c>
-      <c r="B411" s="41" t="s">
+      <c r="B411" s="43" t="s">
         <v>412</v>
       </c>
       <c r="C411">
@@ -6250,7 +6254,7 @@
       <c r="A412">
         <v>7741</v>
       </c>
-      <c r="B412" s="41" t="s">
+      <c r="B412" s="43" t="s">
         <v>413</v>
       </c>
       <c r="C412">
@@ -6261,7 +6265,7 @@
       <c r="A413">
         <v>7751</v>
       </c>
-      <c r="B413" s="41" t="s">
+      <c r="B413" s="43" t="s">
         <v>414</v>
       </c>
       <c r="C413">
@@ -6272,7 +6276,7 @@
       <c r="A414">
         <v>7764</v>
       </c>
-      <c r="B414" s="41" t="s">
+      <c r="B414" s="43" t="s">
         <v>415</v>
       </c>
       <c r="C414">
@@ -6283,7 +6287,7 @@
       <c r="A415">
         <v>7771</v>
       </c>
-      <c r="B415" s="41" t="s">
+      <c r="B415" s="43" t="s">
         <v>416</v>
       </c>
       <c r="C415">
@@ -6294,7 +6298,7 @@
       <c r="A416">
         <v>7772</v>
       </c>
-      <c r="B416" s="41" t="s">
+      <c r="B416" s="43" t="s">
         <v>417</v>
       </c>
       <c r="C416">
@@ -6305,7 +6309,7 @@
       <c r="A417">
         <v>7801</v>
       </c>
-      <c r="B417" s="41" t="s">
+      <c r="B417" s="43" t="s">
         <v>418</v>
       </c>
       <c r="C417">
@@ -6316,7 +6320,7 @@
       <c r="A418">
         <v>7811</v>
       </c>
-      <c r="B418" s="41" t="s">
+      <c r="B418" s="43" t="s">
         <v>419</v>
       </c>
       <c r="C418">
@@ -6327,7 +6331,7 @@
       <c r="A419">
         <v>7813</v>
       </c>
-      <c r="B419" s="41" t="s">
+      <c r="B419" s="43" t="s">
         <v>420</v>
       </c>
       <c r="C419">
@@ -6338,7 +6342,7 @@
       <c r="A420">
         <v>7817</v>
       </c>
-      <c r="B420" s="41" t="s">
+      <c r="B420" s="43" t="s">
         <v>421</v>
       </c>
       <c r="C420">
@@ -6349,7 +6353,7 @@
       <c r="A421">
         <v>7820</v>
       </c>
-      <c r="B421" s="41" t="s">
+      <c r="B421" s="43" t="s">
         <v>422</v>
       </c>
       <c r="C421">
@@ -6360,7 +6364,7 @@
       <c r="A422">
         <v>7821</v>
       </c>
-      <c r="B422" s="41" t="s">
+      <c r="B422" s="43" t="s">
         <v>423</v>
       </c>
       <c r="C422">
@@ -6371,7 +6375,7 @@
       <c r="A423">
         <v>7822</v>
       </c>
-      <c r="B423" s="41" t="s">
+      <c r="B423" s="43" t="s">
         <v>424</v>
       </c>
       <c r="C423">
@@ -6382,7 +6386,7 @@
       <c r="A424">
         <v>7823</v>
       </c>
-      <c r="B424" s="41" t="s">
+      <c r="B424" s="43" t="s">
         <v>425</v>
       </c>
       <c r="C424">
@@ -6393,7 +6397,7 @@
       <c r="A425">
         <v>7824</v>
       </c>
-      <c r="B425" s="41" t="s">
+      <c r="B425" s="43" t="s">
         <v>426</v>
       </c>
       <c r="C425">
@@ -6404,7 +6408,7 @@
       <c r="A426">
         <v>7825</v>
       </c>
-      <c r="B426" s="41" t="s">
+      <c r="B426" s="43" t="s">
         <v>427</v>
       </c>
       <c r="C426">
@@ -6415,7 +6419,7 @@
       <c r="A427">
         <v>7826</v>
       </c>
-      <c r="B427" s="41" t="s">
+      <c r="B427" s="43" t="s">
         <v>428</v>
       </c>
       <c r="C427">
@@ -6426,7 +6430,7 @@
       <c r="A428">
         <v>7827</v>
       </c>
-      <c r="B428" s="41" t="s">
+      <c r="B428" s="43" t="s">
         <v>429</v>
       </c>
       <c r="C428">
@@ -6437,7 +6441,7 @@
       <c r="A429">
         <v>7828</v>
       </c>
-      <c r="B429" s="41" t="s">
+      <c r="B429" s="43" t="s">
         <v>430</v>
       </c>
       <c r="C429">
@@ -6448,7 +6452,7 @@
       <c r="A430">
         <v>7831</v>
       </c>
-      <c r="B430" s="41" t="s">
+      <c r="B430" s="43" t="s">
         <v>431</v>
       </c>
       <c r="C430">
@@ -6459,7 +6463,7 @@
       <c r="A431">
         <v>7832</v>
       </c>
-      <c r="B431" s="41" t="s">
+      <c r="B431" s="43" t="s">
         <v>432</v>
       </c>
       <c r="C431">
@@ -6470,7 +6474,7 @@
       <c r="A432">
         <v>7841</v>
       </c>
-      <c r="B432" s="41" t="s">
+      <c r="B432" s="43" t="s">
         <v>433</v>
       </c>
       <c r="C432">
@@ -6481,7 +6485,7 @@
       <c r="A433">
         <v>7842</v>
       </c>
-      <c r="B433" s="41" t="s">
+      <c r="B433" s="43" t="s">
         <v>434</v>
       </c>
       <c r="C433">
@@ -6492,7 +6496,7 @@
       <c r="A434">
         <v>-1</v>
       </c>
-      <c r="B434" s="41" t="s">
+      <c r="B434" s="43" t="s">
         <v>300</v>
       </c>
       <c r="C434">
@@ -6503,7 +6507,7 @@
       <c r="A435">
         <v>8101</v>
       </c>
-      <c r="B435" s="41" t="s">
+      <c r="B435" s="43" t="s">
         <v>435</v>
       </c>
       <c r="C435">
@@ -6514,7 +6518,7 @@
       <c r="A436">
         <v>8102</v>
       </c>
-      <c r="B436" s="41" t="s">
+      <c r="B436" s="43" t="s">
         <v>436</v>
       </c>
       <c r="C436">
@@ -6525,7 +6529,7 @@
       <c r="A437">
         <v>8103</v>
       </c>
-      <c r="B437" s="41" t="s">
+      <c r="B437" s="43" t="s">
         <v>437</v>
       </c>
       <c r="C437">
@@ -6536,7 +6540,7 @@
       <c r="A438">
         <v>8110</v>
       </c>
-      <c r="B438" s="41" t="s">
+      <c r="B438" s="43" t="s">
         <v>438</v>
       </c>
       <c r="C438">
@@ -6547,7 +6551,7 @@
       <c r="A439">
         <v>8111</v>
       </c>
-      <c r="B439" s="41" t="s">
+      <c r="B439" s="43" t="s">
         <v>439</v>
       </c>
       <c r="C439">
@@ -6558,7 +6562,7 @@
       <c r="A440">
         <v>8112</v>
       </c>
-      <c r="B440" s="41" t="s">
+      <c r="B440" s="43" t="s">
         <v>440</v>
       </c>
       <c r="C440">
@@ -6569,7 +6573,7 @@
       <c r="A441">
         <v>8113</v>
       </c>
-      <c r="B441" s="41" t="s">
+      <c r="B441" s="43" t="s">
         <v>441</v>
       </c>
       <c r="C441">
@@ -6580,7 +6584,7 @@
       <c r="A442">
         <v>8114</v>
       </c>
-      <c r="B442" s="41" t="s">
+      <c r="B442" s="43" t="s">
         <v>442</v>
       </c>
       <c r="C442">
@@ -6591,7 +6595,7 @@
       <c r="A443">
         <v>8115</v>
       </c>
-      <c r="B443" s="41" t="s">
+      <c r="B443" s="43" t="s">
         <v>443</v>
       </c>
       <c r="C443">
@@ -6602,7 +6606,7 @@
       <c r="A444">
         <v>8116</v>
       </c>
-      <c r="B444" s="41" t="s">
+      <c r="B444" s="43" t="s">
         <v>444</v>
       </c>
       <c r="C444">
@@ -6613,7 +6617,7 @@
       <c r="A445">
         <v>8117</v>
       </c>
-      <c r="B445" s="41" t="s">
+      <c r="B445" s="43" t="s">
         <v>445</v>
       </c>
       <c r="C445">
@@ -6624,7 +6628,7 @@
       <c r="A446">
         <v>8118</v>
       </c>
-      <c r="B446" s="41" t="s">
+      <c r="B446" s="43" t="s">
         <v>446</v>
       </c>
       <c r="C446">
@@ -6635,7 +6639,7 @@
       <c r="A447">
         <v>8121</v>
       </c>
-      <c r="B447" s="41" t="s">
+      <c r="B447" s="43" t="s">
         <v>447</v>
       </c>
       <c r="C447">
@@ -6646,7 +6650,7 @@
       <c r="A448">
         <v>8131</v>
       </c>
-      <c r="B448" s="41" t="s">
+      <c r="B448" s="43" t="s">
         <v>448</v>
       </c>
       <c r="C448">
@@ -6657,7 +6661,7 @@
       <c r="A449">
         <v>8181</v>
       </c>
-      <c r="B449" s="41" t="s">
+      <c r="B449" s="43" t="s">
         <v>449</v>
       </c>
       <c r="C449">
@@ -6668,7 +6672,7 @@
       <c r="A450">
         <v>8201</v>
       </c>
-      <c r="B450" s="41" t="s">
+      <c r="B450" s="43" t="s">
         <v>450</v>
       </c>
       <c r="C450">
@@ -6679,7 +6683,7 @@
       <c r="A451">
         <v>8202</v>
       </c>
-      <c r="B451" s="41" t="s">
+      <c r="B451" s="43" t="s">
         <v>451</v>
       </c>
       <c r="C451">
@@ -6690,7 +6694,7 @@
       <c r="A452">
         <v>8211</v>
       </c>
-      <c r="B452" s="41" t="s">
+      <c r="B452" s="43" t="s">
         <v>452</v>
       </c>
       <c r="C452">
@@ -6701,7 +6705,7 @@
       <c r="A453">
         <v>8212</v>
       </c>
-      <c r="B453" s="41" t="s">
+      <c r="B453" s="43" t="s">
         <v>453</v>
       </c>
       <c r="C453">
@@ -6712,7 +6716,7 @@
       <c r="A454">
         <v>8213</v>
       </c>
-      <c r="B454" s="41" t="s">
+      <c r="B454" s="43" t="s">
         <v>454</v>
       </c>
       <c r="C454">
@@ -6723,7 +6727,7 @@
       <c r="A455">
         <v>8214</v>
       </c>
-      <c r="B455" s="41" t="s">
+      <c r="B455" s="43" t="s">
         <v>455</v>
       </c>
       <c r="C455">
@@ -6734,7 +6738,7 @@
       <c r="A456">
         <v>8221</v>
       </c>
-      <c r="B456" s="41" t="s">
+      <c r="B456" s="43" t="s">
         <v>456</v>
       </c>
       <c r="C456">
@@ -6745,7 +6749,7 @@
       <c r="A457">
         <v>8231</v>
       </c>
-      <c r="B457" s="41" t="s">
+      <c r="B457" s="43" t="s">
         <v>457</v>
       </c>
       <c r="C457">
@@ -6756,7 +6760,7 @@
       <c r="A458">
         <v>8232</v>
       </c>
-      <c r="B458" s="41" t="s">
+      <c r="B458" s="43" t="s">
         <v>458</v>
       </c>
       <c r="C458">
@@ -6767,7 +6771,7 @@
       <c r="A459">
         <v>8233</v>
       </c>
-      <c r="B459" s="41" t="s">
+      <c r="B459" s="43" t="s">
         <v>459</v>
       </c>
       <c r="C459">
@@ -6778,7 +6782,7 @@
       <c r="A460">
         <v>8281</v>
       </c>
-      <c r="B460" s="41" t="s">
+      <c r="B460" s="43" t="s">
         <v>460</v>
       </c>
       <c r="C460">
@@ -6789,7 +6793,7 @@
       <c r="A461">
         <v>8301</v>
       </c>
-      <c r="B461" s="41" t="s">
+      <c r="B461" s="43" t="s">
         <v>461</v>
       </c>
       <c r="C461">
@@ -6800,7 +6804,7 @@
       <c r="A462">
         <v>8311</v>
       </c>
-      <c r="B462" s="41" t="s">
+      <c r="B462" s="43" t="s">
         <v>462</v>
       </c>
       <c r="C462">
@@ -6811,7 +6815,7 @@
       <c r="A463">
         <v>8321</v>
       </c>
-      <c r="B463" s="41" t="s">
+      <c r="B463" s="43" t="s">
         <v>463</v>
       </c>
       <c r="C463">
@@ -6822,7 +6826,7 @@
       <c r="A464">
         <v>8339</v>
       </c>
-      <c r="B464" s="41" t="s">
+      <c r="B464" s="43" t="s">
         <v>464</v>
       </c>
       <c r="C464">
@@ -6833,7 +6837,7 @@
       <c r="A465">
         <v>8401</v>
       </c>
-      <c r="B465" s="41" t="s">
+      <c r="B465" s="43" t="s">
         <v>465</v>
       </c>
       <c r="C465">
@@ -6844,7 +6848,7 @@
       <c r="A466">
         <v>8411</v>
       </c>
-      <c r="B466" s="41" t="s">
+      <c r="B466" s="43" t="s">
         <v>466</v>
       </c>
       <c r="C466">
@@ -6855,7 +6859,7 @@
       <c r="A467">
         <v>8412</v>
       </c>
-      <c r="B467" s="41" t="s">
+      <c r="B467" s="43" t="s">
         <v>467</v>
       </c>
       <c r="C467">
@@ -6866,7 +6870,7 @@
       <c r="A468">
         <v>8413</v>
       </c>
-      <c r="B468" s="41" t="s">
+      <c r="B468" s="43" t="s">
         <v>468</v>
       </c>
       <c r="C468">
@@ -6877,7 +6881,7 @@
       <c r="A469">
         <v>8416</v>
       </c>
-      <c r="B469" s="41" t="s">
+      <c r="B469" s="43" t="s">
         <v>469</v>
       </c>
       <c r="C469">
@@ -6888,7 +6892,7 @@
       <c r="A470">
         <v>8417</v>
       </c>
-      <c r="B470" s="41" t="s">
+      <c r="B470" s="43" t="s">
         <v>470</v>
       </c>
       <c r="C470">
@@ -6899,7 +6903,7 @@
       <c r="A471">
         <v>8421</v>
       </c>
-      <c r="B471" s="41" t="s">
+      <c r="B471" s="43" t="s">
         <v>471</v>
       </c>
       <c r="C471">
@@ -6910,7 +6914,7 @@
       <c r="A472">
         <v>8423</v>
       </c>
-      <c r="B472" s="41" t="s">
+      <c r="B472" s="43" t="s">
         <v>472</v>
       </c>
       <c r="C472">
@@ -6921,7 +6925,7 @@
       <c r="A473">
         <v>8429</v>
       </c>
-      <c r="B473" s="41" t="s">
+      <c r="B473" s="43" t="s">
         <v>473</v>
       </c>
       <c r="C473">
@@ -6932,7 +6936,7 @@
       <c r="A474">
         <v>8484</v>
       </c>
-      <c r="B474" s="41" t="s">
+      <c r="B474" s="43" t="s">
         <v>474</v>
       </c>
       <c r="C474">
@@ -6943,7 +6947,7 @@
       <c r="A475">
         <v>8485</v>
       </c>
-      <c r="B475" s="41" t="s">
+      <c r="B475" s="43" t="s">
         <v>475</v>
       </c>
       <c r="C475">
@@ -6954,7 +6958,7 @@
       <c r="A476">
         <v>8491</v>
       </c>
-      <c r="B476" s="41" t="s">
+      <c r="B476" s="43" t="s">
         <v>476</v>
       </c>
       <c r="C476">
@@ -6965,7 +6969,7 @@
       <c r="A477">
         <v>8492</v>
       </c>
-      <c r="B477" s="41" t="s">
+      <c r="B477" s="43" t="s">
         <v>477</v>
       </c>
       <c r="C477">
@@ -6976,7 +6980,7 @@
       <c r="A478">
         <v>8493</v>
       </c>
-      <c r="B478" s="41" t="s">
+      <c r="B478" s="43" t="s">
         <v>478</v>
       </c>
       <c r="C478">
@@ -6987,7 +6991,7 @@
       <c r="A479">
         <v>8601</v>
       </c>
-      <c r="B479" s="41" t="s">
+      <c r="B479" s="43" t="s">
         <v>479</v>
       </c>
       <c r="C479">
@@ -6998,7 +7002,7 @@
       <c r="A480">
         <v>8611</v>
       </c>
-      <c r="B480" s="41" t="s">
+      <c r="B480" s="43" t="s">
         <v>480</v>
       </c>
       <c r="C480">
@@ -7009,7 +7013,7 @@
       <c r="A481">
         <v>8612</v>
       </c>
-      <c r="B481" s="41" t="s">
+      <c r="B481" s="43" t="s">
         <v>481</v>
       </c>
       <c r="C481">
@@ -7020,7 +7024,7 @@
       <c r="A482">
         <v>8621</v>
       </c>
-      <c r="B482" s="41" t="s">
+      <c r="B482" s="43" t="s">
         <v>482</v>
       </c>
       <c r="C482">
@@ -7031,7 +7035,7 @@
       <c r="A483">
         <v>8622</v>
       </c>
-      <c r="B483" s="41" t="s">
+      <c r="B483" s="43" t="s">
         <v>483</v>
       </c>
       <c r="C483">
@@ -7042,7 +7046,7 @@
       <c r="A484">
         <v>8623</v>
       </c>
-      <c r="B484" s="41" t="s">
+      <c r="B484" s="43" t="s">
         <v>484</v>
       </c>
       <c r="C484">
@@ -7053,7 +7057,7 @@
       <c r="A485">
         <v>8624</v>
       </c>
-      <c r="B485" s="41" t="s">
+      <c r="B485" s="43" t="s">
         <v>485</v>
       </c>
       <c r="C485">
@@ -7064,7 +7068,7 @@
       <c r="A486">
         <v>8625</v>
       </c>
-      <c r="B486" s="41" t="s">
+      <c r="B486" s="43" t="s">
         <v>486</v>
       </c>
       <c r="C486">
@@ -7075,7 +7079,7 @@
       <c r="A487">
         <v>8711</v>
       </c>
-      <c r="B487" s="41" t="s">
+      <c r="B487" s="43" t="s">
         <v>487</v>
       </c>
       <c r="C487">
@@ -7086,7 +7090,7 @@
       <c r="A488">
         <v>-1</v>
       </c>
-      <c r="B488" s="41" t="s">
+      <c r="B488" s="43" t="s">
         <v>488</v>
       </c>
       <c r="C488">
@@ -7097,7 +7101,7 @@
       <c r="A489">
         <v>9101</v>
       </c>
-      <c r="B489" s="41" t="s">
+      <c r="B489" s="43" t="s">
         <v>489</v>
       </c>
       <c r="C489">
@@ -7108,7 +7112,7 @@
       <c r="A490">
         <v>9102</v>
       </c>
-      <c r="B490" s="41" t="s">
+      <c r="B490" s="43" t="s">
         <v>490</v>
       </c>
       <c r="C490">
@@ -7119,7 +7123,7 @@
       <c r="A491">
         <v>9109</v>
       </c>
-      <c r="B491" s="41" t="s">
+      <c r="B491" s="43" t="s">
         <v>491</v>
       </c>
       <c r="C491">
@@ -7130,7 +7134,7 @@
       <c r="A492">
         <v>9111</v>
       </c>
-      <c r="B492" s="41" t="s">
+      <c r="B492" s="43" t="s">
         <v>492</v>
       </c>
       <c r="C492">
@@ -7141,7 +7145,7 @@
       <c r="A493">
         <v>9112</v>
       </c>
-      <c r="B493" s="41" t="s">
+      <c r="B493" s="43" t="s">
         <v>493</v>
       </c>
       <c r="C493">
@@ -7152,7 +7156,7 @@
       <c r="A494">
         <v>9113</v>
       </c>
-      <c r="B494" s="41" t="s">
+      <c r="B494" s="43" t="s">
         <v>494</v>
       </c>
       <c r="C494">
@@ -7163,7 +7167,7 @@
       <c r="A495">
         <v>9131</v>
       </c>
-      <c r="B495" s="41" t="s">
+      <c r="B495" s="43" t="s">
         <v>495</v>
       </c>
       <c r="C495">
@@ -7174,7 +7178,7 @@
       <c r="A496">
         <v>9141</v>
       </c>
-      <c r="B496" s="41" t="s">
+      <c r="B496" s="43" t="s">
         <v>496</v>
       </c>
       <c r="C496">
@@ -7185,7 +7189,7 @@
       <c r="A497">
         <v>9142</v>
       </c>
-      <c r="B497" s="41" t="s">
+      <c r="B497" s="43" t="s">
         <v>497</v>
       </c>
       <c r="C497">
@@ -7196,7 +7200,7 @@
       <c r="A498">
         <v>9143</v>
       </c>
-      <c r="B498" s="41" t="s">
+      <c r="B498" s="43" t="s">
         <v>498</v>
       </c>
       <c r="C498">
@@ -7207,7 +7211,7 @@
       <c r="A499">
         <v>9144</v>
       </c>
-      <c r="B499" s="41" t="s">
+      <c r="B499" s="43" t="s">
         <v>499</v>
       </c>
       <c r="C499">
@@ -7218,7 +7222,7 @@
       <c r="A500">
         <v>9151</v>
       </c>
-      <c r="B500" s="41" t="s">
+      <c r="B500" s="43" t="s">
         <v>500</v>
       </c>
       <c r="C500">
@@ -7229,7 +7233,7 @@
       <c r="A501">
         <v>9152</v>
       </c>
-      <c r="B501" s="41" t="s">
+      <c r="B501" s="43" t="s">
         <v>501</v>
       </c>
       <c r="C501">
@@ -7240,7 +7244,7 @@
       <c r="A502">
         <v>9153</v>
       </c>
-      <c r="B502" s="41" t="s">
+      <c r="B502" s="43" t="s">
         <v>502</v>
       </c>
       <c r="C502">
@@ -7251,7 +7255,7 @@
       <c r="A503">
         <v>9154</v>
       </c>
-      <c r="B503" s="41" t="s">
+      <c r="B503" s="43" t="s">
         <v>503</v>
       </c>
       <c r="C503">
@@ -7262,7 +7266,7 @@
       <c r="A504">
         <v>9191</v>
       </c>
-      <c r="B504" s="41" t="s">
+      <c r="B504" s="43" t="s">
         <v>504</v>
       </c>
       <c r="C504">
@@ -7273,7 +7277,7 @@
       <c r="A505">
         <v>9192</v>
       </c>
-      <c r="B505" s="41" t="s">
+      <c r="B505" s="43" t="s">
         <v>505</v>
       </c>
       <c r="C505">
@@ -7284,7 +7288,7 @@
       <c r="A506">
         <v>9193</v>
       </c>
-      <c r="B506" s="41" t="s">
+      <c r="B506" s="43" t="s">
         <v>506</v>
       </c>
       <c r="C506">
@@ -7295,7 +7299,7 @@
       <c r="A507">
         <v>9501</v>
       </c>
-      <c r="B507" s="41" t="s">
+      <c r="B507" s="43" t="s">
         <v>507</v>
       </c>
       <c r="C507">
@@ -7306,7 +7310,7 @@
       <c r="A508">
         <v>9502</v>
       </c>
-      <c r="B508" s="41" t="s">
+      <c r="B508" s="43" t="s">
         <v>508</v>
       </c>
       <c r="C508">
@@ -7317,7 +7321,7 @@
       <c r="A509">
         <v>9503</v>
       </c>
-      <c r="B509" s="41" t="s">
+      <c r="B509" s="43" t="s">
         <v>509</v>
       </c>
       <c r="C509">
@@ -7328,7 +7332,7 @@
       <c r="A510">
         <v>9511</v>
       </c>
-      <c r="B510" s="41" t="s">
+      <c r="B510" s="43" t="s">
         <v>510</v>
       </c>
       <c r="C510">
@@ -7339,7 +7343,7 @@
       <c r="A511">
         <v>9513</v>
       </c>
-      <c r="B511" s="41" t="s">
+      <c r="B511" s="43" t="s">
         <v>511</v>
       </c>
       <c r="C511">
@@ -7350,7 +7354,7 @@
       <c r="A512">
         <v>9531</v>
       </c>
-      <c r="B512" s="41" t="s">
+      <c r="B512" s="43" t="s">
         <v>512</v>
       </c>
       <c r="C512">
@@ -7361,7 +7365,7 @@
       <c r="A513">
         <v>9541</v>
       </c>
-      <c r="B513" s="41" t="s">
+      <c r="B513" s="43" t="s">
         <v>513</v>
       </c>
       <c r="C513">
@@ -7372,7 +7376,7 @@
       <c r="A514">
         <v>9542</v>
       </c>
-      <c r="B514" s="41" t="s">
+      <c r="B514" s="43" t="s">
         <v>514</v>
       </c>
       <c r="C514">
@@ -7383,7 +7387,7 @@
       <c r="A515">
         <v>9543</v>
       </c>
-      <c r="B515" s="41" t="s">
+      <c r="B515" s="43" t="s">
         <v>515</v>
       </c>
       <c r="C515">
@@ -7394,7 +7398,7 @@
       <c r="A516">
         <v>9911</v>
       </c>
-      <c r="B516" s="41" t="s">
+      <c r="B516" s="43" t="s">
         <v>516</v>
       </c>
       <c r="C516">
@@ -7405,7 +7409,7 @@
       <c r="A517">
         <v>9912</v>
       </c>
-      <c r="B517" s="41" t="s">
+      <c r="B517" s="43" t="s">
         <v>517</v>
       </c>
       <c r="C517">
@@ -7416,7 +7420,7 @@
       <c r="A518">
         <v>9913</v>
       </c>
-      <c r="B518" s="41" t="s">
+      <c r="B518" s="43" t="s">
         <v>518</v>
       </c>
       <c r="C518">
@@ -7427,7 +7431,7 @@
       <c r="A519">
         <v>9914</v>
       </c>
-      <c r="B519" s="41" t="s">
+      <c r="B519" s="43" t="s">
         <v>519</v>
       </c>
       <c r="C519">
@@ -7438,7 +7442,7 @@
       <c r="A520">
         <v>9921</v>
       </c>
-      <c r="B520" s="41" t="s">
+      <c r="B520" s="43" t="s">
         <v>520</v>
       </c>
       <c r="C520">
@@ -7449,7 +7453,7 @@
       <c r="A521">
         <v>9922</v>
       </c>
-      <c r="B521" s="41" t="s">
+      <c r="B521" s="43" t="s">
         <v>521</v>
       </c>
       <c r="C521">
@@ -7460,7 +7464,7 @@
       <c r="A522">
         <v>-1</v>
       </c>
-      <c r="B522" s="41" t="s">
+      <c r="B522" s="43" t="s">
         <v>522</v>
       </c>
       <c r="C522">
@@ -7471,7 +7475,7 @@
       <c r="A523">
         <v>9999</v>
       </c>
-      <c r="B523" s="41" t="s">
+      <c r="B523" s="43" t="s">
         <v>523</v>
       </c>
       <c r="C523">

</xml_diff>

<commit_message>
AEJ macro first resubmit
</commit_message>
<xml_diff>
--- a/+dataLH/test_files/readTest.xlsx
+++ b/+dataLH/test_files/readTest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12095" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16820" uniqueCount="525">
   <si>
     <t>Code</t>
   </si>
@@ -1610,7 +1610,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -1664,11 +1664,29 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1716,6 +1734,24 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1728,19 +1764,19 @@
   <dimension ref="A1:C584"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="true"/>
-    <col min="2" max="2" width="127.7109375" customWidth="true"/>
-    <col min="3" max="3" width="7.7109375" customWidth="true"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="2" width="111.140625" customWidth="true"/>
+    <col min="3" max="3" width="8.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="63" t="s">
         <v>524</v>
       </c>
     </row>
@@ -1748,7 +1784,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="63" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -1759,7 +1795,7 @@
       <c r="A3">
         <v>-1</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="63" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -1770,7 +1806,7 @@
       <c r="A4">
         <v>100</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="63" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -1781,7 +1817,7 @@
       <c r="A5">
         <v>200</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="63" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -1792,7 +1828,7 @@
       <c r="A6">
         <v>300</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="63" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -1803,7 +1839,7 @@
       <c r="A7">
         <v>401</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="63" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -1814,7 +1850,7 @@
       <c r="A8">
         <v>402</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="63" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -1825,7 +1861,7 @@
       <c r="A9">
         <v>403</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="63" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -1836,7 +1872,7 @@
       <c r="A10">
         <v>411</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="63" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -1847,7 +1883,7 @@
       <c r="A11">
         <v>412</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="63" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -1858,7 +1894,7 @@
       <c r="A12">
         <v>413</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="63" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -1869,7 +1905,7 @@
       <c r="A13">
         <v>501</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="63" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -1880,7 +1916,7 @@
       <c r="A14">
         <v>502</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="63" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -1891,7 +1927,7 @@
       <c r="A15">
         <v>503</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="63" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -1902,7 +1938,7 @@
       <c r="A16">
         <v>511</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="63" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1913,7 +1949,7 @@
       <c r="A17">
         <v>512</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="63" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -1924,7 +1960,7 @@
       <c r="A18">
         <v>513</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="63" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -1935,7 +1971,7 @@
       <c r="A19">
         <v>-1</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -1946,7 +1982,7 @@
       <c r="A20">
         <v>1111</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1957,7 +1993,7 @@
       <c r="A21">
         <v>1112</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="63" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -1968,7 +2004,7 @@
       <c r="A22">
         <v>1113</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="63" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1979,7 +2015,7 @@
       <c r="A23">
         <v>1122</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="63" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -1990,7 +2026,7 @@
       <c r="A24">
         <v>1123</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="63" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -2001,7 +2037,7 @@
       <c r="A25">
         <v>1130</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="63" t="s">
         <v>25</v>
       </c>
       <c r="C25">
@@ -2012,7 +2048,7 @@
       <c r="A26">
         <v>1140</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="63" t="s">
         <v>27</v>
       </c>
       <c r="C26">
@@ -2023,7 +2059,7 @@
       <c r="A27">
         <v>1210</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="63" t="s">
         <v>28</v>
       </c>
       <c r="C27">
@@ -2034,7 +2070,7 @@
       <c r="A28">
         <v>1219</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="63" t="s">
         <v>29</v>
       </c>
       <c r="C28">
@@ -2045,7 +2081,7 @@
       <c r="A29">
         <v>1220</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C29">
@@ -2056,7 +2092,7 @@
       <c r="A30">
         <v>1230</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="63" t="s">
         <v>31</v>
       </c>
       <c r="C30">
@@ -2067,7 +2103,7 @@
       <c r="A31">
         <v>1310</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="63" t="s">
         <v>32</v>
       </c>
       <c r="C31">
@@ -2078,7 +2114,7 @@
       <c r="A32">
         <v>1320</v>
       </c>
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="63" t="s">
         <v>33</v>
       </c>
       <c r="C32">
@@ -2089,7 +2125,7 @@
       <c r="A33">
         <v>-1</v>
       </c>
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="63" t="s">
         <v>34</v>
       </c>
       <c r="C33">
@@ -2100,7 +2136,7 @@
       <c r="A34">
         <v>2011</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="63" t="s">
         <v>35</v>
       </c>
       <c r="C34">
@@ -2111,7 +2147,7 @@
       <c r="A35">
         <v>2012</v>
       </c>
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="63" t="s">
         <v>36</v>
       </c>
       <c r="C35">
@@ -2122,7 +2158,7 @@
       <c r="A36">
         <v>2021</v>
       </c>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="63" t="s">
         <v>37</v>
       </c>
       <c r="C36">
@@ -2133,7 +2169,7 @@
       <c r="A37">
         <v>2111</v>
       </c>
-      <c r="B37" s="45" t="s">
+      <c r="B37" s="63" t="s">
         <v>38</v>
       </c>
       <c r="C37">
@@ -2144,7 +2180,7 @@
       <c r="A38">
         <v>2112</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="63" t="s">
         <v>39</v>
       </c>
       <c r="C38">
@@ -2155,7 +2191,7 @@
       <c r="A39">
         <v>2121</v>
       </c>
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C39">
@@ -2166,7 +2202,7 @@
       <c r="A40">
         <v>2122</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="63" t="s">
         <v>41</v>
       </c>
       <c r="C40">
@@ -2177,7 +2213,7 @@
       <c r="A41">
         <v>2123</v>
       </c>
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="63" t="s">
         <v>42</v>
       </c>
       <c r="C41">
@@ -2188,7 +2224,7 @@
       <c r="A42">
         <v>2124</v>
       </c>
-      <c r="B42" s="45" t="s">
+      <c r="B42" s="63" t="s">
         <v>43</v>
       </c>
       <c r="C42">
@@ -2199,7 +2235,7 @@
       <c r="A43">
         <v>2125</v>
       </c>
-      <c r="B43" s="45" t="s">
+      <c r="B43" s="63" t="s">
         <v>44</v>
       </c>
       <c r="C43">
@@ -2210,7 +2246,7 @@
       <c r="A44">
         <v>2131</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="63" t="s">
         <v>45</v>
       </c>
       <c r="C44">
@@ -2221,7 +2257,7 @@
       <c r="A45">
         <v>2132</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="63" t="s">
         <v>46</v>
       </c>
       <c r="C45">
@@ -2232,7 +2268,7 @@
       <c r="A46">
         <v>2133</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="63" t="s">
         <v>47</v>
       </c>
       <c r="C46">
@@ -2243,7 +2279,7 @@
       <c r="A47">
         <v>2134</v>
       </c>
-      <c r="B47" s="45" t="s">
+      <c r="B47" s="63" t="s">
         <v>48</v>
       </c>
       <c r="C47">
@@ -2254,7 +2290,7 @@
       <c r="A48">
         <v>2140</v>
       </c>
-      <c r="B48" s="45" t="s">
+      <c r="B48" s="63" t="s">
         <v>49</v>
       </c>
       <c r="C48">
@@ -2265,7 +2301,7 @@
       <c r="A49">
         <v>2141</v>
       </c>
-      <c r="B49" s="45" t="s">
+      <c r="B49" s="63" t="s">
         <v>50</v>
       </c>
       <c r="C49">
@@ -2276,7 +2312,7 @@
       <c r="A50">
         <v>2142</v>
       </c>
-      <c r="B50" s="45" t="s">
+      <c r="B50" s="63" t="s">
         <v>51</v>
       </c>
       <c r="C50">
@@ -2287,7 +2323,7 @@
       <c r="A51">
         <v>2143</v>
       </c>
-      <c r="B51" s="45" t="s">
+      <c r="B51" s="63" t="s">
         <v>52</v>
       </c>
       <c r="C51">
@@ -2298,7 +2334,7 @@
       <c r="A52">
         <v>2144</v>
       </c>
-      <c r="B52" s="45" t="s">
+      <c r="B52" s="63" t="s">
         <v>53</v>
       </c>
       <c r="C52">
@@ -2309,7 +2345,7 @@
       <c r="A53">
         <v>2145</v>
       </c>
-      <c r="B53" s="45" t="s">
+      <c r="B53" s="63" t="s">
         <v>54</v>
       </c>
       <c r="C53">
@@ -2320,7 +2356,7 @@
       <c r="A54">
         <v>2146</v>
       </c>
-      <c r="B54" s="45" t="s">
+      <c r="B54" s="63" t="s">
         <v>55</v>
       </c>
       <c r="C54">
@@ -2331,7 +2367,7 @@
       <c r="A55">
         <v>2147</v>
       </c>
-      <c r="B55" s="45" t="s">
+      <c r="B55" s="63" t="s">
         <v>56</v>
       </c>
       <c r="C55">
@@ -2342,7 +2378,7 @@
       <c r="A56">
         <v>2148</v>
       </c>
-      <c r="B56" s="45" t="s">
+      <c r="B56" s="63" t="s">
         <v>57</v>
       </c>
       <c r="C56">
@@ -2353,7 +2389,7 @@
       <c r="A57">
         <v>2149</v>
       </c>
-      <c r="B57" s="45" t="s">
+      <c r="B57" s="63" t="s">
         <v>58</v>
       </c>
       <c r="C57">
@@ -2364,7 +2400,7 @@
       <c r="A58">
         <v>2151</v>
       </c>
-      <c r="B58" s="45" t="s">
+      <c r="B58" s="63" t="s">
         <v>59</v>
       </c>
       <c r="C58">
@@ -2375,7 +2411,7 @@
       <c r="A59">
         <v>2152</v>
       </c>
-      <c r="B59" s="45" t="s">
+      <c r="B59" s="63" t="s">
         <v>60</v>
       </c>
       <c r="C59">
@@ -2386,7 +2422,7 @@
       <c r="A60">
         <v>2153</v>
       </c>
-      <c r="B60" s="45" t="s">
+      <c r="B60" s="63" t="s">
         <v>61</v>
       </c>
       <c r="C60">
@@ -2397,7 +2433,7 @@
       <c r="A61">
         <v>2211</v>
       </c>
-      <c r="B61" s="45" t="s">
+      <c r="B61" s="63" t="s">
         <v>62</v>
       </c>
       <c r="C61">
@@ -2408,7 +2444,7 @@
       <c r="A62">
         <v>2221</v>
       </c>
-      <c r="B62" s="45" t="s">
+      <c r="B62" s="63" t="s">
         <v>63</v>
       </c>
       <c r="C62">
@@ -2419,7 +2455,7 @@
       <c r="A63">
         <v>2231</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="63" t="s">
         <v>64</v>
       </c>
       <c r="C63">
@@ -2430,7 +2466,7 @@
       <c r="A64">
         <v>2232</v>
       </c>
-      <c r="B64" s="45" t="s">
+      <c r="B64" s="63" t="s">
         <v>65</v>
       </c>
       <c r="C64">
@@ -2441,7 +2477,7 @@
       <c r="A65">
         <v>2233</v>
       </c>
-      <c r="B65" s="45" t="s">
+      <c r="B65" s="63" t="s">
         <v>66</v>
       </c>
       <c r="C65">
@@ -2452,7 +2488,7 @@
       <c r="A66">
         <v>2234</v>
       </c>
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="63" t="s">
         <v>67</v>
       </c>
       <c r="C66">
@@ -2463,7 +2499,7 @@
       <c r="A67">
         <v>2235</v>
       </c>
-      <c r="B67" s="45" t="s">
+      <c r="B67" s="63" t="s">
         <v>68</v>
       </c>
       <c r="C67">
@@ -2474,7 +2510,7 @@
       <c r="A68">
         <v>2236</v>
       </c>
-      <c r="B68" s="45" t="s">
+      <c r="B68" s="63" t="s">
         <v>69</v>
       </c>
       <c r="C68">
@@ -2485,7 +2521,7 @@
       <c r="A69">
         <v>2237</v>
       </c>
-      <c r="B69" s="45" t="s">
+      <c r="B69" s="63" t="s">
         <v>70</v>
       </c>
       <c r="C69">
@@ -2496,7 +2532,7 @@
       <c r="A70">
         <v>2311</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="B70" s="63" t="s">
         <v>71</v>
       </c>
       <c r="C70">
@@ -2507,7 +2543,7 @@
       <c r="A71">
         <v>2312</v>
       </c>
-      <c r="B71" s="45" t="s">
+      <c r="B71" s="63" t="s">
         <v>72</v>
       </c>
       <c r="C71">
@@ -2518,7 +2554,7 @@
       <c r="A72">
         <v>2313</v>
       </c>
-      <c r="B72" s="45" t="s">
+      <c r="B72" s="63" t="s">
         <v>73</v>
       </c>
       <c r="C72">
@@ -2529,7 +2565,7 @@
       <c r="A73">
         <v>2321</v>
       </c>
-      <c r="B73" s="45" t="s">
+      <c r="B73" s="63" t="s">
         <v>74</v>
       </c>
       <c r="C73">
@@ -2540,7 +2576,7 @@
       <c r="A74">
         <v>2330</v>
       </c>
-      <c r="B74" s="45" t="s">
+      <c r="B74" s="63" t="s">
         <v>75</v>
       </c>
       <c r="C74">
@@ -2551,7 +2587,7 @@
       <c r="A75">
         <v>2340</v>
       </c>
-      <c r="B75" s="45" t="s">
+      <c r="B75" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C75">
@@ -2562,7 +2598,7 @@
       <c r="A76">
         <v>2391</v>
       </c>
-      <c r="B76" s="45" t="s">
+      <c r="B76" s="63" t="s">
         <v>77</v>
       </c>
       <c r="C76">
@@ -2573,7 +2609,7 @@
       <c r="A77">
         <v>2392</v>
       </c>
-      <c r="B77" s="45" t="s">
+      <c r="B77" s="63" t="s">
         <v>78</v>
       </c>
       <c r="C77">
@@ -2584,7 +2620,7 @@
       <c r="A78">
         <v>2394</v>
       </c>
-      <c r="B78" s="45" t="s">
+      <c r="B78" s="63" t="s">
         <v>79</v>
       </c>
       <c r="C78">
@@ -2595,7 +2631,7 @@
       <c r="A79">
         <v>2410</v>
       </c>
-      <c r="B79" s="45" t="s">
+      <c r="B79" s="63" t="s">
         <v>80</v>
       </c>
       <c r="C79">
@@ -2606,7 +2642,7 @@
       <c r="A80">
         <v>2412</v>
       </c>
-      <c r="B80" s="45" t="s">
+      <c r="B80" s="63" t="s">
         <v>81</v>
       </c>
       <c r="C80">
@@ -2617,7 +2653,7 @@
       <c r="A81">
         <v>2419</v>
       </c>
-      <c r="B81" s="45" t="s">
+      <c r="B81" s="63" t="s">
         <v>82</v>
       </c>
       <c r="C81">
@@ -2628,7 +2664,7 @@
       <c r="A82">
         <v>2421</v>
       </c>
-      <c r="B82" s="45" t="s">
+      <c r="B82" s="63" t="s">
         <v>83</v>
       </c>
       <c r="C82">
@@ -2639,7 +2675,7 @@
       <c r="A83">
         <v>2422</v>
       </c>
-      <c r="B83" s="45" t="s">
+      <c r="B83" s="63" t="s">
         <v>84</v>
       </c>
       <c r="C83">
@@ -2650,7 +2686,7 @@
       <c r="A84">
         <v>2423</v>
       </c>
-      <c r="B84" s="45" t="s">
+      <c r="B84" s="63" t="s">
         <v>85</v>
       </c>
       <c r="C84">
@@ -2661,7 +2697,7 @@
       <c r="A85">
         <v>2511</v>
       </c>
-      <c r="B85" s="45" t="s">
+      <c r="B85" s="63" t="s">
         <v>86</v>
       </c>
       <c r="C85">
@@ -2672,7 +2708,7 @@
       <c r="A86">
         <v>2512</v>
       </c>
-      <c r="B86" s="45" t="s">
+      <c r="B86" s="63" t="s">
         <v>87</v>
       </c>
       <c r="C86">
@@ -2683,7 +2719,7 @@
       <c r="A87">
         <v>2513</v>
       </c>
-      <c r="B87" s="45" t="s">
+      <c r="B87" s="63" t="s">
         <v>88</v>
       </c>
       <c r="C87">
@@ -2694,7 +2730,7 @@
       <c r="A88">
         <v>2514</v>
       </c>
-      <c r="B88" s="45" t="s">
+      <c r="B88" s="63" t="s">
         <v>89</v>
       </c>
       <c r="C88">
@@ -2705,7 +2741,7 @@
       <c r="A89">
         <v>2515</v>
       </c>
-      <c r="B89" s="45" t="s">
+      <c r="B89" s="63" t="s">
         <v>90</v>
       </c>
       <c r="C89">
@@ -2716,7 +2752,7 @@
       <c r="A90">
         <v>2516</v>
       </c>
-      <c r="B90" s="45" t="s">
+      <c r="B90" s="63" t="s">
         <v>91</v>
       </c>
       <c r="C90">
@@ -2727,7 +2763,7 @@
       <c r="A91">
         <v>2521</v>
       </c>
-      <c r="B91" s="45" t="s">
+      <c r="B91" s="63" t="s">
         <v>92</v>
       </c>
       <c r="C91">
@@ -2738,7 +2774,7 @@
       <c r="A92">
         <v>2522</v>
       </c>
-      <c r="B92" s="45" t="s">
+      <c r="B92" s="63" t="s">
         <v>93</v>
       </c>
       <c r="C92">
@@ -2749,7 +2785,7 @@
       <c r="A93">
         <v>2523</v>
       </c>
-      <c r="B93" s="45" t="s">
+      <c r="B93" s="63" t="s">
         <v>94</v>
       </c>
       <c r="C93">
@@ -2760,7 +2796,7 @@
       <c r="A94">
         <v>2524</v>
       </c>
-      <c r="B94" s="45" t="s">
+      <c r="B94" s="63" t="s">
         <v>95</v>
       </c>
       <c r="C94">
@@ -2771,7 +2807,7 @@
       <c r="A95">
         <v>2525</v>
       </c>
-      <c r="B95" s="45" t="s">
+      <c r="B95" s="63" t="s">
         <v>96</v>
       </c>
       <c r="C95">
@@ -2782,7 +2818,7 @@
       <c r="A96">
         <v>2531</v>
       </c>
-      <c r="B96" s="45" t="s">
+      <c r="B96" s="63" t="s">
         <v>97</v>
       </c>
       <c r="C96">
@@ -2793,7 +2829,7 @@
       <c r="A97">
         <v>2611</v>
       </c>
-      <c r="B97" s="45" t="s">
+      <c r="B97" s="63" t="s">
         <v>98</v>
       </c>
       <c r="C97">
@@ -2804,7 +2840,7 @@
       <c r="A98">
         <v>2612</v>
       </c>
-      <c r="B98" s="45" t="s">
+      <c r="B98" s="63" t="s">
         <v>99</v>
       </c>
       <c r="C98">
@@ -2815,7 +2851,7 @@
       <c r="A99">
         <v>2613</v>
       </c>
-      <c r="B99" s="45" t="s">
+      <c r="B99" s="63" t="s">
         <v>100</v>
       </c>
       <c r="C99">
@@ -2826,7 +2862,7 @@
       <c r="A100">
         <v>2614</v>
       </c>
-      <c r="B100" s="45" t="s">
+      <c r="B100" s="63" t="s">
         <v>101</v>
       </c>
       <c r="C100">
@@ -2837,7 +2873,7 @@
       <c r="A101">
         <v>2615</v>
       </c>
-      <c r="B101" s="45" t="s">
+      <c r="B101" s="63" t="s">
         <v>102</v>
       </c>
       <c r="C101">
@@ -2848,7 +2884,7 @@
       <c r="A102">
         <v>2616</v>
       </c>
-      <c r="B102" s="45" t="s">
+      <c r="B102" s="63" t="s">
         <v>103</v>
       </c>
       <c r="C102">
@@ -2859,7 +2895,7 @@
       <c r="A103">
         <v>2617</v>
       </c>
-      <c r="B103" s="45" t="s">
+      <c r="B103" s="63" t="s">
         <v>104</v>
       </c>
       <c r="C103">
@@ -2870,7 +2906,7 @@
       <c r="A104">
         <v>2621</v>
       </c>
-      <c r="B104" s="45" t="s">
+      <c r="B104" s="63" t="s">
         <v>105</v>
       </c>
       <c r="C104">
@@ -2881,7 +2917,7 @@
       <c r="A105">
         <v>2622</v>
       </c>
-      <c r="B105" s="45" t="s">
+      <c r="B105" s="63" t="s">
         <v>106</v>
       </c>
       <c r="C105">
@@ -2892,7 +2928,7 @@
       <c r="A106">
         <v>2623</v>
       </c>
-      <c r="B106" s="45" t="s">
+      <c r="B106" s="63" t="s">
         <v>107</v>
       </c>
       <c r="C106">
@@ -2903,7 +2939,7 @@
       <c r="A107">
         <v>2624</v>
       </c>
-      <c r="B107" s="45" t="s">
+      <c r="B107" s="63" t="s">
         <v>108</v>
       </c>
       <c r="C107">
@@ -2914,7 +2950,7 @@
       <c r="A108">
         <v>2625</v>
       </c>
-      <c r="B108" s="45" t="s">
+      <c r="B108" s="63" t="s">
         <v>109</v>
       </c>
       <c r="C108">
@@ -2925,7 +2961,7 @@
       <c r="A109">
         <v>2627</v>
       </c>
-      <c r="B109" s="45" t="s">
+      <c r="B109" s="63" t="s">
         <v>110</v>
       </c>
       <c r="C109">
@@ -2936,7 +2972,7 @@
       <c r="A110">
         <v>2631</v>
       </c>
-      <c r="B110" s="45" t="s">
+      <c r="B110" s="63" t="s">
         <v>111</v>
       </c>
       <c r="C110">
@@ -2947,7 +2983,7 @@
       <c r="A111">
         <v>-1</v>
       </c>
-      <c r="B111" s="45" t="s">
+      <c r="B111" s="63" t="s">
         <v>112</v>
       </c>
       <c r="C111">
@@ -2958,7 +2994,7 @@
       <c r="A112">
         <v>3001</v>
       </c>
-      <c r="B112" s="45" t="s">
+      <c r="B112" s="63" t="s">
         <v>113</v>
       </c>
       <c r="C112">
@@ -2969,7 +3005,7 @@
       <c r="A113">
         <v>3003</v>
       </c>
-      <c r="B113" s="45" t="s">
+      <c r="B113" s="63" t="s">
         <v>114</v>
       </c>
       <c r="C113">
@@ -2980,7 +3016,7 @@
       <c r="A114">
         <v>3011</v>
       </c>
-      <c r="B114" s="45" t="s">
+      <c r="B114" s="63" t="s">
         <v>115</v>
       </c>
       <c r="C114">
@@ -2991,7 +3027,7 @@
       <c r="A115">
         <v>3012</v>
       </c>
-      <c r="B115" s="45" t="s">
+      <c r="B115" s="63" t="s">
         <v>116</v>
       </c>
       <c r="C115">
@@ -3002,7 +3038,7 @@
       <c r="A116">
         <v>3111</v>
       </c>
-      <c r="B116" s="45" t="s">
+      <c r="B116" s="63" t="s">
         <v>117</v>
       </c>
       <c r="C116">
@@ -3013,7 +3049,7 @@
       <c r="A117">
         <v>3112</v>
       </c>
-      <c r="B117" s="45" t="s">
+      <c r="B117" s="63" t="s">
         <v>118</v>
       </c>
       <c r="C117">
@@ -3024,7 +3060,7 @@
       <c r="A118">
         <v>3113</v>
       </c>
-      <c r="B118" s="45" t="s">
+      <c r="B118" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C118">
@@ -3035,7 +3071,7 @@
       <c r="A119">
         <v>3114</v>
       </c>
-      <c r="B119" s="45" t="s">
+      <c r="B119" s="63" t="s">
         <v>120</v>
       </c>
       <c r="C119">
@@ -3046,7 +3082,7 @@
       <c r="A120">
         <v>3115</v>
       </c>
-      <c r="B120" s="45" t="s">
+      <c r="B120" s="63" t="s">
         <v>121</v>
       </c>
       <c r="C120">
@@ -3057,7 +3093,7 @@
       <c r="A121">
         <v>3116</v>
       </c>
-      <c r="B121" s="45" t="s">
+      <c r="B121" s="63" t="s">
         <v>122</v>
       </c>
       <c r="C121">
@@ -3068,7 +3104,7 @@
       <c r="A122">
         <v>3117</v>
       </c>
-      <c r="B122" s="45" t="s">
+      <c r="B122" s="63" t="s">
         <v>123</v>
       </c>
       <c r="C122">
@@ -3079,7 +3115,7 @@
       <c r="A123">
         <v>3121</v>
       </c>
-      <c r="B123" s="45" t="s">
+      <c r="B123" s="63" t="s">
         <v>124</v>
       </c>
       <c r="C123">
@@ -3090,7 +3126,7 @@
       <c r="A124">
         <v>3122</v>
       </c>
-      <c r="B124" s="45" t="s">
+      <c r="B124" s="63" t="s">
         <v>125</v>
       </c>
       <c r="C124">
@@ -3101,7 +3137,7 @@
       <c r="A125">
         <v>3123</v>
       </c>
-      <c r="B125" s="45" t="s">
+      <c r="B125" s="63" t="s">
         <v>126</v>
       </c>
       <c r="C125">
@@ -3112,7 +3148,7 @@
       <c r="A126">
         <v>3131</v>
       </c>
-      <c r="B126" s="45" t="s">
+      <c r="B126" s="63" t="s">
         <v>127</v>
       </c>
       <c r="C126">
@@ -3123,7 +3159,7 @@
       <c r="A127">
         <v>3132</v>
       </c>
-      <c r="B127" s="45" t="s">
+      <c r="B127" s="63" t="s">
         <v>128</v>
       </c>
       <c r="C127">
@@ -3134,7 +3170,7 @@
       <c r="A128">
         <v>3134</v>
       </c>
-      <c r="B128" s="45" t="s">
+      <c r="B128" s="63" t="s">
         <v>129</v>
       </c>
       <c r="C128">
@@ -3145,7 +3181,7 @@
       <c r="A129">
         <v>3135</v>
       </c>
-      <c r="B129" s="45" t="s">
+      <c r="B129" s="63" t="s">
         <v>130</v>
       </c>
       <c r="C129">
@@ -3156,7 +3192,7 @@
       <c r="A130">
         <v>3136</v>
       </c>
-      <c r="B130" s="45" t="s">
+      <c r="B130" s="63" t="s">
         <v>131</v>
       </c>
       <c r="C130">
@@ -3167,7 +3203,7 @@
       <c r="A131">
         <v>3141</v>
       </c>
-      <c r="B131" s="45" t="s">
+      <c r="B131" s="63" t="s">
         <v>132</v>
       </c>
       <c r="C131">
@@ -3178,7 +3214,7 @@
       <c r="A132">
         <v>3142</v>
       </c>
-      <c r="B132" s="45" t="s">
+      <c r="B132" s="63" t="s">
         <v>133</v>
       </c>
       <c r="C132">
@@ -3189,7 +3225,7 @@
       <c r="A133">
         <v>3143</v>
       </c>
-      <c r="B133" s="45" t="s">
+      <c r="B133" s="63" t="s">
         <v>134</v>
       </c>
       <c r="C133">
@@ -3200,7 +3236,7 @@
       <c r="A134">
         <v>3144</v>
       </c>
-      <c r="B134" s="45" t="s">
+      <c r="B134" s="63" t="s">
         <v>135</v>
       </c>
       <c r="C134">
@@ -3211,7 +3247,7 @@
       <c r="A135">
         <v>3146</v>
       </c>
-      <c r="B135" s="45" t="s">
+      <c r="B135" s="63" t="s">
         <v>136</v>
       </c>
       <c r="C135">
@@ -3222,7 +3258,7 @@
       <c r="A136">
         <v>3147</v>
       </c>
-      <c r="B136" s="45" t="s">
+      <c r="B136" s="63" t="s">
         <v>137</v>
       </c>
       <c r="C136">
@@ -3233,7 +3269,7 @@
       <c r="A137">
         <v>3161</v>
       </c>
-      <c r="B137" s="45" t="s">
+      <c r="B137" s="63" t="s">
         <v>138</v>
       </c>
       <c r="C137">
@@ -3244,7 +3280,7 @@
       <c r="A138">
         <v>3162</v>
       </c>
-      <c r="B138" s="45" t="s">
+      <c r="B138" s="63" t="s">
         <v>139</v>
       </c>
       <c r="C138">
@@ -3255,7 +3291,7 @@
       <c r="A139">
         <v>3163</v>
       </c>
-      <c r="B139" s="45" t="s">
+      <c r="B139" s="63" t="s">
         <v>140</v>
       </c>
       <c r="C139">
@@ -3266,7 +3302,7 @@
       <c r="A140">
         <v>3171</v>
       </c>
-      <c r="B140" s="45" t="s">
+      <c r="B140" s="63" t="s">
         <v>141</v>
       </c>
       <c r="C140">
@@ -3277,7 +3313,7 @@
       <c r="A141">
         <v>3172</v>
       </c>
-      <c r="B141" s="45" t="s">
+      <c r="B141" s="63" t="s">
         <v>142</v>
       </c>
       <c r="C141">
@@ -3288,7 +3324,7 @@
       <c r="A142">
         <v>3189</v>
       </c>
-      <c r="B142" s="45" t="s">
+      <c r="B142" s="63" t="s">
         <v>143</v>
       </c>
       <c r="C142">
@@ -3299,7 +3335,7 @@
       <c r="A143">
         <v>3191</v>
       </c>
-      <c r="B143" s="45" t="s">
+      <c r="B143" s="63" t="s">
         <v>144</v>
       </c>
       <c r="C143">
@@ -3310,7 +3346,7 @@
       <c r="A144">
         <v>3192</v>
       </c>
-      <c r="B144" s="45" t="s">
+      <c r="B144" s="63" t="s">
         <v>145</v>
       </c>
       <c r="C144">
@@ -3321,7 +3357,7 @@
       <c r="A145">
         <v>3201</v>
       </c>
-      <c r="B145" s="45" t="s">
+      <c r="B145" s="63" t="s">
         <v>146</v>
       </c>
       <c r="C145">
@@ -3332,7 +3368,7 @@
       <c r="A146">
         <v>3210</v>
       </c>
-      <c r="B146" s="45" t="s">
+      <c r="B146" s="63" t="s">
         <v>147</v>
       </c>
       <c r="C146">
@@ -3343,7 +3379,7 @@
       <c r="A147">
         <v>3211</v>
       </c>
-      <c r="B147" s="45" t="s">
+      <c r="B147" s="63" t="s">
         <v>148</v>
       </c>
       <c r="C147">
@@ -3354,7 +3390,7 @@
       <c r="A148">
         <v>3212</v>
       </c>
-      <c r="B148" s="45" t="s">
+      <c r="B148" s="63" t="s">
         <v>149</v>
       </c>
       <c r="C148">
@@ -3365,7 +3401,7 @@
       <c r="A149">
         <v>3213</v>
       </c>
-      <c r="B149" s="45" t="s">
+      <c r="B149" s="63" t="s">
         <v>150</v>
       </c>
       <c r="C149">
@@ -3376,7 +3412,7 @@
       <c r="A150">
         <v>3214</v>
       </c>
-      <c r="B150" s="45" t="s">
+      <c r="B150" s="63" t="s">
         <v>151</v>
       </c>
       <c r="C150">
@@ -3387,7 +3423,7 @@
       <c r="A151">
         <v>3221</v>
       </c>
-      <c r="B151" s="45" t="s">
+      <c r="B151" s="63" t="s">
         <v>152</v>
       </c>
       <c r="C151">
@@ -3398,7 +3434,7 @@
       <c r="A152">
         <v>3222</v>
       </c>
-      <c r="B152" s="45" t="s">
+      <c r="B152" s="63" t="s">
         <v>153</v>
       </c>
       <c r="C152">
@@ -3409,7 +3445,7 @@
       <c r="A153">
         <v>3223</v>
       </c>
-      <c r="B153" s="45" t="s">
+      <c r="B153" s="63" t="s">
         <v>154</v>
       </c>
       <c r="C153">
@@ -3420,7 +3456,7 @@
       <c r="A154">
         <v>3224</v>
       </c>
-      <c r="B154" s="45" t="s">
+      <c r="B154" s="63" t="s">
         <v>155</v>
       </c>
       <c r="C154">
@@ -3431,7 +3467,7 @@
       <c r="A155">
         <v>3225</v>
       </c>
-      <c r="B155" s="45" t="s">
+      <c r="B155" s="63" t="s">
         <v>156</v>
       </c>
       <c r="C155">
@@ -3442,7 +3478,7 @@
       <c r="A156">
         <v>3231</v>
       </c>
-      <c r="B156" s="45" t="s">
+      <c r="B156" s="63" t="s">
         <v>157</v>
       </c>
       <c r="C156">
@@ -3453,7 +3489,7 @@
       <c r="A157">
         <v>3232</v>
       </c>
-      <c r="B157" s="45" t="s">
+      <c r="B157" s="63" t="s">
         <v>158</v>
       </c>
       <c r="C157">
@@ -3464,7 +3500,7 @@
       <c r="A158">
         <v>3241</v>
       </c>
-      <c r="B158" s="45" t="s">
+      <c r="B158" s="63" t="s">
         <v>159</v>
       </c>
       <c r="C158">
@@ -3475,7 +3511,7 @@
       <c r="A159">
         <v>3242</v>
       </c>
-      <c r="B159" s="45" t="s">
+      <c r="B159" s="63" t="s">
         <v>160</v>
       </c>
       <c r="C159">
@@ -3486,7 +3522,7 @@
       <c r="A160">
         <v>3250</v>
       </c>
-      <c r="B160" s="45" t="s">
+      <c r="B160" s="63" t="s">
         <v>161</v>
       </c>
       <c r="C160">
@@ -3497,7 +3533,7 @@
       <c r="A161">
         <v>3251</v>
       </c>
-      <c r="B161" s="45" t="s">
+      <c r="B161" s="63" t="s">
         <v>162</v>
       </c>
       <c r="C161">
@@ -3508,7 +3544,7 @@
       <c r="A162">
         <v>3252</v>
       </c>
-      <c r="B162" s="45" t="s">
+      <c r="B162" s="63" t="s">
         <v>163</v>
       </c>
       <c r="C162">
@@ -3519,7 +3555,7 @@
       <c r="A163">
         <v>3253</v>
       </c>
-      <c r="B163" s="45" t="s">
+      <c r="B163" s="63" t="s">
         <v>164</v>
       </c>
       <c r="C163">
@@ -3530,7 +3566,7 @@
       <c r="A164">
         <v>3281</v>
       </c>
-      <c r="B164" s="45" t="s">
+      <c r="B164" s="63" t="s">
         <v>165</v>
       </c>
       <c r="C164">
@@ -3541,7 +3577,7 @@
       <c r="A165">
         <v>3311</v>
       </c>
-      <c r="B165" s="45" t="s">
+      <c r="B165" s="63" t="s">
         <v>166</v>
       </c>
       <c r="C165">
@@ -3552,7 +3588,7 @@
       <c r="A166">
         <v>3312</v>
       </c>
-      <c r="B166" s="45" t="s">
+      <c r="B166" s="63" t="s">
         <v>167</v>
       </c>
       <c r="C166">
@@ -3563,7 +3599,7 @@
       <c r="A167">
         <v>3313</v>
       </c>
-      <c r="B167" s="45" t="s">
+      <c r="B167" s="63" t="s">
         <v>168</v>
       </c>
       <c r="C167">
@@ -3574,7 +3610,7 @@
       <c r="A168">
         <v>3321</v>
       </c>
-      <c r="B168" s="45" t="s">
+      <c r="B168" s="63" t="s">
         <v>169</v>
       </c>
       <c r="C168">
@@ -3585,7 +3621,7 @@
       <c r="A169">
         <v>3322</v>
       </c>
-      <c r="B169" s="45" t="s">
+      <c r="B169" s="63" t="s">
         <v>170</v>
       </c>
       <c r="C169">
@@ -3596,7 +3632,7 @@
       <c r="A170">
         <v>3331</v>
       </c>
-      <c r="B170" s="45" t="s">
+      <c r="B170" s="63" t="s">
         <v>171</v>
       </c>
       <c r="C170">
@@ -3607,7 +3643,7 @@
       <c r="A171">
         <v>3341</v>
       </c>
-      <c r="B171" s="45" t="s">
+      <c r="B171" s="63" t="s">
         <v>172</v>
       </c>
       <c r="C171">
@@ -3618,7 +3654,7 @@
       <c r="A172">
         <v>3411</v>
       </c>
-      <c r="B172" s="45" t="s">
+      <c r="B172" s="63" t="s">
         <v>173</v>
       </c>
       <c r="C172">
@@ -3629,7 +3665,7 @@
       <c r="A173">
         <v>3412</v>
       </c>
-      <c r="B173" s="45" t="s">
+      <c r="B173" s="63" t="s">
         <v>174</v>
       </c>
       <c r="C173">
@@ -3640,7 +3676,7 @@
       <c r="A174">
         <v>3413</v>
       </c>
-      <c r="B174" s="45" t="s">
+      <c r="B174" s="63" t="s">
         <v>175</v>
       </c>
       <c r="C174">
@@ -3651,7 +3687,7 @@
       <c r="A175">
         <v>3421</v>
       </c>
-      <c r="B175" s="45" t="s">
+      <c r="B175" s="63" t="s">
         <v>176</v>
       </c>
       <c r="C175">
@@ -3662,7 +3698,7 @@
       <c r="A176">
         <v>3422</v>
       </c>
-      <c r="B176" s="45" t="s">
+      <c r="B176" s="63" t="s">
         <v>177</v>
       </c>
       <c r="C176">
@@ -3673,7 +3709,7 @@
       <c r="A177">
         <v>3423</v>
       </c>
-      <c r="B177" s="45" t="s">
+      <c r="B177" s="63" t="s">
         <v>178</v>
       </c>
       <c r="C177">
@@ -3684,7 +3720,7 @@
       <c r="A178">
         <v>3424</v>
       </c>
-      <c r="B178" s="45" t="s">
+      <c r="B178" s="63" t="s">
         <v>179</v>
       </c>
       <c r="C178">
@@ -3695,7 +3731,7 @@
       <c r="A179">
         <v>3425</v>
       </c>
-      <c r="B179" s="45" t="s">
+      <c r="B179" s="63" t="s">
         <v>180</v>
       </c>
       <c r="C179">
@@ -3706,7 +3742,7 @@
       <c r="A180">
         <v>3426</v>
       </c>
-      <c r="B180" s="45" t="s">
+      <c r="B180" s="63" t="s">
         <v>181</v>
       </c>
       <c r="C180">
@@ -3717,7 +3753,7 @@
       <c r="A181">
         <v>3511</v>
       </c>
-      <c r="B181" s="45" t="s">
+      <c r="B181" s="63" t="s">
         <v>182</v>
       </c>
       <c r="C181">
@@ -3728,7 +3764,7 @@
       <c r="A182">
         <v>3512</v>
       </c>
-      <c r="B182" s="45" t="s">
+      <c r="B182" s="63" t="s">
         <v>183</v>
       </c>
       <c r="C182">
@@ -3739,7 +3775,7 @@
       <c r="A183">
         <v>3513</v>
       </c>
-      <c r="B183" s="45" t="s">
+      <c r="B183" s="63" t="s">
         <v>184</v>
       </c>
       <c r="C183">
@@ -3750,7 +3786,7 @@
       <c r="A184">
         <v>3514</v>
       </c>
-      <c r="B184" s="45" t="s">
+      <c r="B184" s="63" t="s">
         <v>185</v>
       </c>
       <c r="C184">
@@ -3761,7 +3797,7 @@
       <c r="A185">
         <v>3515</v>
       </c>
-      <c r="B185" s="45" t="s">
+      <c r="B185" s="63" t="s">
         <v>186</v>
       </c>
       <c r="C185">
@@ -3772,7 +3808,7 @@
       <c r="A186">
         <v>3516</v>
       </c>
-      <c r="B186" s="45" t="s">
+      <c r="B186" s="63" t="s">
         <v>187</v>
       </c>
       <c r="C186">
@@ -3783,7 +3819,7 @@
       <c r="A187">
         <v>3517</v>
       </c>
-      <c r="B187" s="45" t="s">
+      <c r="B187" s="63" t="s">
         <v>188</v>
       </c>
       <c r="C187">
@@ -3794,7 +3830,7 @@
       <c r="A188">
         <v>3518</v>
       </c>
-      <c r="B188" s="45" t="s">
+      <c r="B188" s="63" t="s">
         <v>189</v>
       </c>
       <c r="C188">
@@ -3805,7 +3841,7 @@
       <c r="A189">
         <v>3522</v>
       </c>
-      <c r="B189" s="45" t="s">
+      <c r="B189" s="63" t="s">
         <v>190</v>
       </c>
       <c r="C189">
@@ -3816,7 +3852,7 @@
       <c r="A190">
         <v>3523</v>
       </c>
-      <c r="B190" s="45" t="s">
+      <c r="B190" s="63" t="s">
         <v>191</v>
       </c>
       <c r="C190">
@@ -3827,7 +3863,7 @@
       <c r="A191">
         <v>3524</v>
       </c>
-      <c r="B191" s="45" t="s">
+      <c r="B191" s="63" t="s">
         <v>192</v>
       </c>
       <c r="C191">
@@ -3838,7 +3874,7 @@
       <c r="A192">
         <v>3525</v>
       </c>
-      <c r="B192" s="45" t="s">
+      <c r="B192" s="63" t="s">
         <v>193</v>
       </c>
       <c r="C192">
@@ -3849,7 +3885,7 @@
       <c r="A193">
         <v>3531</v>
       </c>
-      <c r="B193" s="45" t="s">
+      <c r="B193" s="63" t="s">
         <v>194</v>
       </c>
       <c r="C193">
@@ -3860,7 +3896,7 @@
       <c r="A194">
         <v>3532</v>
       </c>
-      <c r="B194" s="45" t="s">
+      <c r="B194" s="63" t="s">
         <v>195</v>
       </c>
       <c r="C194">
@@ -3871,7 +3907,7 @@
       <c r="A195">
         <v>3541</v>
       </c>
-      <c r="B195" s="45" t="s">
+      <c r="B195" s="63" t="s">
         <v>196</v>
       </c>
       <c r="C195">
@@ -3882,7 +3918,7 @@
       <c r="A196">
         <v>3542</v>
       </c>
-      <c r="B196" s="45" t="s">
+      <c r="B196" s="63" t="s">
         <v>197</v>
       </c>
       <c r="C196">
@@ -3893,7 +3929,7 @@
       <c r="A197">
         <v>3543</v>
       </c>
-      <c r="B197" s="45" t="s">
+      <c r="B197" s="63" t="s">
         <v>198</v>
       </c>
       <c r="C197">
@@ -3904,7 +3940,7 @@
       <c r="A198">
         <v>3544</v>
       </c>
-      <c r="B198" s="45" t="s">
+      <c r="B198" s="63" t="s">
         <v>199</v>
       </c>
       <c r="C198">
@@ -3915,7 +3951,7 @@
       <c r="A199">
         <v>3545</v>
       </c>
-      <c r="B199" s="45" t="s">
+      <c r="B199" s="63" t="s">
         <v>200</v>
       </c>
       <c r="C199">
@@ -3926,7 +3962,7 @@
       <c r="A200">
         <v>3546</v>
       </c>
-      <c r="B200" s="45" t="s">
+      <c r="B200" s="63" t="s">
         <v>201</v>
       </c>
       <c r="C200">
@@ -3937,7 +3973,7 @@
       <c r="A201">
         <v>3547</v>
       </c>
-      <c r="B201" s="45" t="s">
+      <c r="B201" s="63" t="s">
         <v>202</v>
       </c>
       <c r="C201">
@@ -3948,7 +3984,7 @@
       <c r="A202">
         <v>3548</v>
       </c>
-      <c r="B202" s="45" t="s">
+      <c r="B202" s="63" t="s">
         <v>203</v>
       </c>
       <c r="C202">
@@ -3959,7 +3995,7 @@
       <c r="A203">
         <v>3711</v>
       </c>
-      <c r="B203" s="45" t="s">
+      <c r="B203" s="63" t="s">
         <v>204</v>
       </c>
       <c r="C203">
@@ -3970,7 +4006,7 @@
       <c r="A204">
         <v>3712</v>
       </c>
-      <c r="B204" s="45" t="s">
+      <c r="B204" s="63" t="s">
         <v>205</v>
       </c>
       <c r="C204">
@@ -3981,7 +4017,7 @@
       <c r="A205">
         <v>3713</v>
       </c>
-      <c r="B205" s="45" t="s">
+      <c r="B205" s="63" t="s">
         <v>206</v>
       </c>
       <c r="C205">
@@ -3992,7 +4028,7 @@
       <c r="A206">
         <v>3721</v>
       </c>
-      <c r="B206" s="45" t="s">
+      <c r="B206" s="63" t="s">
         <v>207</v>
       </c>
       <c r="C206">
@@ -4003,7 +4039,7 @@
       <c r="A207">
         <v>3722</v>
       </c>
-      <c r="B207" s="45" t="s">
+      <c r="B207" s="63" t="s">
         <v>208</v>
       </c>
       <c r="C207">
@@ -4014,7 +4050,7 @@
       <c r="A208">
         <v>3723</v>
       </c>
-      <c r="B208" s="45" t="s">
+      <c r="B208" s="63" t="s">
         <v>209</v>
       </c>
       <c r="C208">
@@ -4025,7 +4061,7 @@
       <c r="A209">
         <v>3731</v>
       </c>
-      <c r="B209" s="45" t="s">
+      <c r="B209" s="63" t="s">
         <v>210</v>
       </c>
       <c r="C209">
@@ -4036,7 +4072,7 @@
       <c r="A210">
         <v>3732</v>
       </c>
-      <c r="B210" s="45" t="s">
+      <c r="B210" s="63" t="s">
         <v>211</v>
       </c>
       <c r="C210">
@@ -4047,7 +4083,7 @@
       <c r="A211">
         <v>3741</v>
       </c>
-      <c r="B211" s="45" t="s">
+      <c r="B211" s="63" t="s">
         <v>212</v>
       </c>
       <c r="C211">
@@ -4058,7 +4094,7 @@
       <c r="A212">
         <v>3742</v>
       </c>
-      <c r="B212" s="45" t="s">
+      <c r="B212" s="63" t="s">
         <v>213</v>
       </c>
       <c r="C212">
@@ -4069,7 +4105,7 @@
       <c r="A213">
         <v>3743</v>
       </c>
-      <c r="B213" s="45" t="s">
+      <c r="B213" s="63" t="s">
         <v>214</v>
       </c>
       <c r="C213">
@@ -4080,7 +4116,7 @@
       <c r="A214">
         <v>3751</v>
       </c>
-      <c r="B214" s="45" t="s">
+      <c r="B214" s="63" t="s">
         <v>215</v>
       </c>
       <c r="C214">
@@ -4091,7 +4127,7 @@
       <c r="A215">
         <v>3761</v>
       </c>
-      <c r="B215" s="45" t="s">
+      <c r="B215" s="63" t="s">
         <v>216</v>
       </c>
       <c r="C215">
@@ -4102,7 +4138,7 @@
       <c r="A216">
         <v>3762</v>
       </c>
-      <c r="B216" s="45" t="s">
+      <c r="B216" s="63" t="s">
         <v>217</v>
       </c>
       <c r="C216">
@@ -4113,7 +4149,7 @@
       <c r="A217">
         <v>3763</v>
       </c>
-      <c r="B217" s="45" t="s">
+      <c r="B217" s="63" t="s">
         <v>218</v>
       </c>
       <c r="C217">
@@ -4124,7 +4160,7 @@
       <c r="A218">
         <v>3764</v>
       </c>
-      <c r="B218" s="45" t="s">
+      <c r="B218" s="63" t="s">
         <v>219</v>
       </c>
       <c r="C218">
@@ -4135,7 +4171,7 @@
       <c r="A219">
         <v>3765</v>
       </c>
-      <c r="B219" s="45" t="s">
+      <c r="B219" s="63" t="s">
         <v>220</v>
       </c>
       <c r="C219">
@@ -4146,7 +4182,7 @@
       <c r="A220">
         <v>3771</v>
       </c>
-      <c r="B220" s="45" t="s">
+      <c r="B220" s="63" t="s">
         <v>221</v>
       </c>
       <c r="C220">
@@ -4157,7 +4193,7 @@
       <c r="A221">
         <v>3772</v>
       </c>
-      <c r="B221" s="45" t="s">
+      <c r="B221" s="63" t="s">
         <v>222</v>
       </c>
       <c r="C221">
@@ -4168,7 +4204,7 @@
       <c r="A222">
         <v>3773</v>
       </c>
-      <c r="B222" s="45" t="s">
+      <c r="B222" s="63" t="s">
         <v>223</v>
       </c>
       <c r="C222">
@@ -4179,7 +4215,7 @@
       <c r="A223">
         <v>3911</v>
       </c>
-      <c r="B223" s="45" t="s">
+      <c r="B223" s="63" t="s">
         <v>224</v>
       </c>
       <c r="C223">
@@ -4190,7 +4226,7 @@
       <c r="A224">
         <v>3912</v>
       </c>
-      <c r="B224" s="45" t="s">
+      <c r="B224" s="63" t="s">
         <v>225</v>
       </c>
       <c r="C224">
@@ -4201,7 +4237,7 @@
       <c r="A225">
         <v>-1</v>
       </c>
-      <c r="B225" s="45" t="s">
+      <c r="B225" s="63" t="s">
         <v>226</v>
       </c>
       <c r="C225">
@@ -4212,7 +4248,7 @@
       <c r="A226">
         <v>4101</v>
       </c>
-      <c r="B226" s="45" t="s">
+      <c r="B226" s="63" t="s">
         <v>227</v>
       </c>
       <c r="C226">
@@ -4223,7 +4259,7 @@
       <c r="A227">
         <v>4102</v>
       </c>
-      <c r="B227" s="45" t="s">
+      <c r="B227" s="63" t="s">
         <v>228</v>
       </c>
       <c r="C227">
@@ -4234,7 +4270,7 @@
       <c r="A228">
         <v>4110</v>
       </c>
-      <c r="B228" s="45" t="s">
+      <c r="B228" s="63" t="s">
         <v>229</v>
       </c>
       <c r="C228">
@@ -4245,7 +4281,7 @@
       <c r="A229">
         <v>4121</v>
       </c>
-      <c r="B229" s="45" t="s">
+      <c r="B229" s="63" t="s">
         <v>230</v>
       </c>
       <c r="C229">
@@ -4256,7 +4292,7 @@
       <c r="A230">
         <v>4122</v>
       </c>
-      <c r="B230" s="45" t="s">
+      <c r="B230" s="63" t="s">
         <v>231</v>
       </c>
       <c r="C230">
@@ -4267,7 +4303,7 @@
       <c r="A231">
         <v>4123</v>
       </c>
-      <c r="B231" s="45" t="s">
+      <c r="B231" s="63" t="s">
         <v>232</v>
       </c>
       <c r="C231">
@@ -4278,7 +4314,7 @@
       <c r="A232">
         <v>4131</v>
       </c>
-      <c r="B232" s="45" t="s">
+      <c r="B232" s="63" t="s">
         <v>233</v>
       </c>
       <c r="C232">
@@ -4289,7 +4325,7 @@
       <c r="A233">
         <v>4132</v>
       </c>
-      <c r="B233" s="45" t="s">
+      <c r="B233" s="63" t="s">
         <v>234</v>
       </c>
       <c r="C233">
@@ -4300,7 +4336,7 @@
       <c r="A234">
         <v>4141</v>
       </c>
-      <c r="B234" s="45" t="s">
+      <c r="B234" s="63" t="s">
         <v>235</v>
       </c>
       <c r="C234">
@@ -4311,7 +4347,7 @@
       <c r="A235">
         <v>4142</v>
       </c>
-      <c r="B235" s="45" t="s">
+      <c r="B235" s="63" t="s">
         <v>236</v>
       </c>
       <c r="C235">
@@ -4322,7 +4358,7 @@
       <c r="A236">
         <v>4151</v>
       </c>
-      <c r="B236" s="45" t="s">
+      <c r="B236" s="63" t="s">
         <v>237</v>
       </c>
       <c r="C236">
@@ -4333,7 +4369,7 @@
       <c r="A237">
         <v>4152</v>
       </c>
-      <c r="B237" s="45" t="s">
+      <c r="B237" s="63" t="s">
         <v>238</v>
       </c>
       <c r="C237">
@@ -4344,7 +4380,7 @@
       <c r="A238">
         <v>4201</v>
       </c>
-      <c r="B238" s="45" t="s">
+      <c r="B238" s="63" t="s">
         <v>239</v>
       </c>
       <c r="C238">
@@ -4355,7 +4391,7 @@
       <c r="A239">
         <v>4211</v>
       </c>
-      <c r="B239" s="45" t="s">
+      <c r="B239" s="63" t="s">
         <v>240</v>
       </c>
       <c r="C239">
@@ -4366,7 +4402,7 @@
       <c r="A240">
         <v>4212</v>
       </c>
-      <c r="B240" s="45" t="s">
+      <c r="B240" s="63" t="s">
         <v>241</v>
       </c>
       <c r="C240">
@@ -4377,7 +4413,7 @@
       <c r="A241">
         <v>4213</v>
       </c>
-      <c r="B241" s="45" t="s">
+      <c r="B241" s="63" t="s">
         <v>242</v>
       </c>
       <c r="C241">
@@ -4388,7 +4424,7 @@
       <c r="A242">
         <v>4214</v>
       </c>
-      <c r="B242" s="45" t="s">
+      <c r="B242" s="63" t="s">
         <v>243</v>
       </c>
       <c r="C242">
@@ -4399,7 +4435,7 @@
       <c r="A243">
         <v>4221</v>
       </c>
-      <c r="B243" s="45" t="s">
+      <c r="B243" s="63" t="s">
         <v>244</v>
       </c>
       <c r="C243">
@@ -4410,7 +4446,7 @@
       <c r="A244">
         <v>4222</v>
       </c>
-      <c r="B244" s="45" t="s">
+      <c r="B244" s="63" t="s">
         <v>245</v>
       </c>
       <c r="C244">
@@ -4421,7 +4457,7 @@
       <c r="A245">
         <v>4223</v>
       </c>
-      <c r="B245" s="45" t="s">
+      <c r="B245" s="63" t="s">
         <v>246</v>
       </c>
       <c r="C245">
@@ -4432,7 +4468,7 @@
       <c r="A246">
         <v>4231</v>
       </c>
-      <c r="B246" s="45" t="s">
+      <c r="B246" s="63" t="s">
         <v>247</v>
       </c>
       <c r="C246">
@@ -4443,7 +4479,7 @@
       <c r="A247">
         <v>4241</v>
       </c>
-      <c r="B247" s="45" t="s">
+      <c r="B247" s="63" t="s">
         <v>248</v>
       </c>
       <c r="C247">
@@ -4454,7 +4490,7 @@
       <c r="A248">
         <v>-1</v>
       </c>
-      <c r="B248" s="45" t="s">
+      <c r="B248" s="63" t="s">
         <v>249</v>
       </c>
       <c r="C248">
@@ -4465,7 +4501,7 @@
       <c r="A249">
         <v>5101</v>
       </c>
-      <c r="B249" s="45" t="s">
+      <c r="B249" s="63" t="s">
         <v>250</v>
       </c>
       <c r="C249">
@@ -4476,7 +4512,7 @@
       <c r="A250">
         <v>5102</v>
       </c>
-      <c r="B250" s="45" t="s">
+      <c r="B250" s="63" t="s">
         <v>251</v>
       </c>
       <c r="C250">
@@ -4487,7 +4523,7 @@
       <c r="A251">
         <v>5103</v>
       </c>
-      <c r="B251" s="45" t="s">
+      <c r="B251" s="63" t="s">
         <v>252</v>
       </c>
       <c r="C251">
@@ -4498,7 +4534,7 @@
       <c r="A252">
         <v>5111</v>
       </c>
-      <c r="B252" s="45" t="s">
+      <c r="B252" s="63" t="s">
         <v>253</v>
       </c>
       <c r="C252">
@@ -4509,7 +4545,7 @@
       <c r="A253">
         <v>5112</v>
       </c>
-      <c r="B253" s="45" t="s">
+      <c r="B253" s="63" t="s">
         <v>254</v>
       </c>
       <c r="C253">
@@ -4520,7 +4556,7 @@
       <c r="A254">
         <v>5114</v>
       </c>
-      <c r="B254" s="45" t="s">
+      <c r="B254" s="63" t="s">
         <v>255</v>
       </c>
       <c r="C254">
@@ -4531,7 +4567,7 @@
       <c r="A255">
         <v>5121</v>
       </c>
-      <c r="B255" s="45" t="s">
+      <c r="B255" s="63" t="s">
         <v>256</v>
       </c>
       <c r="C255">
@@ -4542,7 +4578,7 @@
       <c r="A256">
         <v>5131</v>
       </c>
-      <c r="B256" s="45" t="s">
+      <c r="B256" s="63" t="s">
         <v>257</v>
       </c>
       <c r="C256">
@@ -4553,7 +4589,7 @@
       <c r="A257">
         <v>5132</v>
       </c>
-      <c r="B257" s="45" t="s">
+      <c r="B257" s="63" t="s">
         <v>258</v>
       </c>
       <c r="C257">
@@ -4564,7 +4600,7 @@
       <c r="A258">
         <v>5133</v>
       </c>
-      <c r="B258" s="45" t="s">
+      <c r="B258" s="63" t="s">
         <v>259</v>
       </c>
       <c r="C258">
@@ -4575,7 +4611,7 @@
       <c r="A259">
         <v>5134</v>
       </c>
-      <c r="B259" s="45" t="s">
+      <c r="B259" s="63" t="s">
         <v>260</v>
       </c>
       <c r="C259">
@@ -4586,7 +4622,7 @@
       <c r="A260">
         <v>5141</v>
       </c>
-      <c r="B260" s="45" t="s">
+      <c r="B260" s="63" t="s">
         <v>261</v>
       </c>
       <c r="C260">
@@ -4597,7 +4633,7 @@
       <c r="A261">
         <v>5142</v>
       </c>
-      <c r="B261" s="45" t="s">
+      <c r="B261" s="63" t="s">
         <v>262</v>
       </c>
       <c r="C261">
@@ -4608,7 +4644,7 @@
       <c r="A262">
         <v>5151</v>
       </c>
-      <c r="B262" s="45" t="s">
+      <c r="B262" s="63" t="s">
         <v>263</v>
       </c>
       <c r="C262">
@@ -4619,7 +4655,7 @@
       <c r="A263">
         <v>5152</v>
       </c>
-      <c r="B263" s="45" t="s">
+      <c r="B263" s="63" t="s">
         <v>264</v>
       </c>
       <c r="C263">
@@ -4630,7 +4666,7 @@
       <c r="A264">
         <v>5161</v>
       </c>
-      <c r="B264" s="45" t="s">
+      <c r="B264" s="63" t="s">
         <v>265</v>
       </c>
       <c r="C264">
@@ -4641,7 +4677,7 @@
       <c r="A265">
         <v>5162</v>
       </c>
-      <c r="B265" s="45" t="s">
+      <c r="B265" s="63" t="s">
         <v>266</v>
       </c>
       <c r="C265">
@@ -4652,7 +4688,7 @@
       <c r="A266">
         <v>5165</v>
       </c>
-      <c r="B266" s="45" t="s">
+      <c r="B266" s="63" t="s">
         <v>267</v>
       </c>
       <c r="C266">
@@ -4663,7 +4699,7 @@
       <c r="A267">
         <v>5166</v>
       </c>
-      <c r="B267" s="45" t="s">
+      <c r="B267" s="63" t="s">
         <v>268</v>
       </c>
       <c r="C267">
@@ -4674,7 +4710,7 @@
       <c r="A268">
         <v>5167</v>
       </c>
-      <c r="B268" s="45" t="s">
+      <c r="B268" s="63" t="s">
         <v>269</v>
       </c>
       <c r="C268">
@@ -4685,7 +4721,7 @@
       <c r="A269">
         <v>5169</v>
       </c>
-      <c r="B269" s="45" t="s">
+      <c r="B269" s="63" t="s">
         <v>270</v>
       </c>
       <c r="C269">
@@ -4696,7 +4732,7 @@
       <c r="A270">
         <v>5171</v>
       </c>
-      <c r="B270" s="45" t="s">
+      <c r="B270" s="63" t="s">
         <v>271</v>
       </c>
       <c r="C270">
@@ -4707,7 +4743,7 @@
       <c r="A271">
         <v>5172</v>
       </c>
-      <c r="B271" s="45" t="s">
+      <c r="B271" s="63" t="s">
         <v>272</v>
       </c>
       <c r="C271">
@@ -4718,7 +4754,7 @@
       <c r="A272">
         <v>5173</v>
       </c>
-      <c r="B272" s="45" t="s">
+      <c r="B272" s="63" t="s">
         <v>273</v>
       </c>
       <c r="C272">
@@ -4729,7 +4765,7 @@
       <c r="A273">
         <v>5174</v>
       </c>
-      <c r="B273" s="45" t="s">
+      <c r="B273" s="63" t="s">
         <v>274</v>
       </c>
       <c r="C273">
@@ -4740,7 +4776,7 @@
       <c r="A274">
         <v>5191</v>
       </c>
-      <c r="B274" s="45" t="s">
+      <c r="B274" s="63" t="s">
         <v>275</v>
       </c>
       <c r="C274">
@@ -4751,7 +4787,7 @@
       <c r="A275">
         <v>5192</v>
       </c>
-      <c r="B275" s="45" t="s">
+      <c r="B275" s="63" t="s">
         <v>276</v>
       </c>
       <c r="C275">
@@ -4762,7 +4798,7 @@
       <c r="A276">
         <v>5198</v>
       </c>
-      <c r="B276" s="45" t="s">
+      <c r="B276" s="63" t="s">
         <v>277</v>
       </c>
       <c r="C276">
@@ -4773,7 +4809,7 @@
       <c r="A277">
         <v>5199</v>
       </c>
-      <c r="B277" s="45" t="s">
+      <c r="B277" s="63" t="s">
         <v>278</v>
       </c>
       <c r="C277">
@@ -4784,7 +4820,7 @@
       <c r="A278">
         <v>5201</v>
       </c>
-      <c r="B278" s="45" t="s">
+      <c r="B278" s="63" t="s">
         <v>279</v>
       </c>
       <c r="C278">
@@ -4795,7 +4831,7 @@
       <c r="A279">
         <v>5211</v>
       </c>
-      <c r="B279" s="45" t="s">
+      <c r="B279" s="63" t="s">
         <v>280</v>
       </c>
       <c r="C279">
@@ -4806,7 +4842,7 @@
       <c r="A280">
         <v>5221</v>
       </c>
-      <c r="B280" s="45" t="s">
+      <c r="B280" s="63" t="s">
         <v>281</v>
       </c>
       <c r="C280">
@@ -4817,7 +4853,7 @@
       <c r="A281">
         <v>5231</v>
       </c>
-      <c r="B281" s="45" t="s">
+      <c r="B281" s="63" t="s">
         <v>282</v>
       </c>
       <c r="C281">
@@ -4828,7 +4864,7 @@
       <c r="A282">
         <v>5241</v>
       </c>
-      <c r="B282" s="45" t="s">
+      <c r="B282" s="63" t="s">
         <v>283</v>
       </c>
       <c r="C282">
@@ -4839,7 +4875,7 @@
       <c r="A283">
         <v>5242</v>
       </c>
-      <c r="B283" s="45" t="s">
+      <c r="B283" s="63" t="s">
         <v>284</v>
       </c>
       <c r="C283">
@@ -4850,7 +4886,7 @@
       <c r="A284">
         <v>5243</v>
       </c>
-      <c r="B284" s="45" t="s">
+      <c r="B284" s="63" t="s">
         <v>285</v>
       </c>
       <c r="C284">
@@ -4861,7 +4897,7 @@
       <c r="A285">
         <v>-1</v>
       </c>
-      <c r="B285" s="45" t="s">
+      <c r="B285" s="63" t="s">
         <v>286</v>
       </c>
       <c r="C285">
@@ -4872,7 +4908,7 @@
       <c r="A286">
         <v>6110</v>
       </c>
-      <c r="B286" s="45" t="s">
+      <c r="B286" s="63" t="s">
         <v>287</v>
       </c>
       <c r="C286">
@@ -4883,7 +4919,7 @@
       <c r="A287">
         <v>6129</v>
       </c>
-      <c r="B287" s="45" t="s">
+      <c r="B287" s="63" t="s">
         <v>288</v>
       </c>
       <c r="C287">
@@ -4894,7 +4930,7 @@
       <c r="A288">
         <v>6139</v>
       </c>
-      <c r="B288" s="45" t="s">
+      <c r="B288" s="63" t="s">
         <v>289</v>
       </c>
       <c r="C288">
@@ -4905,7 +4941,7 @@
       <c r="A289">
         <v>6201</v>
       </c>
-      <c r="B289" s="45" t="s">
+      <c r="B289" s="63" t="s">
         <v>290</v>
       </c>
       <c r="C289">
@@ -4916,7 +4952,7 @@
       <c r="A290">
         <v>6210</v>
       </c>
-      <c r="B290" s="45" t="s">
+      <c r="B290" s="63" t="s">
         <v>291</v>
       </c>
       <c r="C290">
@@ -4927,7 +4963,7 @@
       <c r="A291">
         <v>6229</v>
       </c>
-      <c r="B291" s="45" t="s">
+      <c r="B291" s="63" t="s">
         <v>292</v>
       </c>
       <c r="C291">
@@ -4938,7 +4974,7 @@
       <c r="A292">
         <v>6239</v>
       </c>
-      <c r="B292" s="45" t="s">
+      <c r="B292" s="63" t="s">
         <v>293</v>
       </c>
       <c r="C292">
@@ -4949,7 +4985,7 @@
       <c r="A293">
         <v>6301</v>
       </c>
-      <c r="B293" s="45" t="s">
+      <c r="B293" s="63" t="s">
         <v>294</v>
       </c>
       <c r="C293">
@@ -4960,7 +4996,7 @@
       <c r="A294">
         <v>6319</v>
       </c>
-      <c r="B294" s="45" t="s">
+      <c r="B294" s="63" t="s">
         <v>295</v>
       </c>
       <c r="C294">
@@ -4971,7 +5007,7 @@
       <c r="A295">
         <v>6329</v>
       </c>
-      <c r="B295" s="45" t="s">
+      <c r="B295" s="63" t="s">
         <v>296</v>
       </c>
       <c r="C295">
@@ -4982,7 +5018,7 @@
       <c r="A296">
         <v>6410</v>
       </c>
-      <c r="B296" s="45" t="s">
+      <c r="B296" s="63" t="s">
         <v>297</v>
       </c>
       <c r="C296">
@@ -4993,7 +5029,7 @@
       <c r="A297">
         <v>6420</v>
       </c>
-      <c r="B297" s="45" t="s">
+      <c r="B297" s="63" t="s">
         <v>298</v>
       </c>
       <c r="C297">
@@ -5004,7 +5040,7 @@
       <c r="A298">
         <v>6430</v>
       </c>
-      <c r="B298" s="45" t="s">
+      <c r="B298" s="63" t="s">
         <v>299</v>
       </c>
       <c r="C298">
@@ -5015,7 +5051,7 @@
       <c r="A299">
         <v>-1</v>
       </c>
-      <c r="B299" s="45" t="s">
+      <c r="B299" s="63" t="s">
         <v>300</v>
       </c>
       <c r="C299">
@@ -5026,7 +5062,7 @@
       <c r="A300">
         <v>7101</v>
       </c>
-      <c r="B300" s="45" t="s">
+      <c r="B300" s="63" t="s">
         <v>301</v>
       </c>
       <c r="C300">
@@ -5037,7 +5073,7 @@
       <c r="A301">
         <v>7102</v>
       </c>
-      <c r="B301" s="45" t="s">
+      <c r="B301" s="63" t="s">
         <v>302</v>
       </c>
       <c r="C301">
@@ -5048,7 +5084,7 @@
       <c r="A302">
         <v>7111</v>
       </c>
-      <c r="B302" s="45" t="s">
+      <c r="B302" s="63" t="s">
         <v>303</v>
       </c>
       <c r="C302">
@@ -5059,7 +5095,7 @@
       <c r="A303">
         <v>7112</v>
       </c>
-      <c r="B303" s="45" t="s">
+      <c r="B303" s="63" t="s">
         <v>304</v>
       </c>
       <c r="C303">
@@ -5070,7 +5106,7 @@
       <c r="A304">
         <v>7113</v>
       </c>
-      <c r="B304" s="45" t="s">
+      <c r="B304" s="63" t="s">
         <v>305</v>
       </c>
       <c r="C304">
@@ -5081,7 +5117,7 @@
       <c r="A305">
         <v>7114</v>
       </c>
-      <c r="B305" s="45" t="s">
+      <c r="B305" s="63" t="s">
         <v>306</v>
       </c>
       <c r="C305">
@@ -5092,7 +5128,7 @@
       <c r="A306">
         <v>7121</v>
       </c>
-      <c r="B306" s="45" t="s">
+      <c r="B306" s="63" t="s">
         <v>307</v>
       </c>
       <c r="C306">
@@ -5103,7 +5139,7 @@
       <c r="A307">
         <v>7122</v>
       </c>
-      <c r="B307" s="45" t="s">
+      <c r="B307" s="63" t="s">
         <v>308</v>
       </c>
       <c r="C307">
@@ -5114,7 +5150,7 @@
       <c r="A308">
         <v>7151</v>
       </c>
-      <c r="B308" s="45" t="s">
+      <c r="B308" s="63" t="s">
         <v>309</v>
       </c>
       <c r="C308">
@@ -5125,7 +5161,7 @@
       <c r="A309">
         <v>7152</v>
       </c>
-      <c r="B309" s="45" t="s">
+      <c r="B309" s="63" t="s">
         <v>310</v>
       </c>
       <c r="C309">
@@ -5136,7 +5172,7 @@
       <c r="A310">
         <v>7153</v>
       </c>
-      <c r="B310" s="45" t="s">
+      <c r="B310" s="63" t="s">
         <v>311</v>
       </c>
       <c r="C310">
@@ -5147,7 +5183,7 @@
       <c r="A311">
         <v>7154</v>
       </c>
-      <c r="B311" s="45" t="s">
+      <c r="B311" s="63" t="s">
         <v>312</v>
       </c>
       <c r="C311">
@@ -5158,7 +5194,7 @@
       <c r="A312">
         <v>7155</v>
       </c>
-      <c r="B312" s="45" t="s">
+      <c r="B312" s="63" t="s">
         <v>313</v>
       </c>
       <c r="C312">
@@ -5169,7 +5205,7 @@
       <c r="A313">
         <v>7156</v>
       </c>
-      <c r="B313" s="45" t="s">
+      <c r="B313" s="63" t="s">
         <v>314</v>
       </c>
       <c r="C313">
@@ -5180,7 +5216,7 @@
       <c r="A314">
         <v>7157</v>
       </c>
-      <c r="B314" s="45" t="s">
+      <c r="B314" s="63" t="s">
         <v>315</v>
       </c>
       <c r="C314">
@@ -5191,7 +5227,7 @@
       <c r="A315">
         <v>7161</v>
       </c>
-      <c r="B315" s="45" t="s">
+      <c r="B315" s="63" t="s">
         <v>316</v>
       </c>
       <c r="C315">
@@ -5202,7 +5238,7 @@
       <c r="A316">
         <v>7162</v>
       </c>
-      <c r="B316" s="45" t="s">
+      <c r="B316" s="63" t="s">
         <v>317</v>
       </c>
       <c r="C316">
@@ -5213,7 +5249,7 @@
       <c r="A317">
         <v>7163</v>
       </c>
-      <c r="B317" s="45" t="s">
+      <c r="B317" s="63" t="s">
         <v>318</v>
       </c>
       <c r="C317">
@@ -5224,7 +5260,7 @@
       <c r="A318">
         <v>7164</v>
       </c>
-      <c r="B318" s="45" t="s">
+      <c r="B318" s="63" t="s">
         <v>319</v>
       </c>
       <c r="C318">
@@ -5235,7 +5271,7 @@
       <c r="A319">
         <v>7165</v>
       </c>
-      <c r="B319" s="45" t="s">
+      <c r="B319" s="63" t="s">
         <v>320</v>
       </c>
       <c r="C319">
@@ -5246,7 +5282,7 @@
       <c r="A320">
         <v>7166</v>
       </c>
-      <c r="B320" s="45" t="s">
+      <c r="B320" s="63" t="s">
         <v>321</v>
       </c>
       <c r="C320">
@@ -5257,7 +5293,7 @@
       <c r="A321">
         <v>7170</v>
       </c>
-      <c r="B321" s="45" t="s">
+      <c r="B321" s="63" t="s">
         <v>322</v>
       </c>
       <c r="C321">
@@ -5268,7 +5304,7 @@
       <c r="A322">
         <v>7201</v>
       </c>
-      <c r="B322" s="45" t="s">
+      <c r="B322" s="63" t="s">
         <v>323</v>
       </c>
       <c r="C322">
@@ -5279,7 +5315,7 @@
       <c r="A323">
         <v>7202</v>
       </c>
-      <c r="B323" s="45" t="s">
+      <c r="B323" s="63" t="s">
         <v>324</v>
       </c>
       <c r="C323">
@@ -5290,7 +5326,7 @@
       <c r="A324">
         <v>7211</v>
       </c>
-      <c r="B324" s="45" t="s">
+      <c r="B324" s="63" t="s">
         <v>325</v>
       </c>
       <c r="C324">
@@ -5301,7 +5337,7 @@
       <c r="A325">
         <v>7212</v>
       </c>
-      <c r="B325" s="45" t="s">
+      <c r="B325" s="63" t="s">
         <v>326</v>
       </c>
       <c r="C325">
@@ -5312,7 +5348,7 @@
       <c r="A326">
         <v>7213</v>
       </c>
-      <c r="B326" s="45" t="s">
+      <c r="B326" s="63" t="s">
         <v>327</v>
       </c>
       <c r="C326">
@@ -5323,7 +5359,7 @@
       <c r="A327">
         <v>7214</v>
       </c>
-      <c r="B327" s="45" t="s">
+      <c r="B327" s="63" t="s">
         <v>328</v>
       </c>
       <c r="C327">
@@ -5334,7 +5370,7 @@
       <c r="A328">
         <v>7215</v>
       </c>
-      <c r="B328" s="45" t="s">
+      <c r="B328" s="63" t="s">
         <v>329</v>
       </c>
       <c r="C328">
@@ -5345,7 +5381,7 @@
       <c r="A329">
         <v>7221</v>
       </c>
-      <c r="B329" s="45" t="s">
+      <c r="B329" s="63" t="s">
         <v>330</v>
       </c>
       <c r="C329">
@@ -5356,7 +5392,7 @@
       <c r="A330">
         <v>7222</v>
       </c>
-      <c r="B330" s="45" t="s">
+      <c r="B330" s="63" t="s">
         <v>331</v>
       </c>
       <c r="C330">
@@ -5367,7 +5403,7 @@
       <c r="A331">
         <v>7223</v>
       </c>
-      <c r="B331" s="45" t="s">
+      <c r="B331" s="63" t="s">
         <v>332</v>
       </c>
       <c r="C331">
@@ -5378,7 +5414,7 @@
       <c r="A332">
         <v>7224</v>
       </c>
-      <c r="B332" s="45" t="s">
+      <c r="B332" s="63" t="s">
         <v>333</v>
       </c>
       <c r="C332">
@@ -5389,7 +5425,7 @@
       <c r="A333">
         <v>7231</v>
       </c>
-      <c r="B333" s="45" t="s">
+      <c r="B333" s="63" t="s">
         <v>334</v>
       </c>
       <c r="C333">
@@ -5400,7 +5436,7 @@
       <c r="A334">
         <v>7232</v>
       </c>
-      <c r="B334" s="45" t="s">
+      <c r="B334" s="63" t="s">
         <v>335</v>
       </c>
       <c r="C334">
@@ -5411,7 +5447,7 @@
       <c r="A335">
         <v>7233</v>
       </c>
-      <c r="B335" s="45" t="s">
+      <c r="B335" s="63" t="s">
         <v>336</v>
       </c>
       <c r="C335">
@@ -5422,7 +5458,7 @@
       <c r="A336">
         <v>7241</v>
       </c>
-      <c r="B336" s="45" t="s">
+      <c r="B336" s="63" t="s">
         <v>337</v>
       </c>
       <c r="C336">
@@ -5433,7 +5469,7 @@
       <c r="A337">
         <v>7242</v>
       </c>
-      <c r="B337" s="45" t="s">
+      <c r="B337" s="63" t="s">
         <v>338</v>
       </c>
       <c r="C337">
@@ -5444,7 +5480,7 @@
       <c r="A338">
         <v>7243</v>
       </c>
-      <c r="B338" s="45" t="s">
+      <c r="B338" s="63" t="s">
         <v>339</v>
       </c>
       <c r="C338">
@@ -5455,7 +5491,7 @@
       <c r="A339">
         <v>7244</v>
       </c>
-      <c r="B339" s="45" t="s">
+      <c r="B339" s="63" t="s">
         <v>340</v>
       </c>
       <c r="C339">
@@ -5466,7 +5502,7 @@
       <c r="A340">
         <v>7245</v>
       </c>
-      <c r="B340" s="45" t="s">
+      <c r="B340" s="63" t="s">
         <v>341</v>
       </c>
       <c r="C340">
@@ -5477,7 +5513,7 @@
       <c r="A341">
         <v>7246</v>
       </c>
-      <c r="B341" s="45" t="s">
+      <c r="B341" s="63" t="s">
         <v>342</v>
       </c>
       <c r="C341">
@@ -5488,7 +5524,7 @@
       <c r="A342">
         <v>7250</v>
       </c>
-      <c r="B342" s="45" t="s">
+      <c r="B342" s="63" t="s">
         <v>343</v>
       </c>
       <c r="C342">
@@ -5499,7 +5535,7 @@
       <c r="A343">
         <v>7251</v>
       </c>
-      <c r="B343" s="45" t="s">
+      <c r="B343" s="63" t="s">
         <v>344</v>
       </c>
       <c r="C343">
@@ -5510,7 +5546,7 @@
       <c r="A344">
         <v>7252</v>
       </c>
-      <c r="B344" s="45" t="s">
+      <c r="B344" s="63" t="s">
         <v>345</v>
       </c>
       <c r="C344">
@@ -5521,7 +5557,7 @@
       <c r="A345">
         <v>7253</v>
       </c>
-      <c r="B345" s="45" t="s">
+      <c r="B345" s="63" t="s">
         <v>346</v>
       </c>
       <c r="C345">
@@ -5532,7 +5568,7 @@
       <c r="A346">
         <v>7254</v>
       </c>
-      <c r="B346" s="45" t="s">
+      <c r="B346" s="63" t="s">
         <v>347</v>
       </c>
       <c r="C346">
@@ -5543,7 +5579,7 @@
       <c r="A347">
         <v>7255</v>
       </c>
-      <c r="B347" s="45" t="s">
+      <c r="B347" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C347">
@@ -5554,7 +5590,7 @@
       <c r="A348">
         <v>7256</v>
       </c>
-      <c r="B348" s="45" t="s">
+      <c r="B348" s="63" t="s">
         <v>349</v>
       </c>
       <c r="C348">
@@ -5565,7 +5601,7 @@
       <c r="A349">
         <v>7257</v>
       </c>
-      <c r="B349" s="45" t="s">
+      <c r="B349" s="63" t="s">
         <v>350</v>
       </c>
       <c r="C349">
@@ -5576,7 +5612,7 @@
       <c r="A350">
         <v>7301</v>
       </c>
-      <c r="B350" s="45" t="s">
+      <c r="B350" s="63" t="s">
         <v>351</v>
       </c>
       <c r="C350">
@@ -5587,7 +5623,7 @@
       <c r="A351">
         <v>7311</v>
       </c>
-      <c r="B351" s="45" t="s">
+      <c r="B351" s="63" t="s">
         <v>352</v>
       </c>
       <c r="C351">
@@ -5598,7 +5634,7 @@
       <c r="A352">
         <v>7312</v>
       </c>
-      <c r="B352" s="45" t="s">
+      <c r="B352" s="63" t="s">
         <v>353</v>
       </c>
       <c r="C352">
@@ -5609,7 +5645,7 @@
       <c r="A353">
         <v>7313</v>
       </c>
-      <c r="B353" s="45" t="s">
+      <c r="B353" s="63" t="s">
         <v>354</v>
       </c>
       <c r="C353">
@@ -5620,7 +5656,7 @@
       <c r="A354">
         <v>7321</v>
       </c>
-      <c r="B354" s="45" t="s">
+      <c r="B354" s="63" t="s">
         <v>355</v>
       </c>
       <c r="C354">
@@ -5631,7 +5667,7 @@
       <c r="A355">
         <v>7401</v>
       </c>
-      <c r="B355" s="45" t="s">
+      <c r="B355" s="63" t="s">
         <v>356</v>
       </c>
       <c r="C355">
@@ -5642,7 +5678,7 @@
       <c r="A356">
         <v>7411</v>
       </c>
-      <c r="B356" s="45" t="s">
+      <c r="B356" s="63" t="s">
         <v>357</v>
       </c>
       <c r="C356">
@@ -5653,7 +5689,7 @@
       <c r="A357">
         <v>7421</v>
       </c>
-      <c r="B357" s="45" t="s">
+      <c r="B357" s="63" t="s">
         <v>358</v>
       </c>
       <c r="C357">
@@ -5664,7 +5700,7 @@
       <c r="A358">
         <v>7501</v>
       </c>
-      <c r="B358" s="45" t="s">
+      <c r="B358" s="63" t="s">
         <v>359</v>
       </c>
       <c r="C358">
@@ -5675,7 +5711,7 @@
       <c r="A359">
         <v>7502</v>
       </c>
-      <c r="B359" s="45" t="s">
+      <c r="B359" s="63" t="s">
         <v>360</v>
       </c>
       <c r="C359">
@@ -5686,7 +5722,7 @@
       <c r="A360">
         <v>7519</v>
       </c>
-      <c r="B360" s="45" t="s">
+      <c r="B360" s="63" t="s">
         <v>361</v>
       </c>
       <c r="C360">
@@ -5697,7 +5733,7 @@
       <c r="A361">
         <v>7521</v>
       </c>
-      <c r="B361" s="45" t="s">
+      <c r="B361" s="63" t="s">
         <v>362</v>
       </c>
       <c r="C361">
@@ -5708,7 +5744,7 @@
       <c r="A362">
         <v>7522</v>
       </c>
-      <c r="B362" s="45" t="s">
+      <c r="B362" s="63" t="s">
         <v>363</v>
       </c>
       <c r="C362">
@@ -5719,7 +5755,7 @@
       <c r="A363">
         <v>7523</v>
       </c>
-      <c r="B363" s="45" t="s">
+      <c r="B363" s="63" t="s">
         <v>364</v>
       </c>
       <c r="C363">
@@ -5730,7 +5766,7 @@
       <c r="A364">
         <v>7524</v>
       </c>
-      <c r="B364" s="45" t="s">
+      <c r="B364" s="63" t="s">
         <v>365</v>
       </c>
       <c r="C364">
@@ -5741,7 +5777,7 @@
       <c r="A365">
         <v>7601</v>
       </c>
-      <c r="B365" s="45" t="s">
+      <c r="B365" s="63" t="s">
         <v>366</v>
       </c>
       <c r="C365">
@@ -5752,7 +5788,7 @@
       <c r="A366">
         <v>7602</v>
       </c>
-      <c r="B366" s="45" t="s">
+      <c r="B366" s="63" t="s">
         <v>367</v>
       </c>
       <c r="C366">
@@ -5763,7 +5799,7 @@
       <c r="A367">
         <v>7603</v>
       </c>
-      <c r="B367" s="45" t="s">
+      <c r="B367" s="63" t="s">
         <v>368</v>
       </c>
       <c r="C367">
@@ -5774,7 +5810,7 @@
       <c r="A368">
         <v>7604</v>
       </c>
-      <c r="B368" s="45" t="s">
+      <c r="B368" s="63" t="s">
         <v>369</v>
       </c>
       <c r="C368">
@@ -5785,7 +5821,7 @@
       <c r="A369">
         <v>7605</v>
       </c>
-      <c r="B369" s="45" t="s">
+      <c r="B369" s="63" t="s">
         <v>370</v>
       </c>
       <c r="C369">
@@ -5796,7 +5832,7 @@
       <c r="A370">
         <v>7606</v>
       </c>
-      <c r="B370" s="45" t="s">
+      <c r="B370" s="63" t="s">
         <v>371</v>
       </c>
       <c r="C370">
@@ -5807,7 +5843,7 @@
       <c r="A371">
         <v>7610</v>
       </c>
-      <c r="B371" s="45" t="s">
+      <c r="B371" s="63" t="s">
         <v>372</v>
       </c>
       <c r="C371">
@@ -5818,7 +5854,7 @@
       <c r="A372">
         <v>7611</v>
       </c>
-      <c r="B372" s="45" t="s">
+      <c r="B372" s="63" t="s">
         <v>373</v>
       </c>
       <c r="C372">
@@ -5829,7 +5865,7 @@
       <c r="A373">
         <v>7612</v>
       </c>
-      <c r="B373" s="45" t="s">
+      <c r="B373" s="63" t="s">
         <v>374</v>
       </c>
       <c r="C373">
@@ -5840,7 +5876,7 @@
       <c r="A374">
         <v>7613</v>
       </c>
-      <c r="B374" s="45" t="s">
+      <c r="B374" s="63" t="s">
         <v>375</v>
       </c>
       <c r="C374">
@@ -5851,7 +5887,7 @@
       <c r="A375">
         <v>7614</v>
       </c>
-      <c r="B375" s="45" t="s">
+      <c r="B375" s="63" t="s">
         <v>376</v>
       </c>
       <c r="C375">
@@ -5862,7 +5898,7 @@
       <c r="A376">
         <v>7618</v>
       </c>
-      <c r="B376" s="45" t="s">
+      <c r="B376" s="63" t="s">
         <v>377</v>
       </c>
       <c r="C376">
@@ -5873,7 +5909,7 @@
       <c r="A377">
         <v>7620</v>
       </c>
-      <c r="B377" s="45" t="s">
+      <c r="B377" s="63" t="s">
         <v>378</v>
       </c>
       <c r="C377">
@@ -5884,7 +5920,7 @@
       <c r="A378">
         <v>7621</v>
       </c>
-      <c r="B378" s="45" t="s">
+      <c r="B378" s="63" t="s">
         <v>379</v>
       </c>
       <c r="C378">
@@ -5895,7 +5931,7 @@
       <c r="A379">
         <v>7622</v>
       </c>
-      <c r="B379" s="45" t="s">
+      <c r="B379" s="63" t="s">
         <v>380</v>
       </c>
       <c r="C379">
@@ -5906,7 +5942,7 @@
       <c r="A380">
         <v>7623</v>
       </c>
-      <c r="B380" s="45" t="s">
+      <c r="B380" s="63" t="s">
         <v>381</v>
       </c>
       <c r="C380">
@@ -5917,7 +5953,7 @@
       <c r="A381">
         <v>7630</v>
       </c>
-      <c r="B381" s="45" t="s">
+      <c r="B381" s="63" t="s">
         <v>382</v>
       </c>
       <c r="C381">
@@ -5928,7 +5964,7 @@
       <c r="A382">
         <v>7631</v>
       </c>
-      <c r="B382" s="45" t="s">
+      <c r="B382" s="63" t="s">
         <v>383</v>
       </c>
       <c r="C382">
@@ -5939,7 +5975,7 @@
       <c r="A383">
         <v>7632</v>
       </c>
-      <c r="B383" s="45" t="s">
+      <c r="B383" s="63" t="s">
         <v>384</v>
       </c>
       <c r="C383">
@@ -5950,7 +5986,7 @@
       <c r="A384">
         <v>7633</v>
       </c>
-      <c r="B384" s="45" t="s">
+      <c r="B384" s="63" t="s">
         <v>385</v>
       </c>
       <c r="C384">
@@ -5961,7 +5997,7 @@
       <c r="A385">
         <v>7640</v>
       </c>
-      <c r="B385" s="45" t="s">
+      <c r="B385" s="63" t="s">
         <v>386</v>
       </c>
       <c r="C385">
@@ -5972,7 +6008,7 @@
       <c r="A386">
         <v>7641</v>
       </c>
-      <c r="B386" s="45" t="s">
+      <c r="B386" s="63" t="s">
         <v>387</v>
       </c>
       <c r="C386">
@@ -5983,7 +6019,7 @@
       <c r="A387">
         <v>7642</v>
       </c>
-      <c r="B387" s="45" t="s">
+      <c r="B387" s="63" t="s">
         <v>388</v>
       </c>
       <c r="C387">
@@ -5994,7 +6030,7 @@
       <c r="A388">
         <v>7643</v>
       </c>
-      <c r="B388" s="45" t="s">
+      <c r="B388" s="63" t="s">
         <v>389</v>
       </c>
       <c r="C388">
@@ -6005,7 +6041,7 @@
       <c r="A389">
         <v>7650</v>
       </c>
-      <c r="B389" s="45" t="s">
+      <c r="B389" s="63" t="s">
         <v>390</v>
       </c>
       <c r="C389">
@@ -6016,7 +6052,7 @@
       <c r="A390">
         <v>7651</v>
       </c>
-      <c r="B390" s="45" t="s">
+      <c r="B390" s="63" t="s">
         <v>391</v>
       </c>
       <c r="C390">
@@ -6027,7 +6063,7 @@
       <c r="A391">
         <v>7652</v>
       </c>
-      <c r="B391" s="45" t="s">
+      <c r="B391" s="63" t="s">
         <v>392</v>
       </c>
       <c r="C391">
@@ -6038,7 +6074,7 @@
       <c r="A392">
         <v>7653</v>
       </c>
-      <c r="B392" s="45" t="s">
+      <c r="B392" s="63" t="s">
         <v>393</v>
       </c>
       <c r="C392">
@@ -6049,7 +6085,7 @@
       <c r="A393">
         <v>7654</v>
       </c>
-      <c r="B393" s="45" t="s">
+      <c r="B393" s="63" t="s">
         <v>394</v>
       </c>
       <c r="C393">
@@ -6060,7 +6096,7 @@
       <c r="A394">
         <v>7660</v>
       </c>
-      <c r="B394" s="45" t="s">
+      <c r="B394" s="63" t="s">
         <v>395</v>
       </c>
       <c r="C394">
@@ -6071,7 +6107,7 @@
       <c r="A395">
         <v>7661</v>
       </c>
-      <c r="B395" s="45" t="s">
+      <c r="B395" s="63" t="s">
         <v>396</v>
       </c>
       <c r="C395">
@@ -6082,7 +6118,7 @@
       <c r="A396">
         <v>7662</v>
       </c>
-      <c r="B396" s="45" t="s">
+      <c r="B396" s="63" t="s">
         <v>397</v>
       </c>
       <c r="C396">
@@ -6093,7 +6129,7 @@
       <c r="A397">
         <v>7663</v>
       </c>
-      <c r="B397" s="45" t="s">
+      <c r="B397" s="63" t="s">
         <v>398</v>
       </c>
       <c r="C397">
@@ -6104,7 +6140,7 @@
       <c r="A398">
         <v>7664</v>
       </c>
-      <c r="B398" s="45" t="s">
+      <c r="B398" s="63" t="s">
         <v>399</v>
       </c>
       <c r="C398">
@@ -6115,7 +6151,7 @@
       <c r="A399">
         <v>7681</v>
       </c>
-      <c r="B399" s="45" t="s">
+      <c r="B399" s="63" t="s">
         <v>400</v>
       </c>
       <c r="C399">
@@ -6126,7 +6162,7 @@
       <c r="A400">
         <v>7682</v>
       </c>
-      <c r="B400" s="45" t="s">
+      <c r="B400" s="63" t="s">
         <v>401</v>
       </c>
       <c r="C400">
@@ -6137,7 +6173,7 @@
       <c r="A401">
         <v>7683</v>
       </c>
-      <c r="B401" s="45" t="s">
+      <c r="B401" s="63" t="s">
         <v>402</v>
       </c>
       <c r="C401">
@@ -6148,7 +6184,7 @@
       <c r="A402">
         <v>7686</v>
       </c>
-      <c r="B402" s="45" t="s">
+      <c r="B402" s="63" t="s">
         <v>403</v>
       </c>
       <c r="C402">
@@ -6159,7 +6195,7 @@
       <c r="A403">
         <v>7687</v>
       </c>
-      <c r="B403" s="45" t="s">
+      <c r="B403" s="63" t="s">
         <v>404</v>
       </c>
       <c r="C403">
@@ -6170,7 +6206,7 @@
       <c r="A404">
         <v>7701</v>
       </c>
-      <c r="B404" s="45" t="s">
+      <c r="B404" s="63" t="s">
         <v>405</v>
       </c>
       <c r="C404">
@@ -6181,7 +6217,7 @@
       <c r="A405">
         <v>7711</v>
       </c>
-      <c r="B405" s="45" t="s">
+      <c r="B405" s="63" t="s">
         <v>406</v>
       </c>
       <c r="C405">
@@ -6192,7 +6228,7 @@
       <c r="A406">
         <v>7721</v>
       </c>
-      <c r="B406" s="45" t="s">
+      <c r="B406" s="63" t="s">
         <v>407</v>
       </c>
       <c r="C406">
@@ -6203,7 +6239,7 @@
       <c r="A407">
         <v>7731</v>
       </c>
-      <c r="B407" s="45" t="s">
+      <c r="B407" s="63" t="s">
         <v>408</v>
       </c>
       <c r="C407">
@@ -6214,7 +6250,7 @@
       <c r="A408">
         <v>7732</v>
       </c>
-      <c r="B408" s="45" t="s">
+      <c r="B408" s="63" t="s">
         <v>409</v>
       </c>
       <c r="C408">
@@ -6225,7 +6261,7 @@
       <c r="A409">
         <v>7733</v>
       </c>
-      <c r="B409" s="45" t="s">
+      <c r="B409" s="63" t="s">
         <v>410</v>
       </c>
       <c r="C409">
@@ -6236,7 +6272,7 @@
       <c r="A410">
         <v>7734</v>
       </c>
-      <c r="B410" s="45" t="s">
+      <c r="B410" s="63" t="s">
         <v>411</v>
       </c>
       <c r="C410">
@@ -6247,7 +6283,7 @@
       <c r="A411">
         <v>7735</v>
       </c>
-      <c r="B411" s="45" t="s">
+      <c r="B411" s="63" t="s">
         <v>412</v>
       </c>
       <c r="C411">
@@ -6258,7 +6294,7 @@
       <c r="A412">
         <v>7741</v>
       </c>
-      <c r="B412" s="45" t="s">
+      <c r="B412" s="63" t="s">
         <v>413</v>
       </c>
       <c r="C412">
@@ -6269,7 +6305,7 @@
       <c r="A413">
         <v>7751</v>
       </c>
-      <c r="B413" s="45" t="s">
+      <c r="B413" s="63" t="s">
         <v>414</v>
       </c>
       <c r="C413">
@@ -6280,7 +6316,7 @@
       <c r="A414">
         <v>7764</v>
       </c>
-      <c r="B414" s="45" t="s">
+      <c r="B414" s="63" t="s">
         <v>415</v>
       </c>
       <c r="C414">
@@ -6291,7 +6327,7 @@
       <c r="A415">
         <v>7771</v>
       </c>
-      <c r="B415" s="45" t="s">
+      <c r="B415" s="63" t="s">
         <v>416</v>
       </c>
       <c r="C415">
@@ -6302,7 +6338,7 @@
       <c r="A416">
         <v>7772</v>
       </c>
-      <c r="B416" s="45" t="s">
+      <c r="B416" s="63" t="s">
         <v>417</v>
       </c>
       <c r="C416">
@@ -6313,7 +6349,7 @@
       <c r="A417">
         <v>7801</v>
       </c>
-      <c r="B417" s="45" t="s">
+      <c r="B417" s="63" t="s">
         <v>418</v>
       </c>
       <c r="C417">
@@ -6324,7 +6360,7 @@
       <c r="A418">
         <v>7811</v>
       </c>
-      <c r="B418" s="45" t="s">
+      <c r="B418" s="63" t="s">
         <v>419</v>
       </c>
       <c r="C418">
@@ -6335,7 +6371,7 @@
       <c r="A419">
         <v>7813</v>
       </c>
-      <c r="B419" s="45" t="s">
+      <c r="B419" s="63" t="s">
         <v>420</v>
       </c>
       <c r="C419">
@@ -6346,7 +6382,7 @@
       <c r="A420">
         <v>7817</v>
       </c>
-      <c r="B420" s="45" t="s">
+      <c r="B420" s="63" t="s">
         <v>421</v>
       </c>
       <c r="C420">
@@ -6357,7 +6393,7 @@
       <c r="A421">
         <v>7820</v>
       </c>
-      <c r="B421" s="45" t="s">
+      <c r="B421" s="63" t="s">
         <v>422</v>
       </c>
       <c r="C421">
@@ -6368,7 +6404,7 @@
       <c r="A422">
         <v>7821</v>
       </c>
-      <c r="B422" s="45" t="s">
+      <c r="B422" s="63" t="s">
         <v>423</v>
       </c>
       <c r="C422">
@@ -6379,7 +6415,7 @@
       <c r="A423">
         <v>7822</v>
       </c>
-      <c r="B423" s="45" t="s">
+      <c r="B423" s="63" t="s">
         <v>424</v>
       </c>
       <c r="C423">
@@ -6390,7 +6426,7 @@
       <c r="A424">
         <v>7823</v>
       </c>
-      <c r="B424" s="45" t="s">
+      <c r="B424" s="63" t="s">
         <v>425</v>
       </c>
       <c r="C424">
@@ -6401,7 +6437,7 @@
       <c r="A425">
         <v>7824</v>
       </c>
-      <c r="B425" s="45" t="s">
+      <c r="B425" s="63" t="s">
         <v>426</v>
       </c>
       <c r="C425">
@@ -6412,7 +6448,7 @@
       <c r="A426">
         <v>7825</v>
       </c>
-      <c r="B426" s="45" t="s">
+      <c r="B426" s="63" t="s">
         <v>427</v>
       </c>
       <c r="C426">
@@ -6423,7 +6459,7 @@
       <c r="A427">
         <v>7826</v>
       </c>
-      <c r="B427" s="45" t="s">
+      <c r="B427" s="63" t="s">
         <v>428</v>
       </c>
       <c r="C427">
@@ -6434,7 +6470,7 @@
       <c r="A428">
         <v>7827</v>
       </c>
-      <c r="B428" s="45" t="s">
+      <c r="B428" s="63" t="s">
         <v>429</v>
       </c>
       <c r="C428">
@@ -6445,7 +6481,7 @@
       <c r="A429">
         <v>7828</v>
       </c>
-      <c r="B429" s="45" t="s">
+      <c r="B429" s="63" t="s">
         <v>430</v>
       </c>
       <c r="C429">
@@ -6456,7 +6492,7 @@
       <c r="A430">
         <v>7831</v>
       </c>
-      <c r="B430" s="45" t="s">
+      <c r="B430" s="63" t="s">
         <v>431</v>
       </c>
       <c r="C430">
@@ -6467,7 +6503,7 @@
       <c r="A431">
         <v>7832</v>
       </c>
-      <c r="B431" s="45" t="s">
+      <c r="B431" s="63" t="s">
         <v>432</v>
       </c>
       <c r="C431">
@@ -6478,7 +6514,7 @@
       <c r="A432">
         <v>7841</v>
       </c>
-      <c r="B432" s="45" t="s">
+      <c r="B432" s="63" t="s">
         <v>433</v>
       </c>
       <c r="C432">
@@ -6489,7 +6525,7 @@
       <c r="A433">
         <v>7842</v>
       </c>
-      <c r="B433" s="45" t="s">
+      <c r="B433" s="63" t="s">
         <v>434</v>
       </c>
       <c r="C433">
@@ -6500,7 +6536,7 @@
       <c r="A434">
         <v>-1</v>
       </c>
-      <c r="B434" s="45" t="s">
+      <c r="B434" s="63" t="s">
         <v>300</v>
       </c>
       <c r="C434">
@@ -6511,7 +6547,7 @@
       <c r="A435">
         <v>8101</v>
       </c>
-      <c r="B435" s="45" t="s">
+      <c r="B435" s="63" t="s">
         <v>435</v>
       </c>
       <c r="C435">
@@ -6522,7 +6558,7 @@
       <c r="A436">
         <v>8102</v>
       </c>
-      <c r="B436" s="45" t="s">
+      <c r="B436" s="63" t="s">
         <v>436</v>
       </c>
       <c r="C436">
@@ -6533,7 +6569,7 @@
       <c r="A437">
         <v>8103</v>
       </c>
-      <c r="B437" s="45" t="s">
+      <c r="B437" s="63" t="s">
         <v>437</v>
       </c>
       <c r="C437">
@@ -6544,7 +6580,7 @@
       <c r="A438">
         <v>8110</v>
       </c>
-      <c r="B438" s="45" t="s">
+      <c r="B438" s="63" t="s">
         <v>438</v>
       </c>
       <c r="C438">
@@ -6555,7 +6591,7 @@
       <c r="A439">
         <v>8111</v>
       </c>
-      <c r="B439" s="45" t="s">
+      <c r="B439" s="63" t="s">
         <v>439</v>
       </c>
       <c r="C439">
@@ -6566,7 +6602,7 @@
       <c r="A440">
         <v>8112</v>
       </c>
-      <c r="B440" s="45" t="s">
+      <c r="B440" s="63" t="s">
         <v>440</v>
       </c>
       <c r="C440">
@@ -6577,7 +6613,7 @@
       <c r="A441">
         <v>8113</v>
       </c>
-      <c r="B441" s="45" t="s">
+      <c r="B441" s="63" t="s">
         <v>441</v>
       </c>
       <c r="C441">
@@ -6588,7 +6624,7 @@
       <c r="A442">
         <v>8114</v>
       </c>
-      <c r="B442" s="45" t="s">
+      <c r="B442" s="63" t="s">
         <v>442</v>
       </c>
       <c r="C442">
@@ -6599,7 +6635,7 @@
       <c r="A443">
         <v>8115</v>
       </c>
-      <c r="B443" s="45" t="s">
+      <c r="B443" s="63" t="s">
         <v>443</v>
       </c>
       <c r="C443">
@@ -6610,7 +6646,7 @@
       <c r="A444">
         <v>8116</v>
       </c>
-      <c r="B444" s="45" t="s">
+      <c r="B444" s="63" t="s">
         <v>444</v>
       </c>
       <c r="C444">
@@ -6621,7 +6657,7 @@
       <c r="A445">
         <v>8117</v>
       </c>
-      <c r="B445" s="45" t="s">
+      <c r="B445" s="63" t="s">
         <v>445</v>
       </c>
       <c r="C445">
@@ -6632,7 +6668,7 @@
       <c r="A446">
         <v>8118</v>
       </c>
-      <c r="B446" s="45" t="s">
+      <c r="B446" s="63" t="s">
         <v>446</v>
       </c>
       <c r="C446">
@@ -6643,7 +6679,7 @@
       <c r="A447">
         <v>8121</v>
       </c>
-      <c r="B447" s="45" t="s">
+      <c r="B447" s="63" t="s">
         <v>447</v>
       </c>
       <c r="C447">
@@ -6654,7 +6690,7 @@
       <c r="A448">
         <v>8131</v>
       </c>
-      <c r="B448" s="45" t="s">
+      <c r="B448" s="63" t="s">
         <v>448</v>
       </c>
       <c r="C448">
@@ -6665,7 +6701,7 @@
       <c r="A449">
         <v>8181</v>
       </c>
-      <c r="B449" s="45" t="s">
+      <c r="B449" s="63" t="s">
         <v>449</v>
       </c>
       <c r="C449">
@@ -6676,7 +6712,7 @@
       <c r="A450">
         <v>8201</v>
       </c>
-      <c r="B450" s="45" t="s">
+      <c r="B450" s="63" t="s">
         <v>450</v>
       </c>
       <c r="C450">
@@ -6687,7 +6723,7 @@
       <c r="A451">
         <v>8202</v>
       </c>
-      <c r="B451" s="45" t="s">
+      <c r="B451" s="63" t="s">
         <v>451</v>
       </c>
       <c r="C451">
@@ -6698,7 +6734,7 @@
       <c r="A452">
         <v>8211</v>
       </c>
-      <c r="B452" s="45" t="s">
+      <c r="B452" s="63" t="s">
         <v>452</v>
       </c>
       <c r="C452">
@@ -6709,7 +6745,7 @@
       <c r="A453">
         <v>8212</v>
       </c>
-      <c r="B453" s="45" t="s">
+      <c r="B453" s="63" t="s">
         <v>453</v>
       </c>
       <c r="C453">
@@ -6720,7 +6756,7 @@
       <c r="A454">
         <v>8213</v>
       </c>
-      <c r="B454" s="45" t="s">
+      <c r="B454" s="63" t="s">
         <v>454</v>
       </c>
       <c r="C454">
@@ -6731,7 +6767,7 @@
       <c r="A455">
         <v>8214</v>
       </c>
-      <c r="B455" s="45" t="s">
+      <c r="B455" s="63" t="s">
         <v>455</v>
       </c>
       <c r="C455">
@@ -6742,7 +6778,7 @@
       <c r="A456">
         <v>8221</v>
       </c>
-      <c r="B456" s="45" t="s">
+      <c r="B456" s="63" t="s">
         <v>456</v>
       </c>
       <c r="C456">
@@ -6753,7 +6789,7 @@
       <c r="A457">
         <v>8231</v>
       </c>
-      <c r="B457" s="45" t="s">
+      <c r="B457" s="63" t="s">
         <v>457</v>
       </c>
       <c r="C457">
@@ -6764,7 +6800,7 @@
       <c r="A458">
         <v>8232</v>
       </c>
-      <c r="B458" s="45" t="s">
+      <c r="B458" s="63" t="s">
         <v>458</v>
       </c>
       <c r="C458">
@@ -6775,7 +6811,7 @@
       <c r="A459">
         <v>8233</v>
       </c>
-      <c r="B459" s="45" t="s">
+      <c r="B459" s="63" t="s">
         <v>459</v>
       </c>
       <c r="C459">
@@ -6786,7 +6822,7 @@
       <c r="A460">
         <v>8281</v>
       </c>
-      <c r="B460" s="45" t="s">
+      <c r="B460" s="63" t="s">
         <v>460</v>
       </c>
       <c r="C460">
@@ -6797,7 +6833,7 @@
       <c r="A461">
         <v>8301</v>
       </c>
-      <c r="B461" s="45" t="s">
+      <c r="B461" s="63" t="s">
         <v>461</v>
       </c>
       <c r="C461">
@@ -6808,7 +6844,7 @@
       <c r="A462">
         <v>8311</v>
       </c>
-      <c r="B462" s="45" t="s">
+      <c r="B462" s="63" t="s">
         <v>462</v>
       </c>
       <c r="C462">
@@ -6819,7 +6855,7 @@
       <c r="A463">
         <v>8321</v>
       </c>
-      <c r="B463" s="45" t="s">
+      <c r="B463" s="63" t="s">
         <v>463</v>
       </c>
       <c r="C463">
@@ -6830,7 +6866,7 @@
       <c r="A464">
         <v>8339</v>
       </c>
-      <c r="B464" s="45" t="s">
+      <c r="B464" s="63" t="s">
         <v>464</v>
       </c>
       <c r="C464">
@@ -6841,7 +6877,7 @@
       <c r="A465">
         <v>8401</v>
       </c>
-      <c r="B465" s="45" t="s">
+      <c r="B465" s="63" t="s">
         <v>465</v>
       </c>
       <c r="C465">
@@ -6852,7 +6888,7 @@
       <c r="A466">
         <v>8411</v>
       </c>
-      <c r="B466" s="45" t="s">
+      <c r="B466" s="63" t="s">
         <v>466</v>
       </c>
       <c r="C466">
@@ -6863,7 +6899,7 @@
       <c r="A467">
         <v>8412</v>
       </c>
-      <c r="B467" s="45" t="s">
+      <c r="B467" s="63" t="s">
         <v>467</v>
       </c>
       <c r="C467">
@@ -6874,7 +6910,7 @@
       <c r="A468">
         <v>8413</v>
       </c>
-      <c r="B468" s="45" t="s">
+      <c r="B468" s="63" t="s">
         <v>468</v>
       </c>
       <c r="C468">
@@ -6885,7 +6921,7 @@
       <c r="A469">
         <v>8416</v>
       </c>
-      <c r="B469" s="45" t="s">
+      <c r="B469" s="63" t="s">
         <v>469</v>
       </c>
       <c r="C469">
@@ -6896,7 +6932,7 @@
       <c r="A470">
         <v>8417</v>
       </c>
-      <c r="B470" s="45" t="s">
+      <c r="B470" s="63" t="s">
         <v>470</v>
       </c>
       <c r="C470">
@@ -6907,7 +6943,7 @@
       <c r="A471">
         <v>8421</v>
       </c>
-      <c r="B471" s="45" t="s">
+      <c r="B471" s="63" t="s">
         <v>471</v>
       </c>
       <c r="C471">
@@ -6918,7 +6954,7 @@
       <c r="A472">
         <v>8423</v>
       </c>
-      <c r="B472" s="45" t="s">
+      <c r="B472" s="63" t="s">
         <v>472</v>
       </c>
       <c r="C472">
@@ -6929,7 +6965,7 @@
       <c r="A473">
         <v>8429</v>
       </c>
-      <c r="B473" s="45" t="s">
+      <c r="B473" s="63" t="s">
         <v>473</v>
       </c>
       <c r="C473">
@@ -6940,7 +6976,7 @@
       <c r="A474">
         <v>8484</v>
       </c>
-      <c r="B474" s="45" t="s">
+      <c r="B474" s="63" t="s">
         <v>474</v>
       </c>
       <c r="C474">
@@ -6951,7 +6987,7 @@
       <c r="A475">
         <v>8485</v>
       </c>
-      <c r="B475" s="45" t="s">
+      <c r="B475" s="63" t="s">
         <v>475</v>
       </c>
       <c r="C475">
@@ -6962,7 +6998,7 @@
       <c r="A476">
         <v>8491</v>
       </c>
-      <c r="B476" s="45" t="s">
+      <c r="B476" s="63" t="s">
         <v>476</v>
       </c>
       <c r="C476">
@@ -6973,7 +7009,7 @@
       <c r="A477">
         <v>8492</v>
       </c>
-      <c r="B477" s="45" t="s">
+      <c r="B477" s="63" t="s">
         <v>477</v>
       </c>
       <c r="C477">
@@ -6984,7 +7020,7 @@
       <c r="A478">
         <v>8493</v>
       </c>
-      <c r="B478" s="45" t="s">
+      <c r="B478" s="63" t="s">
         <v>478</v>
       </c>
       <c r="C478">
@@ -6995,7 +7031,7 @@
       <c r="A479">
         <v>8601</v>
       </c>
-      <c r="B479" s="45" t="s">
+      <c r="B479" s="63" t="s">
         <v>479</v>
       </c>
       <c r="C479">
@@ -7006,7 +7042,7 @@
       <c r="A480">
         <v>8611</v>
       </c>
-      <c r="B480" s="45" t="s">
+      <c r="B480" s="63" t="s">
         <v>480</v>
       </c>
       <c r="C480">
@@ -7017,7 +7053,7 @@
       <c r="A481">
         <v>8612</v>
       </c>
-      <c r="B481" s="45" t="s">
+      <c r="B481" s="63" t="s">
         <v>481</v>
       </c>
       <c r="C481">
@@ -7028,7 +7064,7 @@
       <c r="A482">
         <v>8621</v>
       </c>
-      <c r="B482" s="45" t="s">
+      <c r="B482" s="63" t="s">
         <v>482</v>
       </c>
       <c r="C482">
@@ -7039,7 +7075,7 @@
       <c r="A483">
         <v>8622</v>
       </c>
-      <c r="B483" s="45" t="s">
+      <c r="B483" s="63" t="s">
         <v>483</v>
       </c>
       <c r="C483">
@@ -7050,7 +7086,7 @@
       <c r="A484">
         <v>8623</v>
       </c>
-      <c r="B484" s="45" t="s">
+      <c r="B484" s="63" t="s">
         <v>484</v>
       </c>
       <c r="C484">
@@ -7061,7 +7097,7 @@
       <c r="A485">
         <v>8624</v>
       </c>
-      <c r="B485" s="45" t="s">
+      <c r="B485" s="63" t="s">
         <v>485</v>
       </c>
       <c r="C485">
@@ -7072,7 +7108,7 @@
       <c r="A486">
         <v>8625</v>
       </c>
-      <c r="B486" s="45" t="s">
+      <c r="B486" s="63" t="s">
         <v>486</v>
       </c>
       <c r="C486">
@@ -7083,7 +7119,7 @@
       <c r="A487">
         <v>8711</v>
       </c>
-      <c r="B487" s="45" t="s">
+      <c r="B487" s="63" t="s">
         <v>487</v>
       </c>
       <c r="C487">
@@ -7094,7 +7130,7 @@
       <c r="A488">
         <v>-1</v>
       </c>
-      <c r="B488" s="45" t="s">
+      <c r="B488" s="63" t="s">
         <v>488</v>
       </c>
       <c r="C488">
@@ -7105,7 +7141,7 @@
       <c r="A489">
         <v>9101</v>
       </c>
-      <c r="B489" s="45" t="s">
+      <c r="B489" s="63" t="s">
         <v>489</v>
       </c>
       <c r="C489">
@@ -7116,7 +7152,7 @@
       <c r="A490">
         <v>9102</v>
       </c>
-      <c r="B490" s="45" t="s">
+      <c r="B490" s="63" t="s">
         <v>490</v>
       </c>
       <c r="C490">
@@ -7127,7 +7163,7 @@
       <c r="A491">
         <v>9109</v>
       </c>
-      <c r="B491" s="45" t="s">
+      <c r="B491" s="63" t="s">
         <v>491</v>
       </c>
       <c r="C491">
@@ -7138,7 +7174,7 @@
       <c r="A492">
         <v>9111</v>
       </c>
-      <c r="B492" s="45" t="s">
+      <c r="B492" s="63" t="s">
         <v>492</v>
       </c>
       <c r="C492">
@@ -7149,7 +7185,7 @@
       <c r="A493">
         <v>9112</v>
       </c>
-      <c r="B493" s="45" t="s">
+      <c r="B493" s="63" t="s">
         <v>493</v>
       </c>
       <c r="C493">
@@ -7160,7 +7196,7 @@
       <c r="A494">
         <v>9113</v>
       </c>
-      <c r="B494" s="45" t="s">
+      <c r="B494" s="63" t="s">
         <v>494</v>
       </c>
       <c r="C494">
@@ -7171,7 +7207,7 @@
       <c r="A495">
         <v>9131</v>
       </c>
-      <c r="B495" s="45" t="s">
+      <c r="B495" s="63" t="s">
         <v>495</v>
       </c>
       <c r="C495">
@@ -7182,7 +7218,7 @@
       <c r="A496">
         <v>9141</v>
       </c>
-      <c r="B496" s="45" t="s">
+      <c r="B496" s="63" t="s">
         <v>496</v>
       </c>
       <c r="C496">
@@ -7193,7 +7229,7 @@
       <c r="A497">
         <v>9142</v>
       </c>
-      <c r="B497" s="45" t="s">
+      <c r="B497" s="63" t="s">
         <v>497</v>
       </c>
       <c r="C497">
@@ -7204,7 +7240,7 @@
       <c r="A498">
         <v>9143</v>
       </c>
-      <c r="B498" s="45" t="s">
+      <c r="B498" s="63" t="s">
         <v>498</v>
       </c>
       <c r="C498">
@@ -7215,7 +7251,7 @@
       <c r="A499">
         <v>9144</v>
       </c>
-      <c r="B499" s="45" t="s">
+      <c r="B499" s="63" t="s">
         <v>499</v>
       </c>
       <c r="C499">
@@ -7226,7 +7262,7 @@
       <c r="A500">
         <v>9151</v>
       </c>
-      <c r="B500" s="45" t="s">
+      <c r="B500" s="63" t="s">
         <v>500</v>
       </c>
       <c r="C500">
@@ -7237,7 +7273,7 @@
       <c r="A501">
         <v>9152</v>
       </c>
-      <c r="B501" s="45" t="s">
+      <c r="B501" s="63" t="s">
         <v>501</v>
       </c>
       <c r="C501">
@@ -7248,7 +7284,7 @@
       <c r="A502">
         <v>9153</v>
       </c>
-      <c r="B502" s="45" t="s">
+      <c r="B502" s="63" t="s">
         <v>502</v>
       </c>
       <c r="C502">
@@ -7259,7 +7295,7 @@
       <c r="A503">
         <v>9154</v>
       </c>
-      <c r="B503" s="45" t="s">
+      <c r="B503" s="63" t="s">
         <v>503</v>
       </c>
       <c r="C503">
@@ -7270,7 +7306,7 @@
       <c r="A504">
         <v>9191</v>
       </c>
-      <c r="B504" s="45" t="s">
+      <c r="B504" s="63" t="s">
         <v>504</v>
       </c>
       <c r="C504">
@@ -7281,7 +7317,7 @@
       <c r="A505">
         <v>9192</v>
       </c>
-      <c r="B505" s="45" t="s">
+      <c r="B505" s="63" t="s">
         <v>505</v>
       </c>
       <c r="C505">
@@ -7292,7 +7328,7 @@
       <c r="A506">
         <v>9193</v>
       </c>
-      <c r="B506" s="45" t="s">
+      <c r="B506" s="63" t="s">
         <v>506</v>
       </c>
       <c r="C506">
@@ -7303,7 +7339,7 @@
       <c r="A507">
         <v>9501</v>
       </c>
-      <c r="B507" s="45" t="s">
+      <c r="B507" s="63" t="s">
         <v>507</v>
       </c>
       <c r="C507">
@@ -7314,7 +7350,7 @@
       <c r="A508">
         <v>9502</v>
       </c>
-      <c r="B508" s="45" t="s">
+      <c r="B508" s="63" t="s">
         <v>508</v>
       </c>
       <c r="C508">
@@ -7325,7 +7361,7 @@
       <c r="A509">
         <v>9503</v>
       </c>
-      <c r="B509" s="45" t="s">
+      <c r="B509" s="63" t="s">
         <v>509</v>
       </c>
       <c r="C509">
@@ -7336,7 +7372,7 @@
       <c r="A510">
         <v>9511</v>
       </c>
-      <c r="B510" s="45" t="s">
+      <c r="B510" s="63" t="s">
         <v>510</v>
       </c>
       <c r="C510">
@@ -7347,7 +7383,7 @@
       <c r="A511">
         <v>9513</v>
       </c>
-      <c r="B511" s="45" t="s">
+      <c r="B511" s="63" t="s">
         <v>511</v>
       </c>
       <c r="C511">
@@ -7358,7 +7394,7 @@
       <c r="A512">
         <v>9531</v>
       </c>
-      <c r="B512" s="45" t="s">
+      <c r="B512" s="63" t="s">
         <v>512</v>
       </c>
       <c r="C512">
@@ -7369,7 +7405,7 @@
       <c r="A513">
         <v>9541</v>
       </c>
-      <c r="B513" s="45" t="s">
+      <c r="B513" s="63" t="s">
         <v>513</v>
       </c>
       <c r="C513">
@@ -7380,7 +7416,7 @@
       <c r="A514">
         <v>9542</v>
       </c>
-      <c r="B514" s="45" t="s">
+      <c r="B514" s="63" t="s">
         <v>514</v>
       </c>
       <c r="C514">
@@ -7391,7 +7427,7 @@
       <c r="A515">
         <v>9543</v>
       </c>
-      <c r="B515" s="45" t="s">
+      <c r="B515" s="63" t="s">
         <v>515</v>
       </c>
       <c r="C515">
@@ -7402,7 +7438,7 @@
       <c r="A516">
         <v>9911</v>
       </c>
-      <c r="B516" s="45" t="s">
+      <c r="B516" s="63" t="s">
         <v>516</v>
       </c>
       <c r="C516">
@@ -7413,7 +7449,7 @@
       <c r="A517">
         <v>9912</v>
       </c>
-      <c r="B517" s="45" t="s">
+      <c r="B517" s="63" t="s">
         <v>517</v>
       </c>
       <c r="C517">
@@ -7424,7 +7460,7 @@
       <c r="A518">
         <v>9913</v>
       </c>
-      <c r="B518" s="45" t="s">
+      <c r="B518" s="63" t="s">
         <v>518</v>
       </c>
       <c r="C518">
@@ -7435,7 +7471,7 @@
       <c r="A519">
         <v>9914</v>
       </c>
-      <c r="B519" s="45" t="s">
+      <c r="B519" s="63" t="s">
         <v>519</v>
       </c>
       <c r="C519">
@@ -7446,7 +7482,7 @@
       <c r="A520">
         <v>9921</v>
       </c>
-      <c r="B520" s="45" t="s">
+      <c r="B520" s="63" t="s">
         <v>520</v>
       </c>
       <c r="C520">
@@ -7457,7 +7493,7 @@
       <c r="A521">
         <v>9922</v>
       </c>
-      <c r="B521" s="45" t="s">
+      <c r="B521" s="63" t="s">
         <v>521</v>
       </c>
       <c r="C521">
@@ -7468,7 +7504,7 @@
       <c r="A522">
         <v>-1</v>
       </c>
-      <c r="B522" s="45" t="s">
+      <c r="B522" s="63" t="s">
         <v>522</v>
       </c>
       <c r="C522">
@@ -7479,7 +7515,7 @@
       <c r="A523">
         <v>9999</v>
       </c>
-      <c r="B523" s="45" t="s">
+      <c r="B523" s="63" t="s">
         <v>523</v>
       </c>
       <c r="C523">

</xml_diff>